<commit_message>
[2020-10-20] VoteMatch Controller 완성 & Post Check Done
</commit_message>
<xml_diff>
--- a/docs/srs/fbt_docs.xlsx
+++ b/docs/srs/fbt_docs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Socio_02\Desktop\kjy\fbt\docs\srs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\kjy\fbt\docs\srs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D11E9EC-7D14-4A66-8751-552D611230F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D007A29-8362-41C9-A532-B3CAFD5E084A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2F0AD6B2-A8A2-4F73-BAF4-7193D3382EE1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2F0AD6B2-A8A2-4F73-BAF4-7193D3382EE1}"/>
   </bookViews>
   <sheets>
     <sheet name="요구사항명세서" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="TestCase_SQL" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">요구사항명세서!$B$8:$H$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">요구사항명세서!$B$8:$H$46</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="193">
   <si>
     <t>요구사항 정의서</t>
   </si>
@@ -4165,6 +4165,122 @@
         <charset val="129"/>
       </rPr>
       <t xml:space="preserve"> - transaction</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>V011</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>투표</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">결과 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>삭제</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>지인이 불참으로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>시</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>삭제</t>
     </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -4625,6 +4741,15 @@
     <xf numFmtId="0" fontId="11" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4641,15 +4766,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4967,34 +5083,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60EA499F-775F-49C1-B26C-B60E223B5AF8}">
-  <dimension ref="B1:I45"/>
+  <dimension ref="B1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="4.25" customWidth="1"/>
+    <col min="1" max="1" width="4.19921875" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="44" customWidth="1"/>
-    <col min="5" max="5" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.75" customWidth="1"/>
+    <col min="5" max="5" width="15.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.09765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.69921875" customWidth="1"/>
     <col min="8" max="8" width="9.5" customWidth="1"/>
-    <col min="9" max="9" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="17.25" thickBot="1"/>
-    <row r="2" spans="2:9" ht="18.75" thickBot="1">
-      <c r="B2" s="34" t="s">
+    <row r="1" spans="2:9" ht="18" thickBot="1"/>
+    <row r="2" spans="2:9" ht="18" thickBot="1">
+      <c r="B2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="35"/>
+      <c r="C2" s="38"/>
       <c r="E2" s="3" t="s">
         <v>64</v>
       </c>
@@ -5005,7 +5121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="17.25" thickBot="1">
+    <row r="3" spans="2:9" ht="18" thickBot="1">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -5020,7 +5136,7 @@
       </c>
       <c r="G3" s="21"/>
     </row>
-    <row r="4" spans="2:9" ht="17.25" thickBot="1">
+    <row r="4" spans="2:9" ht="18" thickBot="1">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -5035,7 +5151,7 @@
       </c>
       <c r="G4" s="21"/>
     </row>
-    <row r="5" spans="2:9" ht="17.25" thickBot="1">
+    <row r="5" spans="2:9" ht="18" thickBot="1">
       <c r="E5" s="25" t="s">
         <v>63</v>
       </c>
@@ -5043,7 +5159,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="17.25" thickBot="1">
+    <row r="6" spans="2:9" ht="18" thickBot="1">
       <c r="E6" s="30" t="s">
         <v>161</v>
       </c>
@@ -5051,46 +5167,46 @@
         <v>171</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="17.25" thickBot="1"/>
-    <row r="8" spans="2:9" ht="17.25" thickBot="1">
-      <c r="B8" s="32" t="s">
+    <row r="7" spans="2:9" ht="18" thickBot="1"/>
+    <row r="8" spans="2:9" ht="18" thickBot="1">
+      <c r="B8" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="37"/>
-      <c r="G8" s="32" t="s">
+      <c r="F8" s="40"/>
+      <c r="G8" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="32" t="s">
+      <c r="H8" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="32" t="s">
+      <c r="I8" s="35" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="17.25" thickBot="1">
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
+    <row r="9" spans="2:9" ht="18" thickBot="1">
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
       <c r="E9" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
     </row>
-    <row r="10" spans="2:9" ht="26.25" thickBot="1">
+    <row r="10" spans="2:9" ht="27" thickBot="1">
       <c r="B10" s="11" t="s">
         <v>65</v>
       </c>
@@ -5113,7 +5229,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="17.25" thickBot="1">
+    <row r="11" spans="2:9" ht="18" thickBot="1">
       <c r="B11" s="11" t="s">
         <v>66</v>
       </c>
@@ -5134,7 +5250,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="17.25" thickBot="1">
+    <row r="12" spans="2:9" ht="18" thickBot="1">
       <c r="B12" s="11" t="s">
         <v>67</v>
       </c>
@@ -5155,7 +5271,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="17.25" thickBot="1">
+    <row r="13" spans="2:9" ht="18" thickBot="1">
       <c r="B13" s="11" t="s">
         <v>68</v>
       </c>
@@ -5176,7 +5292,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="17.25" thickBot="1">
+    <row r="14" spans="2:9" ht="18" thickBot="1">
       <c r="B14" s="11" t="s">
         <v>69</v>
       </c>
@@ -5197,7 +5313,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="17.25" thickBot="1">
+    <row r="15" spans="2:9" ht="18" thickBot="1">
       <c r="B15" s="11" t="s">
         <v>70</v>
       </c>
@@ -5217,11 +5333,11 @@
       <c r="H15" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I15" s="38" t="s">
+      <c r="I15" s="32" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="17.25" thickBot="1">
+    <row r="16" spans="2:9" ht="18" thickBot="1">
       <c r="B16" s="17" t="s">
         <v>39</v>
       </c>
@@ -5241,11 +5357,11 @@
       <c r="H16" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="38" t="s">
+      <c r="I16" s="32" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="17.25" thickBot="1">
+    <row r="17" spans="2:9" ht="18" thickBot="1">
       <c r="B17" s="17" t="s">
         <v>172</v>
       </c>
@@ -5265,9 +5381,9 @@
       <c r="H17" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="38"/>
+      <c r="I17" s="32"/>
     </row>
-    <row r="18" spans="2:9" ht="27.75" thickBot="1">
+    <row r="18" spans="2:9" ht="31.8" thickBot="1">
       <c r="B18" s="17" t="s">
         <v>40</v>
       </c>
@@ -5287,11 +5403,11 @@
       <c r="H18" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I18" s="38" t="s">
+      <c r="I18" s="32" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="120.75" thickBot="1">
+    <row r="19" spans="2:9" ht="136.19999999999999" thickBot="1">
       <c r="B19" s="17" t="s">
         <v>41</v>
       </c>
@@ -5311,11 +5427,11 @@
       <c r="H19" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I19" s="39" t="s">
+      <c r="I19" s="33" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="68.25" thickBot="1">
+    <row r="20" spans="2:9" ht="78.599999999999994" thickBot="1">
       <c r="B20" s="17" t="s">
         <v>43</v>
       </c>
@@ -5335,11 +5451,11 @@
       <c r="H20" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="I20" s="39" t="s">
+      <c r="I20" s="33" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="291.75" thickBot="1">
+    <row r="21" spans="2:9" ht="324.60000000000002" thickBot="1">
       <c r="B21" s="17" t="s">
         <v>47</v>
       </c>
@@ -5360,7 +5476,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="26.25" thickBot="1">
+    <row r="22" spans="2:9" ht="27" thickBot="1">
       <c r="B22" s="19" t="s">
         <v>48</v>
       </c>
@@ -5382,12 +5498,12 @@
       <c r="H22" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="I22" s="39" t="s">
+      <c r="I22" s="33" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="27" thickBot="1">
-      <c r="B23" s="40" t="s">
+    <row r="23" spans="2:9" ht="29.4" thickBot="1">
+      <c r="B23" s="34" t="s">
         <v>178</v>
       </c>
       <c r="C23" s="12" t="s">
@@ -5404,10 +5520,10 @@
       </c>
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
-      <c r="I23" s="39"/>
+      <c r="I23" s="33"/>
     </row>
-    <row r="24" spans="2:9" ht="17.25" thickBot="1">
-      <c r="B24" s="40" t="s">
+    <row r="24" spans="2:9" ht="18" thickBot="1">
+      <c r="B24" s="34" t="s">
         <v>180</v>
       </c>
       <c r="C24" s="12" t="s">
@@ -5424,10 +5540,10 @@
       </c>
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
-      <c r="I24" s="39"/>
+      <c r="I24" s="33"/>
     </row>
-    <row r="25" spans="2:9" ht="27" thickBot="1">
-      <c r="B25" s="40" t="s">
+    <row r="25" spans="2:9" ht="29.4" thickBot="1">
+      <c r="B25" s="34" t="s">
         <v>182</v>
       </c>
       <c r="C25" s="12" t="s">
@@ -5444,38 +5560,35 @@
       </c>
       <c r="G25" s="12"/>
       <c r="H25" s="12"/>
-      <c r="I25" s="39"/>
+      <c r="I25" s="33"/>
     </row>
-    <row r="26" spans="2:9" ht="17.25" thickBot="1">
-      <c r="B26" s="20" t="s">
+    <row r="26" spans="2:9" ht="18" thickBot="1">
+      <c r="B26" s="34" t="s">
+        <v>190</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" s="15"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="33"/>
+    </row>
+    <row r="27" spans="2:9" ht="18" thickBot="1">
+      <c r="B27" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C27" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D27" s="13" t="s">
         <v>53</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H26" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" ht="17.25" thickBot="1">
-      <c r="B27" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>55</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>45</v>
@@ -5485,60 +5598,60 @@
         <v>16</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="28" spans="2:9" ht="26.25" thickBot="1">
+    <row r="28" spans="2:9" ht="18" thickBot="1">
       <c r="B28" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>56</v>
+        <v>26</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>54</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>45</v>
       </c>
       <c r="F28" s="12"/>
       <c r="G28" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H28" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="H28" s="12" t="s">
-        <v>46</v>
-      </c>
     </row>
-    <row r="29" spans="2:9" ht="17.25" thickBot="1">
+    <row r="29" spans="2:9" ht="27" thickBot="1">
       <c r="B29" s="20" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>45</v>
       </c>
       <c r="F29" s="12"/>
       <c r="G29" s="12" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="30" spans="2:9" ht="17.25" thickBot="1">
+    <row r="30" spans="2:9" ht="18" thickBot="1">
       <c r="B30" s="20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>45</v>
@@ -5548,104 +5661,104 @@
         <v>16</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="31" spans="2:9" ht="80.25" thickBot="1">
+    <row r="31" spans="2:9" ht="18" thickBot="1">
       <c r="B31" s="20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="D31" s="18" t="s">
-        <v>82</v>
+        <v>74</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>75</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>45</v>
       </c>
       <c r="F31" s="12"/>
       <c r="G31" s="12" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="H31" s="12" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="2:9" ht="17.25" thickBot="1">
+    <row r="32" spans="2:9" ht="91.8" thickBot="1">
       <c r="B32" s="20" t="s">
-        <v>77</v>
+        <v>36</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>45</v>
       </c>
       <c r="F32" s="12"/>
       <c r="G32" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H32" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H32" s="12" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="27.75" thickBot="1">
+    <row r="33" spans="2:8" ht="18" thickBot="1">
       <c r="B33" s="20" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="E33" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E33" s="12" t="s">
         <v>45</v>
       </c>
       <c r="F33" s="12"/>
       <c r="G33" s="12" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="H33" s="15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="17.25" thickBot="1">
-      <c r="B34" s="22" t="s">
-        <v>71</v>
+    <row r="34" spans="2:8" ht="31.8" thickBot="1">
+      <c r="B34" s="20" t="s">
+        <v>80</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>24</v>
+        <v>81</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>45</v>
       </c>
       <c r="F34" s="12"/>
       <c r="G34" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H34" s="12" t="s">
-        <v>16</v>
+        <v>25</v>
+      </c>
+      <c r="H34" s="15" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="17.25" thickBot="1">
+    <row r="35" spans="2:8" ht="18" thickBot="1">
       <c r="B35" s="22" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="E35" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" s="12" t="s">
         <v>24</v>
       </c>
       <c r="F35" s="12"/>
@@ -5653,83 +5766,83 @@
         <v>16</v>
       </c>
       <c r="H35" s="12" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="17.25" thickBot="1">
+    <row r="36" spans="2:8" ht="18" thickBot="1">
       <c r="B36" s="22" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="F36" s="12"/>
       <c r="G36" s="12" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="H36" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="17.25" thickBot="1">
+    <row r="37" spans="2:8" ht="18" thickBot="1">
       <c r="B37" s="22" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="F37" s="12"/>
       <c r="G37" s="12" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H37" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="17.25" thickBot="1">
+    <row r="38" spans="2:8" ht="18" thickBot="1">
       <c r="B38" s="22" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="F38" s="12"/>
       <c r="G38" s="12" t="s">
         <v>16</v>
       </c>
       <c r="H38" s="12" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="17.25" thickBot="1">
-      <c r="B39" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>101</v>
+    <row r="39" spans="2:8" ht="18" thickBot="1">
+      <c r="B39" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>96</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="E39" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E39" s="15" t="s">
         <v>45</v>
       </c>
       <c r="F39" s="12"/>
@@ -5737,18 +5850,18 @@
         <v>16</v>
       </c>
       <c r="H39" s="12" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="17.25" thickBot="1">
+    <row r="40" spans="2:8" ht="18" thickBot="1">
       <c r="B40" s="29" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="D40" s="18" t="s">
-        <v>103</v>
+        <v>101</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>99</v>
       </c>
       <c r="E40" s="12" t="s">
         <v>45</v>
@@ -5761,15 +5874,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="17.25" thickBot="1">
+    <row r="41" spans="2:8" ht="18" thickBot="1">
       <c r="B41" s="29" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E41" s="12" t="s">
         <v>45</v>
@@ -5782,15 +5895,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="2:8" ht="17.25" thickBot="1">
+    <row r="42" spans="2:8" ht="18" thickBot="1">
       <c r="B42" s="29" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E42" s="12" t="s">
         <v>45</v>
@@ -5800,18 +5913,18 @@
         <v>16</v>
       </c>
       <c r="H42" s="12" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="17.25" thickBot="1">
+    <row r="43" spans="2:8" ht="18" thickBot="1">
       <c r="B43" s="29" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E43" s="12" t="s">
         <v>45</v>
@@ -5821,17 +5934,19 @@
         <v>16</v>
       </c>
       <c r="H43" s="12" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="44" spans="2:8" ht="17.25" thickBot="1">
+    <row r="44" spans="2:8" ht="18" thickBot="1">
       <c r="B44" s="29" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="D44" s="18"/>
+        <v>111</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>112</v>
+      </c>
       <c r="E44" s="12" t="s">
         <v>45</v>
       </c>
@@ -5839,18 +5954,18 @@
       <c r="G44" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="H44" s="12"/>
+      <c r="H44" s="12" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="45" spans="2:8" ht="27.75" thickBot="1">
-      <c r="B45" s="31" t="s">
-        <v>162</v>
+    <row r="45" spans="2:8" ht="18" thickBot="1">
+      <c r="B45" s="29" t="s">
+        <v>113</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="D45" s="18" t="s">
-        <v>166</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="D45" s="18"/>
       <c r="E45" s="12" t="s">
         <v>45</v>
       </c>
@@ -5858,12 +5973,31 @@
       <c r="G45" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="H45" s="12" t="s">
+      <c r="H45" s="12"/>
+    </row>
+    <row r="46" spans="2:8" ht="31.8" thickBot="1">
+      <c r="B46" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H46" s="12" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B8:H45" xr:uid="{08681459-A406-4CEE-9A8A-D3DF83B63176}">
+  <autoFilter ref="B8:H46" xr:uid="{08681459-A406-4CEE-9A8A-D3DF83B63176}">
     <filterColumn colId="3" showButton="0"/>
   </autoFilter>
   <mergeCells count="8">
@@ -5890,9 +6024,9 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -5933,10 +6067,10 @@
       <selection activeCell="Q24" sqref="Q24:Q38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38">
@@ -6021,21 +6155,21 @@
       </c>
       <c r="AB1">
         <f ca="1">RANDBETWEEN(170,185)</f>
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="AC1" t="s">
         <v>120</v>
       </c>
       <c r="AD1">
         <f ca="1">RANDBETWEEN(70,80)</f>
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="AE1" t="s">
         <v>120</v>
       </c>
       <c r="AF1">
         <f ca="1">RANDBETWEEN(0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG1" t="s">
         <v>120</v>
@@ -6055,7 +6189,7 @@
       </c>
       <c r="AL1" t="str">
         <f ca="1">_xlfn.CONCAT(A1:AK1)</f>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman1@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,182,78,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman1@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,172,70,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="2" spans="1:38">
@@ -6140,28 +6274,28 @@
       </c>
       <c r="AB2">
         <f t="shared" ref="AB2:AB17" ca="1" si="0">RANDBETWEEN(170,185)</f>
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="AC2" t="s">
         <v>120</v>
       </c>
       <c r="AD2">
         <f t="shared" ref="AD2:AD17" ca="1" si="1">RANDBETWEEN(70,80)</f>
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AE2" t="s">
         <v>120</v>
       </c>
       <c r="AF2">
         <f t="shared" ref="AF2:AF17" ca="1" si="2">RANDBETWEEN(0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG2" t="s">
         <v>120</v>
       </c>
       <c r="AH2">
         <f t="shared" ref="AH2:AH17" ca="1" si="3">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI2" t="s">
         <v>120</v>
@@ -6174,7 +6308,7 @@
       </c>
       <c r="AL2" t="str">
         <f t="shared" ref="AL2:AL17" ca="1" si="4">_xlfn.CONCAT(A2:AK2)</f>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman2@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,177,80,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman2@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,174,79,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="3" spans="1:38">
@@ -6259,21 +6393,21 @@
       </c>
       <c r="AB3">
         <f t="shared" ca="1" si="0"/>
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="AC3" t="s">
         <v>120</v>
       </c>
       <c r="AD3">
         <f t="shared" ca="1" si="1"/>
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="AE3" t="s">
         <v>120</v>
       </c>
       <c r="AF3">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG3" t="s">
         <v>120</v>
@@ -6293,7 +6427,7 @@
       </c>
       <c r="AL3" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman3@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,175,72,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman3@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,171,75,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="4" spans="1:38">
@@ -6378,28 +6512,28 @@
       </c>
       <c r="AB4">
         <f t="shared" ca="1" si="0"/>
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="AC4" t="s">
         <v>120</v>
       </c>
       <c r="AD4">
         <f t="shared" ca="1" si="1"/>
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="AE4" t="s">
         <v>120</v>
       </c>
       <c r="AF4">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG4" t="s">
         <v>120</v>
       </c>
       <c r="AH4">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI4" t="s">
         <v>120</v>
@@ -6412,7 +6546,7 @@
       </c>
       <c r="AL4" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman4@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,185,76,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman4@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,181,73,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="5" spans="1:38">
@@ -6497,28 +6631,28 @@
       </c>
       <c r="AB5">
         <f t="shared" ca="1" si="0"/>
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="AC5" t="s">
         <v>120</v>
       </c>
       <c r="AD5">
         <f t="shared" ca="1" si="1"/>
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="AE5" t="s">
         <v>120</v>
       </c>
       <c r="AF5">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG5" t="s">
         <v>120</v>
       </c>
       <c r="AH5">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI5" t="s">
         <v>120</v>
@@ -6531,7 +6665,7 @@
       </c>
       <c r="AL5" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman5@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,173,76,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman5@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,184,79,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="6" spans="1:38">
@@ -6616,7 +6750,7 @@
       </c>
       <c r="AB6">
         <f t="shared" ca="1" si="0"/>
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="AC6" t="s">
         <v>120</v>
@@ -6650,7 +6784,7 @@
       </c>
       <c r="AL6" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman6@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,183,74,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman6@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,177,74,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="7" spans="1:38">
@@ -6735,28 +6869,28 @@
       </c>
       <c r="AB7">
         <f t="shared" ca="1" si="0"/>
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="AC7" t="s">
         <v>120</v>
       </c>
       <c r="AD7">
         <f t="shared" ca="1" si="1"/>
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="AE7" t="s">
         <v>120</v>
       </c>
       <c r="AF7">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG7" t="s">
         <v>120</v>
       </c>
       <c r="AH7">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI7" t="s">
         <v>120</v>
@@ -6769,7 +6903,7 @@
       </c>
       <c r="AL7" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman7@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,171,74,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman7@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,173,79,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="8" spans="1:38">
@@ -6854,21 +6988,21 @@
       </c>
       <c r="AB8">
         <f t="shared" ca="1" si="0"/>
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="AC8" t="s">
         <v>120</v>
       </c>
       <c r="AD8">
         <f t="shared" ca="1" si="1"/>
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="AE8" t="s">
         <v>120</v>
       </c>
       <c r="AF8">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG8" t="s">
         <v>120</v>
@@ -6888,7 +7022,7 @@
       </c>
       <c r="AL8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman8@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,178,72,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman8@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,174,79,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="9" spans="1:38">
@@ -6980,7 +7114,7 @@
       </c>
       <c r="AD9">
         <f t="shared" ca="1" si="1"/>
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="AE9" t="s">
         <v>120</v>
@@ -6994,7 +7128,7 @@
       </c>
       <c r="AH9">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI9" t="s">
         <v>120</v>
@@ -7007,7 +7141,7 @@
       </c>
       <c r="AL9" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman9@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,174,80,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman9@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,174,78,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="10" spans="1:38">
@@ -7092,21 +7226,21 @@
       </c>
       <c r="AB10">
         <f t="shared" ca="1" si="0"/>
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="AC10" t="s">
         <v>120</v>
       </c>
       <c r="AD10">
         <f t="shared" ca="1" si="1"/>
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="AE10" t="s">
         <v>120</v>
       </c>
       <c r="AF10">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG10" t="s">
         <v>120</v>
@@ -7126,7 +7260,7 @@
       </c>
       <c r="AL10" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman10@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,185,76,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman10@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,177,71,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="11" spans="1:38">
@@ -7211,14 +7345,14 @@
       </c>
       <c r="AB11">
         <f t="shared" ca="1" si="0"/>
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AC11" t="s">
         <v>120</v>
       </c>
       <c r="AD11">
         <f t="shared" ca="1" si="1"/>
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AE11" t="s">
         <v>120</v>
@@ -7232,7 +7366,7 @@
       </c>
       <c r="AH11">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI11" t="s">
         <v>120</v>
@@ -7245,7 +7379,7 @@
       </c>
       <c r="AL11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman11@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,178,75,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman11@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,177,73,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="12" spans="1:38">
@@ -7330,14 +7464,14 @@
       </c>
       <c r="AB12">
         <f t="shared" ca="1" si="0"/>
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="AC12" t="s">
         <v>120</v>
       </c>
       <c r="AD12">
         <f t="shared" ca="1" si="1"/>
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="AE12" t="s">
         <v>120</v>
@@ -7364,7 +7498,7 @@
       </c>
       <c r="AL12" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman12@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,172,71,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman12@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,176,77,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="13" spans="1:38">
@@ -7449,28 +7583,28 @@
       </c>
       <c r="AB13">
         <f t="shared" ca="1" si="0"/>
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="AC13" t="s">
         <v>120</v>
       </c>
       <c r="AD13">
         <f t="shared" ca="1" si="1"/>
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="AE13" t="s">
         <v>120</v>
       </c>
       <c r="AF13">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG13" t="s">
         <v>120</v>
       </c>
       <c r="AH13">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI13" t="s">
         <v>120</v>
@@ -7483,7 +7617,7 @@
       </c>
       <c r="AL13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman13@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,181,70,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman13@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,174,73,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="14" spans="1:38">
@@ -7568,14 +7702,14 @@
       </c>
       <c r="AB14">
         <f t="shared" ca="1" si="0"/>
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="AC14" t="s">
         <v>120</v>
       </c>
       <c r="AD14">
         <f t="shared" ca="1" si="1"/>
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="AE14" t="s">
         <v>120</v>
@@ -7589,7 +7723,7 @@
       </c>
       <c r="AH14">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI14" t="s">
         <v>120</v>
@@ -7602,7 +7736,7 @@
       </c>
       <c r="AL14" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman14@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,185,71,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman14@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,176,73,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="15" spans="1:38">
@@ -7687,28 +7821,28 @@
       </c>
       <c r="AB15">
         <f t="shared" ca="1" si="0"/>
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="AC15" t="s">
         <v>120</v>
       </c>
       <c r="AD15">
         <f t="shared" ca="1" si="1"/>
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="AE15" t="s">
         <v>120</v>
       </c>
       <c r="AF15">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG15" t="s">
         <v>120</v>
       </c>
       <c r="AH15">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI15" t="s">
         <v>120</v>
@@ -7721,7 +7855,7 @@
       </c>
       <c r="AL15" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman15@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,178,76,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman15@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,185,78,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="16" spans="1:38">
@@ -7813,7 +7947,7 @@
       </c>
       <c r="AD16">
         <f t="shared" ca="1" si="1"/>
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AE16" t="s">
         <v>120</v>
@@ -7840,7 +7974,7 @@
       </c>
       <c r="AL16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman16@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,179,75,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman16@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,179,76,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="17" spans="1:38">
@@ -7925,14 +8059,14 @@
       </c>
       <c r="AB17">
         <f t="shared" ca="1" si="0"/>
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="AC17" t="s">
         <v>120</v>
       </c>
       <c r="AD17">
         <f t="shared" ca="1" si="1"/>
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AE17" t="s">
         <v>120</v>
@@ -7959,7 +8093,7 @@
       </c>
       <c r="AL17" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman17@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,178,72,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman17@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,171,70,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="20" spans="1:38">
@@ -8014,7 +8148,7 @@
       </c>
       <c r="Q20">
         <f ca="1">RANDBETWEEN(0,5)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R20" t="s">
         <v>120</v>
@@ -8048,7 +8182,7 @@
       </c>
       <c r="AB20" t="str">
         <f ca="1">_xlfn.CONCAT(A20:AA20)</f>
-        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('왕십리FC','왕십리FC201018.jpg','성동구','성동구 구장','red',0,'2016-01-01',sysdate(),'1234','기업');</v>
+        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('왕십리FC','왕십리FC201018.jpg','성동구','성동구 구장','red',3,'2016-01-01',sysdate(),'1234','기업');</v>
       </c>
     </row>
     <row r="21" spans="1:38">
@@ -8103,7 +8237,7 @@
       </c>
       <c r="Q21">
         <f t="shared" ref="Q21:Q22" ca="1" si="6">RANDBETWEEN(0,5)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R21" t="s">
         <v>120</v>
@@ -8137,7 +8271,7 @@
       </c>
       <c r="AB21" t="str">
         <f t="shared" ref="AB21:AB22" ca="1" si="7">_xlfn.CONCAT(A21:AA21)</f>
-        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('답십리FC','답십리FC201018.jpg','성동구','응봉동 구장','blue',3,'2017-01-01',sysdate(),'5678','하나');</v>
+        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('답십리FC','답십리FC201018.jpg','성동구','응봉동 구장','blue',0,'2017-01-01',sysdate(),'5678','하나');</v>
       </c>
     </row>
     <row r="22" spans="1:38">
@@ -8192,7 +8326,7 @@
       </c>
       <c r="Q22">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R22" t="s">
         <v>120</v>
@@ -8226,7 +8360,7 @@
       </c>
       <c r="AB22" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('대구FC','대구FC201018.jpg','달서구','달서구 구장','green',0,'2018-01-01',sysdate(),'2345','기업');</v>
+        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('대구FC','대구FC201018.jpg','달서구','달서구 구장','green',5,'2018-01-01',sysdate(),'2345','기업');</v>
       </c>
     </row>
     <row r="24" spans="1:38">

</xml_diff>

<commit_message>
[2020-10-28 21:36] VoteMach View 수정 중
</commit_message>
<xml_diff>
--- a/docs/srs/fbt_docs.xlsx
+++ b/docs/srs/fbt_docs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\kjy\fbt\docs\srs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Socio_02\Desktop\kjy\fbt\docs\srs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D007A29-8362-41C9-A532-B3CAFD5E084A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65AD6BEA-D3D8-40F0-9C1E-3CAD07619263}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2F0AD6B2-A8A2-4F73-BAF4-7193D3382EE1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2F0AD6B2-A8A2-4F73-BAF4-7193D3382EE1}"/>
   </bookViews>
   <sheets>
     <sheet name="요구사항명세서" sheetId="1" r:id="rId1"/>
@@ -2210,98 +2210,225 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>설정에</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>따라</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>해당</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>기능들을</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>연결하기</t>
+    <t>완성 여부</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>ㅇ</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AL - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>알림</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>관련</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>기능</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>V002</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>참</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>또는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>불</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수정</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>참</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>또는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>불</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>입력</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Nanum Gothic"/>
-        <family val="2"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t xml:space="preserve">
 - </t>
@@ -2314,6 +2441,1385 @@
         <family val="3"/>
         <charset val="129"/>
       </rPr>
+      <t>에러</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>기투표</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>시</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> update</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>전환</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>화면단에서</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> V003</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>해당</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>지인에게</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>초대</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>보내기(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">invite)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>투표하면</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>안</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>하면</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>아예</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>넣지</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>않기(투표 취소)
+추후</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>채팅으로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>변환</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>생각</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">중
+경기 관련 글은 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">match_schedule </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>참조</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>알람</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>화면</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>단에서</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>투표</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">?
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>insert</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>를 진행하나 에러 뜨면 기투표 여부 확인 후 기투표 시, 이미 투표했다고 알림 아니면 에러 페이지</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+V003</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>으로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>연결
+마이페이지에서 투표 취소</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>투표 결과</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수정</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>투표 결과</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>입력</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>V008</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>투표 내용 수정</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>V009</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>투표 삭제</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>V010</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>투표 설정 수정</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>진행 중 투표 출력</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>작성자만 가능(닉은 유니크)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>진행</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>중인</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>투표</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>내용</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+?? 수정일이 필요한가?</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>진행</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>중인</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>투표</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>삭제</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>기설정된</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>투표</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>설정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>변경</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+- 변경된 설정에 맞게 자동화도 수정</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>입력한</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>내용에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>따라</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>투표</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>입력하기
+팀 경기 일정 자동 추가(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t>S001)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>팀원</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>전체에게</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>알람</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>보내기(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t>T002)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+카톡 푸시 알람(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t>T003)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>투표</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>설정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(V006)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> - transaction</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>V011</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>투표</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">결과 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>삭제</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>지인이 불참으로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>시</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>삭제</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>설정에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>따라</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>해당</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>기능들을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>연결하기</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
       <t xml:space="preserve">용병구하기
 </t>
     </r>
@@ -2473,18 +3979,18 @@
         <family val="3"/>
         <charset val="129"/>
       </rPr>
-      <t xml:space="preserve">type
-0 : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">수동
+      <t>type
+0 : 수동</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -2775,1512 +4281,6 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> : cancel_num, away_min_num, emp_min_num, self_min_num, self_max_num, emp_due_date, away_due_date</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>완성 여부</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>ㅇ</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">AL - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>알림</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>관련</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>기능</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>V002</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>참</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>또는</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>불</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>수정</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>참</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>또는</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>불</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>입력</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nanum Gothic"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">
-- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>에러</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>기투표</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>시</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> update</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>로</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>전환</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nanum Gothic"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>화면단에서</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nanum Gothic"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve"> V003</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>해당</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>지인에게</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>초대</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>보내기(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nanum Gothic"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">invite)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>투표하면</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 1 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>안</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>하면</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>아예</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>넣지</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>않기(투표 취소)
-추후</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>채팅으로</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>변환</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>생각</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">중
-경기 관련 글은 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nanum Gothic"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">match_schedule </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>참조</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nanum Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>알람</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>화면</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>단에서</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>투표</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">?
-- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nanum Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>insert</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nanum Gothic"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>를 진행하나 에러 뜨면 기투표 여부 확인 후 기투표 시, 이미 투표했다고 알림 아니면 에러 페이지</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nanum Gothic"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">
-V003</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>으로</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>연결
-마이페이지에서 투표 취소</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>투표 결과</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>수정</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>투표 결과</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>입력</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>V008</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>투표 내용 수정</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>V009</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>투표 삭제</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>V010</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>투표 설정 수정</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>진행 중 투표 출력</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>작성자만 가능(닉은 유니크)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>진행</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>중인</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>투표</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>내용</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>수정</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nanum Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-?? 수정일이 필요한가?</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>진행</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>중인</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>투표</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>삭제</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>기설정된</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>투표</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>설정</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>변경</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nanum Gothic"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">
-- 변경된 설정에 맞게 자동화도 수정</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>입력한</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>내용에</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>따라</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>투표</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>입력하기
-팀 경기 일정 자동 추가(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nanum Gothic"/>
-        <family val="3"/>
-      </rPr>
-      <t>S001)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nanum Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>팀원</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>전체에게</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>알람</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>보내기(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nanum Gothic"/>
-        <family val="3"/>
-      </rPr>
-      <t>T002)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">
-카톡 푸시 알람(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nanum Gothic"/>
-        <family val="3"/>
-      </rPr>
-      <t>T003)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nanum Gothic"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>투표</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>설정</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(V006)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nanum Gothic"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve"> - transaction</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>V011</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>투표</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="돋움"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">결과 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>삭제</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>지인이 불참으로</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>수정</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>시</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>삭제</t>
     </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -5086,27 +5086,27 @@
   <dimension ref="B1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
+      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="4.19921875" customWidth="1"/>
+    <col min="1" max="1" width="4.25" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="44" customWidth="1"/>
-    <col min="5" max="5" width="15.8984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.09765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.69921875" customWidth="1"/>
+    <col min="5" max="5" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.75" customWidth="1"/>
     <col min="8" max="8" width="9.5" customWidth="1"/>
-    <col min="9" max="9" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="18" thickBot="1"/>
-    <row r="2" spans="2:9" ht="18" thickBot="1">
+    <row r="1" spans="2:9" ht="17.25" thickBot="1"/>
+    <row r="2" spans="2:9" ht="18.75" thickBot="1">
       <c r="B2" s="37" t="s">
         <v>0</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="18" thickBot="1">
+    <row r="3" spans="2:9" ht="17.25" thickBot="1">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -5136,7 +5136,7 @@
       </c>
       <c r="G3" s="21"/>
     </row>
-    <row r="4" spans="2:9" ht="18" thickBot="1">
+    <row r="4" spans="2:9" ht="17.25" thickBot="1">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -5151,7 +5151,7 @@
       </c>
       <c r="G4" s="21"/>
     </row>
-    <row r="5" spans="2:9" ht="18" thickBot="1">
+    <row r="5" spans="2:9" ht="17.25" thickBot="1">
       <c r="E5" s="25" t="s">
         <v>63</v>
       </c>
@@ -5159,16 +5159,16 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="18" thickBot="1">
+    <row r="6" spans="2:9" ht="17.25" thickBot="1">
       <c r="E6" s="30" t="s">
         <v>161</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="18" thickBot="1"/>
-    <row r="8" spans="2:9" ht="18" thickBot="1">
+    <row r="7" spans="2:9" ht="17.25" thickBot="1"/>
+    <row r="8" spans="2:9" ht="17.25" thickBot="1">
       <c r="B8" s="35" t="s">
         <v>4</v>
       </c>
@@ -5189,10 +5189,10 @@
         <v>11</v>
       </c>
       <c r="I8" s="35" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="18" thickBot="1">
+    <row r="9" spans="2:9" ht="17.25" thickBot="1">
       <c r="B9" s="36"/>
       <c r="C9" s="36"/>
       <c r="D9" s="36"/>
@@ -5206,7 +5206,7 @@
       <c r="H9" s="36"/>
       <c r="I9" s="36"/>
     </row>
-    <row r="10" spans="2:9" ht="27" thickBot="1">
+    <row r="10" spans="2:9" ht="26.25" thickBot="1">
       <c r="B10" s="11" t="s">
         <v>65</v>
       </c>
@@ -5229,7 +5229,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="18" thickBot="1">
+    <row r="11" spans="2:9" ht="17.25" thickBot="1">
       <c r="B11" s="11" t="s">
         <v>66</v>
       </c>
@@ -5250,7 +5250,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="18" thickBot="1">
+    <row r="12" spans="2:9" ht="17.25" thickBot="1">
       <c r="B12" s="11" t="s">
         <v>67</v>
       </c>
@@ -5271,7 +5271,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="18" thickBot="1">
+    <row r="13" spans="2:9" ht="17.25" thickBot="1">
       <c r="B13" s="11" t="s">
         <v>68</v>
       </c>
@@ -5292,7 +5292,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="18" thickBot="1">
+    <row r="14" spans="2:9" ht="17.25" thickBot="1">
       <c r="B14" s="11" t="s">
         <v>69</v>
       </c>
@@ -5313,7 +5313,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="18" thickBot="1">
+    <row r="15" spans="2:9" ht="17.25" thickBot="1">
       <c r="B15" s="11" t="s">
         <v>70</v>
       </c>
@@ -5334,15 +5334,15 @@
         <v>16</v>
       </c>
       <c r="I15" s="32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="18" thickBot="1">
+    <row r="16" spans="2:9" ht="17.25" thickBot="1">
       <c r="B16" s="17" t="s">
         <v>39</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>86</v>
@@ -5358,18 +5358,18 @@
         <v>25</v>
       </c>
       <c r="I16" s="32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="18" thickBot="1">
+    <row r="17" spans="2:9" ht="17.25" thickBot="1">
       <c r="B17" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="D17" s="18" t="s">
         <v>172</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>176</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>173</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>30</v>
@@ -5383,15 +5383,15 @@
       </c>
       <c r="I17" s="32"/>
     </row>
-    <row r="18" spans="2:9" ht="31.8" thickBot="1">
+    <row r="18" spans="2:9" ht="27.75" thickBot="1">
       <c r="B18" s="17" t="s">
         <v>40</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>30</v>
@@ -5404,10 +5404,10 @@
         <v>25</v>
       </c>
       <c r="I18" s="32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="136.19999999999999" thickBot="1">
+    <row r="19" spans="2:9" ht="120.75" thickBot="1">
       <c r="B19" s="17" t="s">
         <v>41</v>
       </c>
@@ -5415,7 +5415,7 @@
         <v>42</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E19" s="12" t="s">
         <v>30</v>
@@ -5428,10 +5428,10 @@
         <v>25</v>
       </c>
       <c r="I19" s="33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="78.599999999999994" thickBot="1">
+    <row r="20" spans="2:9" ht="68.25" thickBot="1">
       <c r="B20" s="17" t="s">
         <v>43</v>
       </c>
@@ -5439,7 +5439,7 @@
         <v>44</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>45</v>
@@ -5452,10 +5452,10 @@
         <v>46</v>
       </c>
       <c r="I20" s="33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="324.60000000000002" thickBot="1">
+    <row r="21" spans="2:9" ht="291.75" thickBot="1">
       <c r="B21" s="17" t="s">
         <v>47</v>
       </c>
@@ -5463,7 +5463,7 @@
         <v>167</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>168</v>
+        <v>192</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>45</v>
@@ -5476,7 +5476,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="27" thickBot="1">
+    <row r="22" spans="2:9" ht="26.25" thickBot="1">
       <c r="B22" s="19" t="s">
         <v>48</v>
       </c>
@@ -5499,78 +5499,78 @@
         <v>46</v>
       </c>
       <c r="I22" s="33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="29.4" thickBot="1">
+    <row r="23" spans="2:9" ht="27" thickBot="1">
       <c r="B23" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="C23" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>179</v>
-      </c>
       <c r="D23" s="18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E23" s="12" t="s">
         <v>45</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
       <c r="I23" s="33"/>
     </row>
-    <row r="24" spans="2:9" ht="18" thickBot="1">
+    <row r="24" spans="2:9" ht="17.25" thickBot="1">
       <c r="B24" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="C24" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>181</v>
-      </c>
       <c r="D24" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>45</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
       <c r="I24" s="33"/>
     </row>
-    <row r="25" spans="2:9" ht="29.4" thickBot="1">
+    <row r="25" spans="2:9" ht="27" thickBot="1">
       <c r="B25" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="C25" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>183</v>
-      </c>
       <c r="D25" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>45</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G25" s="12"/>
       <c r="H25" s="12"/>
       <c r="I25" s="33"/>
     </row>
-    <row r="26" spans="2:9" ht="18" thickBot="1">
+    <row r="26" spans="2:9" ht="17.25" thickBot="1">
       <c r="B26" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="C26" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="D26" s="18" t="s">
         <v>191</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>192</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>30</v>
@@ -5580,7 +5580,7 @@
       <c r="H26" s="12"/>
       <c r="I26" s="33"/>
     </row>
-    <row r="27" spans="2:9" ht="18" thickBot="1">
+    <row r="27" spans="2:9" ht="17.25" thickBot="1">
       <c r="B27" s="20" t="s">
         <v>18</v>
       </c>
@@ -5601,7 +5601,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="2:9" ht="18" thickBot="1">
+    <row r="28" spans="2:9" ht="17.25" thickBot="1">
       <c r="B28" s="20" t="s">
         <v>26</v>
       </c>
@@ -5622,7 +5622,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="2:9" ht="27" thickBot="1">
+    <row r="29" spans="2:9" ht="26.25" thickBot="1">
       <c r="B29" s="20" t="s">
         <v>27</v>
       </c>
@@ -5643,7 +5643,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="2:9" ht="18" thickBot="1">
+    <row r="30" spans="2:9" ht="17.25" thickBot="1">
       <c r="B30" s="20" t="s">
         <v>31</v>
       </c>
@@ -5664,7 +5664,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="2:9" ht="18" thickBot="1">
+    <row r="31" spans="2:9" ht="17.25" thickBot="1">
       <c r="B31" s="20" t="s">
         <v>34</v>
       </c>
@@ -5685,7 +5685,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="2:9" ht="91.8" thickBot="1">
+    <row r="32" spans="2:9" ht="80.25" thickBot="1">
       <c r="B32" s="20" t="s">
         <v>36</v>
       </c>
@@ -5706,7 +5706,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="18" thickBot="1">
+    <row r="33" spans="2:8" ht="17.25" thickBot="1">
       <c r="B33" s="20" t="s">
         <v>77</v>
       </c>
@@ -5727,7 +5727,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="31.8" thickBot="1">
+    <row r="34" spans="2:8" ht="27.75" thickBot="1">
       <c r="B34" s="20" t="s">
         <v>80</v>
       </c>
@@ -5748,7 +5748,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="18" thickBot="1">
+    <row r="35" spans="2:8" ht="17.25" thickBot="1">
       <c r="B35" s="22" t="s">
         <v>71</v>
       </c>
@@ -5769,7 +5769,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="18" thickBot="1">
+    <row r="36" spans="2:8" ht="17.25" thickBot="1">
       <c r="B36" s="22" t="s">
         <v>84</v>
       </c>
@@ -5790,7 +5790,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="18" thickBot="1">
+    <row r="37" spans="2:8" ht="17.25" thickBot="1">
       <c r="B37" s="22" t="s">
         <v>88</v>
       </c>
@@ -5811,7 +5811,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="18" thickBot="1">
+    <row r="38" spans="2:8" ht="17.25" thickBot="1">
       <c r="B38" s="22" t="s">
         <v>92</v>
       </c>
@@ -5832,7 +5832,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="18" thickBot="1">
+    <row r="39" spans="2:8" ht="17.25" thickBot="1">
       <c r="B39" s="22" t="s">
         <v>95</v>
       </c>
@@ -5853,7 +5853,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="18" thickBot="1">
+    <row r="40" spans="2:8" ht="17.25" thickBot="1">
       <c r="B40" s="29" t="s">
         <v>98</v>
       </c>
@@ -5874,7 +5874,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="18" thickBot="1">
+    <row r="41" spans="2:8" ht="17.25" thickBot="1">
       <c r="B41" s="29" t="s">
         <v>100</v>
       </c>
@@ -5895,7 +5895,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="2:8" ht="18" thickBot="1">
+    <row r="42" spans="2:8" ht="17.25" thickBot="1">
       <c r="B42" s="29" t="s">
         <v>104</v>
       </c>
@@ -5916,7 +5916,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="18" thickBot="1">
+    <row r="43" spans="2:8" ht="17.25" thickBot="1">
       <c r="B43" s="29" t="s">
         <v>107</v>
       </c>
@@ -5937,7 +5937,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="2:8" ht="18" thickBot="1">
+    <row r="44" spans="2:8" ht="17.25" thickBot="1">
       <c r="B44" s="29" t="s">
         <v>110</v>
       </c>
@@ -5958,7 +5958,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="2:8" ht="18" thickBot="1">
+    <row r="45" spans="2:8" ht="17.25" thickBot="1">
       <c r="B45" s="29" t="s">
         <v>113</v>
       </c>
@@ -5975,7 +5975,7 @@
       </c>
       <c r="H45" s="12"/>
     </row>
-    <row r="46" spans="2:8" ht="31.8" thickBot="1">
+    <row r="46" spans="2:8" ht="27.75" thickBot="1">
       <c r="B46" s="31" t="s">
         <v>162</v>
       </c>
@@ -6024,9 +6024,9 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -6067,10 +6067,10 @@
       <selection activeCell="Q24" sqref="Q24:Q38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="12.69921875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38">
@@ -6155,14 +6155,14 @@
       </c>
       <c r="AB1">
         <f ca="1">RANDBETWEEN(170,185)</f>
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="AC1" t="s">
         <v>120</v>
       </c>
       <c r="AD1">
         <f ca="1">RANDBETWEEN(70,80)</f>
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AE1" t="s">
         <v>120</v>
@@ -6189,7 +6189,7 @@
       </c>
       <c r="AL1" t="str">
         <f ca="1">_xlfn.CONCAT(A1:AK1)</f>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman1@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,172,70,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman1@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,179,71,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="2" spans="1:38">
@@ -6274,14 +6274,14 @@
       </c>
       <c r="AB2">
         <f t="shared" ref="AB2:AB17" ca="1" si="0">RANDBETWEEN(170,185)</f>
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="AC2" t="s">
         <v>120</v>
       </c>
       <c r="AD2">
         <f t="shared" ref="AD2:AD17" ca="1" si="1">RANDBETWEEN(70,80)</f>
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AE2" t="s">
         <v>120</v>
@@ -6308,7 +6308,7 @@
       </c>
       <c r="AL2" t="str">
         <f t="shared" ref="AL2:AL17" ca="1" si="4">_xlfn.CONCAT(A2:AK2)</f>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman2@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,174,79,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman2@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,176,80,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="3" spans="1:38">
@@ -6393,28 +6393,28 @@
       </c>
       <c r="AB3">
         <f t="shared" ca="1" si="0"/>
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="AC3" t="s">
         <v>120</v>
       </c>
       <c r="AD3">
         <f t="shared" ca="1" si="1"/>
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AE3" t="s">
         <v>120</v>
       </c>
       <c r="AF3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG3" t="s">
         <v>120</v>
       </c>
       <c r="AH3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI3" t="s">
         <v>120</v>
@@ -6427,7 +6427,7 @@
       </c>
       <c r="AL3" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman3@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,171,75,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman3@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,181,73,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="4" spans="1:38">
@@ -6512,28 +6512,28 @@
       </c>
       <c r="AB4">
         <f t="shared" ca="1" si="0"/>
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="AC4" t="s">
         <v>120</v>
       </c>
       <c r="AD4">
         <f t="shared" ca="1" si="1"/>
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="AE4" t="s">
         <v>120</v>
       </c>
       <c r="AF4">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG4" t="s">
         <v>120</v>
       </c>
       <c r="AH4">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI4" t="s">
         <v>120</v>
@@ -6546,7 +6546,7 @@
       </c>
       <c r="AL4" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman4@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,181,73,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman4@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,178,75,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="5" spans="1:38">
@@ -6631,14 +6631,14 @@
       </c>
       <c r="AB5">
         <f t="shared" ca="1" si="0"/>
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="AC5" t="s">
         <v>120</v>
       </c>
       <c r="AD5">
         <f t="shared" ca="1" si="1"/>
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AE5" t="s">
         <v>120</v>
@@ -6652,7 +6652,7 @@
       </c>
       <c r="AH5">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI5" t="s">
         <v>120</v>
@@ -6665,7 +6665,7 @@
       </c>
       <c r="AL5" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman5@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,184,79,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman5@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,176,80,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="6" spans="1:38">
@@ -6750,21 +6750,21 @@
       </c>
       <c r="AB6">
         <f t="shared" ca="1" si="0"/>
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="AC6" t="s">
         <v>120</v>
       </c>
       <c r="AD6">
         <f t="shared" ca="1" si="1"/>
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AE6" t="s">
         <v>120</v>
       </c>
       <c r="AF6">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG6" t="s">
         <v>120</v>
@@ -6784,7 +6784,7 @@
       </c>
       <c r="AL6" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman6@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,177,74,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman6@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,172,73,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="7" spans="1:38">
@@ -6869,14 +6869,14 @@
       </c>
       <c r="AB7">
         <f t="shared" ca="1" si="0"/>
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AC7" t="s">
         <v>120</v>
       </c>
       <c r="AD7">
         <f t="shared" ca="1" si="1"/>
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="AE7" t="s">
         <v>120</v>
@@ -6890,7 +6890,7 @@
       </c>
       <c r="AH7">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI7" t="s">
         <v>120</v>
@@ -6903,7 +6903,7 @@
       </c>
       <c r="AL7" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman7@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,173,79,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman7@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,172,76,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="8" spans="1:38">
@@ -6988,7 +6988,7 @@
       </c>
       <c r="AB8">
         <f t="shared" ca="1" si="0"/>
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="AC8" t="s">
         <v>120</v>
@@ -7002,7 +7002,7 @@
       </c>
       <c r="AF8">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG8" t="s">
         <v>120</v>
@@ -7022,7 +7022,7 @@
       </c>
       <c r="AL8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman8@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,174,79,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman8@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,179,79,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="9" spans="1:38">
@@ -7107,28 +7107,28 @@
       </c>
       <c r="AB9">
         <f t="shared" ca="1" si="0"/>
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AC9" t="s">
         <v>120</v>
       </c>
       <c r="AD9">
         <f t="shared" ca="1" si="1"/>
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="AE9" t="s">
         <v>120</v>
       </c>
       <c r="AF9">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG9" t="s">
         <v>120</v>
       </c>
       <c r="AH9">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI9" t="s">
         <v>120</v>
@@ -7141,7 +7141,7 @@
       </c>
       <c r="AL9" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman9@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,174,78,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman9@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,175,71,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="10" spans="1:38">
@@ -7226,14 +7226,14 @@
       </c>
       <c r="AB10">
         <f t="shared" ca="1" si="0"/>
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="AC10" t="s">
         <v>120</v>
       </c>
       <c r="AD10">
         <f t="shared" ca="1" si="1"/>
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="AE10" t="s">
         <v>120</v>
@@ -7247,7 +7247,7 @@
       </c>
       <c r="AH10">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI10" t="s">
         <v>120</v>
@@ -7260,7 +7260,7 @@
       </c>
       <c r="AL10" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman10@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,177,71,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman10@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,181,78,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="11" spans="1:38">
@@ -7345,14 +7345,14 @@
       </c>
       <c r="AB11">
         <f t="shared" ca="1" si="0"/>
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="AC11" t="s">
         <v>120</v>
       </c>
       <c r="AD11">
         <f t="shared" ca="1" si="1"/>
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="AE11" t="s">
         <v>120</v>
@@ -7379,7 +7379,7 @@
       </c>
       <c r="AL11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman11@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,177,73,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman11@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,182,75,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="12" spans="1:38">
@@ -7464,21 +7464,21 @@
       </c>
       <c r="AB12">
         <f t="shared" ca="1" si="0"/>
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AC12" t="s">
         <v>120</v>
       </c>
       <c r="AD12">
         <f t="shared" ca="1" si="1"/>
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="AE12" t="s">
         <v>120</v>
       </c>
       <c r="AF12">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG12" t="s">
         <v>120</v>
@@ -7498,7 +7498,7 @@
       </c>
       <c r="AL12" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman12@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,176,77,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman12@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,179,71,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="13" spans="1:38">
@@ -7583,7 +7583,7 @@
       </c>
       <c r="AB13">
         <f t="shared" ca="1" si="0"/>
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="AC13" t="s">
         <v>120</v>
@@ -7604,7 +7604,7 @@
       </c>
       <c r="AH13">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI13" t="s">
         <v>120</v>
@@ -7617,7 +7617,7 @@
       </c>
       <c r="AL13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman13@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,174,73,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman13@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,176,73,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="14" spans="1:38">
@@ -7702,28 +7702,28 @@
       </c>
       <c r="AB14">
         <f t="shared" ca="1" si="0"/>
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="AC14" t="s">
         <v>120</v>
       </c>
       <c r="AD14">
         <f t="shared" ca="1" si="1"/>
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AE14" t="s">
         <v>120</v>
       </c>
       <c r="AF14">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG14" t="s">
         <v>120</v>
       </c>
       <c r="AH14">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI14" t="s">
         <v>120</v>
@@ -7736,7 +7736,7 @@
       </c>
       <c r="AL14" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman14@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,176,73,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman14@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,185,72,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="15" spans="1:38">
@@ -7821,14 +7821,14 @@
       </c>
       <c r="AB15">
         <f t="shared" ca="1" si="0"/>
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="AC15" t="s">
         <v>120</v>
       </c>
       <c r="AD15">
         <f t="shared" ca="1" si="1"/>
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="AE15" t="s">
         <v>120</v>
@@ -7842,7 +7842,7 @@
       </c>
       <c r="AH15">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI15" t="s">
         <v>120</v>
@@ -7855,7 +7855,7 @@
       </c>
       <c r="AL15" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman15@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,185,78,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman15@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,179,72,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="16" spans="1:38">
@@ -7940,21 +7940,21 @@
       </c>
       <c r="AB16">
         <f t="shared" ca="1" si="0"/>
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="AC16" t="s">
         <v>120</v>
       </c>
       <c r="AD16">
         <f t="shared" ca="1" si="1"/>
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="AE16" t="s">
         <v>120</v>
       </c>
       <c r="AF16">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG16" t="s">
         <v>120</v>
@@ -7974,7 +7974,7 @@
       </c>
       <c r="AL16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman16@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,179,76,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman16@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,171,70,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="17" spans="1:38">
@@ -8059,14 +8059,14 @@
       </c>
       <c r="AB17">
         <f t="shared" ca="1" si="0"/>
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="AC17" t="s">
         <v>120</v>
       </c>
       <c r="AD17">
         <f t="shared" ca="1" si="1"/>
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AE17" t="s">
         <v>120</v>
@@ -8080,7 +8080,7 @@
       </c>
       <c r="AH17">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI17" t="s">
         <v>120</v>
@@ -8093,7 +8093,7 @@
       </c>
       <c r="AL17" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman17@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,171,70,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman17@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,180,71,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="20" spans="1:38">
@@ -8148,7 +8148,7 @@
       </c>
       <c r="Q20">
         <f ca="1">RANDBETWEEN(0,5)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R20" t="s">
         <v>120</v>
@@ -8182,7 +8182,7 @@
       </c>
       <c r="AB20" t="str">
         <f ca="1">_xlfn.CONCAT(A20:AA20)</f>
-        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('왕십리FC','왕십리FC201018.jpg','성동구','성동구 구장','red',3,'2016-01-01',sysdate(),'1234','기업');</v>
+        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('왕십리FC','왕십리FC201018.jpg','성동구','성동구 구장','red',1,'2016-01-01',sysdate(),'1234','기업');</v>
       </c>
     </row>
     <row r="21" spans="1:38">
@@ -8237,7 +8237,7 @@
       </c>
       <c r="Q21">
         <f t="shared" ref="Q21:Q22" ca="1" si="6">RANDBETWEEN(0,5)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R21" t="s">
         <v>120</v>
@@ -8271,7 +8271,7 @@
       </c>
       <c r="AB21" t="str">
         <f t="shared" ref="AB21:AB22" ca="1" si="7">_xlfn.CONCAT(A21:AA21)</f>
-        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('답십리FC','답십리FC201018.jpg','성동구','응봉동 구장','blue',0,'2017-01-01',sysdate(),'5678','하나');</v>
+        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('답십리FC','답십리FC201018.jpg','성동구','응봉동 구장','blue',5,'2017-01-01',sysdate(),'5678','하나');</v>
       </c>
     </row>
     <row r="22" spans="1:38">
@@ -8326,7 +8326,7 @@
       </c>
       <c r="Q22">
         <f t="shared" ca="1" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="R22" t="s">
         <v>120</v>
@@ -8360,7 +8360,7 @@
       </c>
       <c r="AB22" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('대구FC','대구FC201018.jpg','달서구','달서구 구장','green',5,'2018-01-01',sysdate(),'2345','기업');</v>
+        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('대구FC','대구FC201018.jpg','달서구','달서구 구장','green',2,'2018-01-01',sysdate(),'2345','기업');</v>
       </c>
     </row>
     <row r="24" spans="1:38">

</xml_diff>

<commit_message>
[2020-11-03] VoteMatch 명단보기, 지인초청 구현
</commit_message>
<xml_diff>
--- a/docs/srs/fbt_docs.xlsx
+++ b/docs/srs/fbt_docs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Socio_02\Desktop\kjy\fbt\docs\srs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\kjy\fbt\docs\srs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACED58DD-881D-44E3-A0FA-E92EF7F67EBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB471EC-BFAD-4703-B2B9-E9C36362A56A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2F0AD6B2-A8A2-4F73-BAF4-7193D3382EE1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2F0AD6B2-A8A2-4F73-BAF4-7193D3382EE1}"/>
   </bookViews>
   <sheets>
     <sheet name="요구사항명세서" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="TestCase_SQL" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">요구사항명세서!$B$8:$H$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">요구사항명세서!$B$8:$H$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="199">
   <si>
     <t>요구사항 정의서</t>
   </si>
@@ -4380,6 +4380,88 @@
       <t xml:space="preserve"> V003
 투표결과ID 양식 : '투표ID-팀멤버ID or 이메일(지인)'</t>
     </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>카톡공유</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>카페 공유하기(
+- 글 복사
+- 네이버카페</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>테이블</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> --&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>달력</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>V012</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>투표 결과 보기</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>해당 팀의 진행 중인 투표 결과(멤버) 보기</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -4742,7 +4824,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4847,6 +4929,15 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5181,34 +5272,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60EA499F-775F-49C1-B26C-B60E223B5AF8}">
-  <dimension ref="B1:I46"/>
+  <dimension ref="B1:I50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="4.25" customWidth="1"/>
+    <col min="1" max="1" width="4.19921875" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="44" customWidth="1"/>
-    <col min="5" max="5" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.75" customWidth="1"/>
+    <col min="5" max="5" width="15.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.09765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.69921875" customWidth="1"/>
     <col min="8" max="8" width="9.5" customWidth="1"/>
-    <col min="9" max="9" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="17.25" thickBot="1"/>
-    <row r="2" spans="2:9" ht="18.75" thickBot="1">
-      <c r="B2" s="37" t="s">
+    <row r="1" spans="2:9" ht="18" thickBot="1"/>
+    <row r="2" spans="2:9" ht="18" thickBot="1">
+      <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="38"/>
+      <c r="C2" s="41"/>
       <c r="E2" s="3" t="s">
         <v>63</v>
       </c>
@@ -5219,7 +5310,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="17.25" thickBot="1">
+    <row r="3" spans="2:9" ht="18" thickBot="1">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -5234,7 +5325,7 @@
       </c>
       <c r="G3" s="21"/>
     </row>
-    <row r="4" spans="2:9" ht="17.25" thickBot="1">
+    <row r="4" spans="2:9" ht="18" thickBot="1">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -5249,7 +5340,7 @@
       </c>
       <c r="G4" s="21"/>
     </row>
-    <row r="5" spans="2:9" ht="17.25" thickBot="1">
+    <row r="5" spans="2:9" ht="18" thickBot="1">
       <c r="E5" s="25" t="s">
         <v>62</v>
       </c>
@@ -5257,7 +5348,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="17.25" thickBot="1">
+    <row r="6" spans="2:9" ht="18" thickBot="1">
       <c r="E6" s="30" t="s">
         <v>160</v>
       </c>
@@ -5265,46 +5356,46 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="17.25" thickBot="1"/>
-    <row r="8" spans="2:9" ht="17.25" thickBot="1">
-      <c r="B8" s="35" t="s">
+    <row r="7" spans="2:9" ht="18" thickBot="1"/>
+    <row r="8" spans="2:9" ht="18" thickBot="1">
+      <c r="B8" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="39" t="s">
+      <c r="E8" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="40"/>
-      <c r="G8" s="35" t="s">
+      <c r="F8" s="43"/>
+      <c r="G8" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="35" t="s">
+      <c r="H8" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="35" t="s">
+      <c r="I8" s="38" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="17.25" thickBot="1">
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
+    <row r="9" spans="2:9" ht="18" thickBot="1">
+      <c r="B9" s="39"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
       <c r="E9" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
     </row>
-    <row r="10" spans="2:9" ht="26.25" thickBot="1">
+    <row r="10" spans="2:9" ht="27" thickBot="1">
       <c r="B10" s="11" t="s">
         <v>64</v>
       </c>
@@ -5327,7 +5418,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="17.25" thickBot="1">
+    <row r="11" spans="2:9" ht="18" thickBot="1">
       <c r="B11" s="11" t="s">
         <v>65</v>
       </c>
@@ -5348,7 +5439,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="17.25" thickBot="1">
+    <row r="12" spans="2:9" ht="18" thickBot="1">
       <c r="B12" s="11" t="s">
         <v>66</v>
       </c>
@@ -5369,7 +5460,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="27" thickBot="1">
+    <row r="13" spans="2:9" ht="29.4" thickBot="1">
       <c r="B13" s="11" t="s">
         <v>67</v>
       </c>
@@ -5390,7 +5481,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="17.25" thickBot="1">
+    <row r="14" spans="2:9" ht="18" thickBot="1">
       <c r="B14" s="11" t="s">
         <v>68</v>
       </c>
@@ -5411,7 +5502,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="17.25" thickBot="1">
+    <row r="15" spans="2:9" ht="18" thickBot="1">
       <c r="B15" s="11" t="s">
         <v>69</v>
       </c>
@@ -5435,7 +5526,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="17.25" thickBot="1">
+    <row r="16" spans="2:9" ht="18" thickBot="1">
       <c r="B16" s="17" t="s">
         <v>38</v>
       </c>
@@ -5459,7 +5550,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="17.25" thickBot="1">
+    <row r="17" spans="2:9" ht="18" thickBot="1">
       <c r="B17" s="17" t="s">
         <v>170</v>
       </c>
@@ -5481,7 +5572,7 @@
       </c>
       <c r="I17" s="32"/>
     </row>
-    <row r="18" spans="2:9" ht="40.5" thickBot="1">
+    <row r="18" spans="2:9" ht="45" thickBot="1">
       <c r="B18" s="17" t="s">
         <v>39</v>
       </c>
@@ -5505,7 +5596,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="120.75" thickBot="1">
+    <row r="19" spans="2:9" ht="136.19999999999999" thickBot="1">
       <c r="B19" s="17" t="s">
         <v>40</v>
       </c>
@@ -5529,7 +5620,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="81" thickBot="1">
+    <row r="20" spans="2:9" ht="91.8" thickBot="1">
       <c r="B20" s="17" t="s">
         <v>42</v>
       </c>
@@ -5553,7 +5644,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="291.75" thickBot="1">
+    <row r="21" spans="2:9" ht="324.60000000000002" thickBot="1">
       <c r="B21" s="17" t="s">
         <v>46</v>
       </c>
@@ -5574,7 +5665,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="26.25" thickBot="1">
+    <row r="22" spans="2:9" ht="27" thickBot="1">
       <c r="B22" s="19" t="s">
         <v>47</v>
       </c>
@@ -5600,7 +5691,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="27" thickBot="1">
+    <row r="23" spans="2:9" ht="29.4" thickBot="1">
       <c r="B23" s="34" t="s">
         <v>175</v>
       </c>
@@ -5620,7 +5711,7 @@
       <c r="H23" s="12"/>
       <c r="I23" s="33"/>
     </row>
-    <row r="24" spans="2:9" ht="17.25" thickBot="1">
+    <row r="24" spans="2:9" ht="18" thickBot="1">
       <c r="B24" s="34" t="s">
         <v>177</v>
       </c>
@@ -5640,7 +5731,7 @@
       <c r="H24" s="12"/>
       <c r="I24" s="33"/>
     </row>
-    <row r="25" spans="2:9" ht="27" thickBot="1">
+    <row r="25" spans="2:9" ht="29.4" thickBot="1">
       <c r="B25" s="34" t="s">
         <v>179</v>
       </c>
@@ -5660,7 +5751,7 @@
       <c r="H25" s="12"/>
       <c r="I25" s="33"/>
     </row>
-    <row r="26" spans="2:9" ht="17.25" thickBot="1">
+    <row r="26" spans="2:9" ht="18" thickBot="1">
       <c r="B26" s="34" t="s">
         <v>186</v>
       </c>
@@ -5678,36 +5769,33 @@
       <c r="H26" s="12"/>
       <c r="I26" s="33"/>
     </row>
-    <row r="27" spans="2:9" ht="17.25" thickBot="1">
-      <c r="B27" s="20" t="s">
+    <row r="27" spans="2:9" ht="18" thickBot="1">
+      <c r="B27" s="34" t="s">
+        <v>196</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" s="15"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="33"/>
+    </row>
+    <row r="28" spans="2:9" ht="18" thickBot="1">
+      <c r="B28" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C28" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D28" s="13" t="s">
         <v>52</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H27" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" ht="17.25" thickBot="1">
-      <c r="B28" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>54</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>44</v>
@@ -5717,60 +5805,60 @@
         <v>16</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
     </row>
-    <row r="29" spans="2:9" ht="26.25" thickBot="1">
+    <row r="29" spans="2:9" ht="18" thickBot="1">
       <c r="B29" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>55</v>
+        <v>26</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>53</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>44</v>
       </c>
       <c r="F29" s="12"/>
       <c r="G29" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H29" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="H29" s="12" t="s">
-        <v>45</v>
-      </c>
     </row>
-    <row r="30" spans="2:9" ht="17.25" thickBot="1">
+    <row r="30" spans="2:9" ht="27" thickBot="1">
       <c r="B30" s="20" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>44</v>
       </c>
       <c r="F30" s="12"/>
       <c r="G30" s="12" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
     </row>
-    <row r="31" spans="2:9" ht="17.25" thickBot="1">
+    <row r="31" spans="2:9" ht="18" thickBot="1">
       <c r="B31" s="20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>44</v>
@@ -5780,104 +5868,104 @@
         <v>16</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="32" spans="2:9" ht="80.25" thickBot="1">
+    <row r="32" spans="2:9" ht="18" thickBot="1">
       <c r="B32" s="20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D32" s="18" t="s">
-        <v>81</v>
+        <v>73</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>44</v>
       </c>
       <c r="F32" s="12"/>
       <c r="G32" s="12" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="H32" s="12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="17.25" thickBot="1">
+    <row r="33" spans="2:8" ht="91.8" thickBot="1">
       <c r="B33" s="20" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E33" s="12" t="s">
         <v>44</v>
       </c>
       <c r="F33" s="12"/>
       <c r="G33" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H33" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H33" s="12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="27.75" thickBot="1">
+    <row r="34" spans="2:8" ht="18" thickBot="1">
       <c r="B34" s="20" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="E34" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E34" s="12" t="s">
         <v>44</v>
       </c>
       <c r="F34" s="12"/>
       <c r="G34" s="12" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="H34" s="15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="17.25" thickBot="1">
-      <c r="B35" s="22" t="s">
-        <v>70</v>
+    <row r="35" spans="2:8" ht="31.8" thickBot="1">
+      <c r="B35" s="20" t="s">
+        <v>79</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="D35" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>24</v>
+        <v>80</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>44</v>
       </c>
       <c r="F35" s="12"/>
       <c r="G35" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H35" s="12" t="s">
-        <v>16</v>
+        <v>25</v>
+      </c>
+      <c r="H35" s="15" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="17.25" thickBot="1">
+    <row r="36" spans="2:8" ht="18" thickBot="1">
       <c r="B36" s="22" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="E36" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E36" s="12" t="s">
         <v>24</v>
       </c>
       <c r="F36" s="12"/>
@@ -5885,83 +5973,83 @@
         <v>16</v>
       </c>
       <c r="H36" s="12" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="17.25" thickBot="1">
+    <row r="37" spans="2:8" ht="18" thickBot="1">
       <c r="B37" s="22" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="F37" s="12"/>
       <c r="G37" s="12" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="H37" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="17.25" thickBot="1">
+    <row r="38" spans="2:8" ht="18" thickBot="1">
       <c r="B38" s="22" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="F38" s="12"/>
       <c r="G38" s="12" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H38" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="17.25" thickBot="1">
+    <row r="39" spans="2:8" ht="18" thickBot="1">
       <c r="B39" s="22" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="F39" s="12"/>
       <c r="G39" s="12" t="s">
         <v>16</v>
       </c>
       <c r="H39" s="12" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="17.25" thickBot="1">
-      <c r="B40" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="C40" s="16" t="s">
-        <v>100</v>
+    <row r="40" spans="2:8" ht="18" thickBot="1">
+      <c r="B40" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>95</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="E40" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="E40" s="15" t="s">
         <v>44</v>
       </c>
       <c r="F40" s="12"/>
@@ -5969,18 +6057,18 @@
         <v>16</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="17.25" thickBot="1">
+    <row r="41" spans="2:8" ht="18" thickBot="1">
       <c r="B41" s="29" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="D41" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>98</v>
       </c>
       <c r="E41" s="12" t="s">
         <v>44</v>
@@ -5993,15 +6081,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="2:8" ht="17.25" thickBot="1">
+    <row r="42" spans="2:8" ht="18" thickBot="1">
       <c r="B42" s="29" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E42" s="12" t="s">
         <v>44</v>
@@ -6014,15 +6102,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="17.25" thickBot="1">
+    <row r="43" spans="2:8" ht="18" thickBot="1">
       <c r="B43" s="29" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E43" s="12" t="s">
         <v>44</v>
@@ -6032,18 +6120,18 @@
         <v>16</v>
       </c>
       <c r="H43" s="12" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="44" spans="2:8" ht="17.25" thickBot="1">
+    <row r="44" spans="2:8" ht="18" thickBot="1">
       <c r="B44" s="29" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E44" s="12" t="s">
         <v>44</v>
@@ -6053,17 +6141,19 @@
         <v>16</v>
       </c>
       <c r="H44" s="12" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="45" spans="2:8" ht="17.25" thickBot="1">
+    <row r="45" spans="2:8" ht="18" thickBot="1">
       <c r="B45" s="29" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="D45" s="18"/>
+        <v>110</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>111</v>
+      </c>
       <c r="E45" s="12" t="s">
         <v>44</v>
       </c>
@@ -6071,18 +6161,18 @@
       <c r="G45" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="H45" s="12"/>
+      <c r="H45" s="12" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="46" spans="2:8" ht="27.75" thickBot="1">
-      <c r="B46" s="31" t="s">
-        <v>161</v>
+    <row r="46" spans="2:8" ht="18" thickBot="1">
+      <c r="B46" s="29" t="s">
+        <v>112</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="D46" s="18" t="s">
-        <v>165</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="D46" s="18"/>
       <c r="E46" s="12" t="s">
         <v>44</v>
       </c>
@@ -6090,12 +6180,46 @@
       <c r="G46" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="H46" s="12" t="s">
+      <c r="H46" s="12"/>
+    </row>
+    <row r="47" spans="2:8" ht="31.8" thickBot="1">
+      <c r="B47" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H47" s="12" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8">
+      <c r="D48" s="35" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" ht="52.2">
+      <c r="D49" s="36" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4">
+      <c r="D50" s="37" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B8:H46" xr:uid="{08681459-A406-4CEE-9A8A-D3DF83B63176}">
+  <autoFilter ref="B8:H47" xr:uid="{08681459-A406-4CEE-9A8A-D3DF83B63176}">
     <filterColumn colId="3" showButton="0"/>
   </autoFilter>
   <mergeCells count="8">
@@ -6122,9 +6246,9 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -6165,10 +6289,10 @@
       <selection activeCell="Q24" sqref="Q24:Q38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38">
@@ -6253,21 +6377,21 @@
       </c>
       <c r="AB1">
         <f ca="1">RANDBETWEEN(170,185)</f>
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="AC1" t="s">
         <v>119</v>
       </c>
       <c r="AD1">
         <f ca="1">RANDBETWEEN(70,80)</f>
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="AE1" t="s">
         <v>119</v>
       </c>
       <c r="AF1">
         <f ca="1">RANDBETWEEN(0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG1" t="s">
         <v>119</v>
@@ -6287,7 +6411,7 @@
       </c>
       <c r="AL1" t="str">
         <f ca="1">_xlfn.CONCAT(A1:AK1)</f>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman1@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,178,77,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman1@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,181,80,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="2" spans="1:38">
@@ -6372,28 +6496,28 @@
       </c>
       <c r="AB2">
         <f t="shared" ref="AB2:AB17" ca="1" si="0">RANDBETWEEN(170,185)</f>
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="AC2" t="s">
         <v>119</v>
       </c>
       <c r="AD2">
         <f t="shared" ref="AD2:AD17" ca="1" si="1">RANDBETWEEN(70,80)</f>
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="AE2" t="s">
         <v>119</v>
       </c>
       <c r="AF2">
         <f t="shared" ref="AF2:AF17" ca="1" si="2">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG2" t="s">
         <v>119</v>
       </c>
       <c r="AH2">
         <f t="shared" ref="AH2:AH17" ca="1" si="3">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI2" t="s">
         <v>119</v>
@@ -6406,7 +6530,7 @@
       </c>
       <c r="AL2" t="str">
         <f t="shared" ref="AL2:AL17" ca="1" si="4">_xlfn.CONCAT(A2:AK2)</f>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman2@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,177,76,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman2@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,182,79,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="3" spans="1:38">
@@ -6491,21 +6615,21 @@
       </c>
       <c r="AB3">
         <f t="shared" ca="1" si="0"/>
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="AC3" t="s">
         <v>119</v>
       </c>
       <c r="AD3">
         <f t="shared" ca="1" si="1"/>
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AE3" t="s">
         <v>119</v>
       </c>
       <c r="AF3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG3" t="s">
         <v>119</v>
@@ -6525,7 +6649,7 @@
       </c>
       <c r="AL3" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman3@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,177,71,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman3@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,183,72,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="4" spans="1:38">
@@ -6610,28 +6734,28 @@
       </c>
       <c r="AB4">
         <f t="shared" ca="1" si="0"/>
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="AC4" t="s">
         <v>119</v>
       </c>
       <c r="AD4">
         <f t="shared" ca="1" si="1"/>
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="AE4" t="s">
         <v>119</v>
       </c>
       <c r="AF4">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG4" t="s">
         <v>119</v>
       </c>
       <c r="AH4">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI4" t="s">
         <v>119</v>
@@ -6644,7 +6768,7 @@
       </c>
       <c r="AL4" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman4@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,172,76,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman4@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,179,70,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="5" spans="1:38">
@@ -6729,14 +6853,14 @@
       </c>
       <c r="AB5">
         <f t="shared" ca="1" si="0"/>
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AC5" t="s">
         <v>119</v>
       </c>
       <c r="AD5">
         <f t="shared" ca="1" si="1"/>
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AE5" t="s">
         <v>119</v>
@@ -6750,7 +6874,7 @@
       </c>
       <c r="AH5">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI5" t="s">
         <v>119</v>
@@ -6763,7 +6887,7 @@
       </c>
       <c r="AL5" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman5@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,181,73,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman5@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,180,72,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="6" spans="1:38">
@@ -6848,21 +6972,21 @@
       </c>
       <c r="AB6">
         <f t="shared" ca="1" si="0"/>
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="AC6" t="s">
         <v>119</v>
       </c>
       <c r="AD6">
         <f t="shared" ca="1" si="1"/>
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="AE6" t="s">
         <v>119</v>
       </c>
       <c r="AF6">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG6" t="s">
         <v>119</v>
@@ -6882,7 +7006,7 @@
       </c>
       <c r="AL6" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman6@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,178,73,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman6@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,174,80,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="7" spans="1:38">
@@ -6967,14 +7091,14 @@
       </c>
       <c r="AB7">
         <f t="shared" ca="1" si="0"/>
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AC7" t="s">
         <v>119</v>
       </c>
       <c r="AD7">
         <f t="shared" ca="1" si="1"/>
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="AE7" t="s">
         <v>119</v>
@@ -7001,7 +7125,7 @@
       </c>
       <c r="AL7" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman7@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,184,76,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman7@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,185,73,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="8" spans="1:38">
@@ -7086,14 +7210,14 @@
       </c>
       <c r="AB8">
         <f t="shared" ca="1" si="0"/>
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="AC8" t="s">
         <v>119</v>
       </c>
       <c r="AD8">
         <f t="shared" ca="1" si="1"/>
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="AE8" t="s">
         <v>119</v>
@@ -7107,7 +7231,7 @@
       </c>
       <c r="AH8">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI8" t="s">
         <v>119</v>
@@ -7120,7 +7244,7 @@
       </c>
       <c r="AL8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman8@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,173,76,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman8@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,177,71,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="9" spans="1:38">
@@ -7205,28 +7329,28 @@
       </c>
       <c r="AB9">
         <f t="shared" ca="1" si="0"/>
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AC9" t="s">
         <v>119</v>
       </c>
       <c r="AD9">
         <f t="shared" ca="1" si="1"/>
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="AE9" t="s">
         <v>119</v>
       </c>
       <c r="AF9">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG9" t="s">
         <v>119</v>
       </c>
       <c r="AH9">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI9" t="s">
         <v>119</v>
@@ -7239,7 +7363,7 @@
       </c>
       <c r="AL9" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman9@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,181,70,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman9@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,180,78,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="10" spans="1:38">
@@ -7331,14 +7455,14 @@
       </c>
       <c r="AD10">
         <f t="shared" ca="1" si="1"/>
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="AE10" t="s">
         <v>119</v>
       </c>
       <c r="AF10">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG10" t="s">
         <v>119</v>
@@ -7358,7 +7482,7 @@
       </c>
       <c r="AL10" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman10@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,183,70,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman10@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,183,72,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="11" spans="1:38">
@@ -7443,21 +7567,21 @@
       </c>
       <c r="AB11">
         <f t="shared" ca="1" si="0"/>
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="AC11" t="s">
         <v>119</v>
       </c>
       <c r="AD11">
         <f t="shared" ca="1" si="1"/>
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AE11" t="s">
         <v>119</v>
       </c>
       <c r="AF11">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG11" t="s">
         <v>119</v>
@@ -7477,7 +7601,7 @@
       </c>
       <c r="AL11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman11@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,182,72,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman11@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,175,73,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="12" spans="1:38">
@@ -7562,14 +7686,14 @@
       </c>
       <c r="AB12">
         <f t="shared" ca="1" si="0"/>
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="AC12" t="s">
         <v>119</v>
       </c>
       <c r="AD12">
         <f t="shared" ca="1" si="1"/>
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AE12" t="s">
         <v>119</v>
@@ -7596,7 +7720,7 @@
       </c>
       <c r="AL12" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman12@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,181,74,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman12@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,183,72,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="13" spans="1:38">
@@ -7681,21 +7805,21 @@
       </c>
       <c r="AB13">
         <f t="shared" ca="1" si="0"/>
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="AC13" t="s">
         <v>119</v>
       </c>
       <c r="AD13">
         <f t="shared" ca="1" si="1"/>
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="AE13" t="s">
         <v>119</v>
       </c>
       <c r="AF13">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG13" t="s">
         <v>119</v>
@@ -7715,7 +7839,7 @@
       </c>
       <c r="AL13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman13@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,184,73,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman13@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,170,80,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="14" spans="1:38">
@@ -7800,7 +7924,7 @@
       </c>
       <c r="AB14">
         <f t="shared" ca="1" si="0"/>
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="AC14" t="s">
         <v>119</v>
@@ -7834,7 +7958,7 @@
       </c>
       <c r="AL14" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman14@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,174,75,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman14@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,178,75,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="15" spans="1:38">
@@ -7919,7 +8043,7 @@
       </c>
       <c r="AB15">
         <f t="shared" ca="1" si="0"/>
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AC15" t="s">
         <v>119</v>
@@ -7940,7 +8064,7 @@
       </c>
       <c r="AH15">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI15" t="s">
         <v>119</v>
@@ -7953,7 +8077,7 @@
       </c>
       <c r="AL15" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman15@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,170,76,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman15@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,171,76,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="16" spans="1:38">
@@ -8038,14 +8162,14 @@
       </c>
       <c r="AB16">
         <f t="shared" ca="1" si="0"/>
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="AC16" t="s">
         <v>119</v>
       </c>
       <c r="AD16">
         <f t="shared" ca="1" si="1"/>
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="AE16" t="s">
         <v>119</v>
@@ -8059,7 +8183,7 @@
       </c>
       <c r="AH16">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI16" t="s">
         <v>119</v>
@@ -8072,7 +8196,7 @@
       </c>
       <c r="AL16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman16@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,173,76,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman16@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,171,79,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="17" spans="1:38">
@@ -8157,28 +8281,28 @@
       </c>
       <c r="AB17">
         <f t="shared" ca="1" si="0"/>
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="AC17" t="s">
         <v>119</v>
       </c>
       <c r="AD17">
         <f t="shared" ca="1" si="1"/>
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="AE17" t="s">
         <v>119</v>
       </c>
       <c r="AF17">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG17" t="s">
         <v>119</v>
       </c>
       <c r="AH17">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI17" t="s">
         <v>119</v>
@@ -8191,7 +8315,7 @@
       </c>
       <c r="AL17" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman17@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,172,74,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman17@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,183,78,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="20" spans="1:38">
@@ -8246,7 +8370,7 @@
       </c>
       <c r="Q20">
         <f ca="1">RANDBETWEEN(0,5)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R20" t="s">
         <v>119</v>
@@ -8280,7 +8404,7 @@
       </c>
       <c r="AB20" t="str">
         <f ca="1">_xlfn.CONCAT(A20:AA20)</f>
-        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('왕십리FC','왕십리FC201018.jpg','성동구','성동구 구장','red',1,'2016-01-01',sysdate(),'1234','기업');</v>
+        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('왕십리FC','왕십리FC201018.jpg','성동구','성동구 구장','red',4,'2016-01-01',sysdate(),'1234','기업');</v>
       </c>
     </row>
     <row r="21" spans="1:38">
@@ -8424,7 +8548,7 @@
       </c>
       <c r="Q22">
         <f t="shared" ca="1" si="6"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R22" t="s">
         <v>119</v>
@@ -8458,7 +8582,7 @@
       </c>
       <c r="AB22" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('대구FC','대구FC201018.jpg','달서구','달서구 구장','green',4,'2018-01-01',sysdate(),'2345','기업');</v>
+        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('대구FC','대구FC201018.jpg','달서구','달서구 구장','green',2,'2018-01-01',sysdate(),'2345','기업');</v>
       </c>
     </row>
     <row r="24" spans="1:38">

</xml_diff>

<commit_message>
[2020-11-05 10:31] VoteMatch 개인 기능, View 다 구현
</commit_message>
<xml_diff>
--- a/docs/srs/fbt_docs.xlsx
+++ b/docs/srs/fbt_docs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\kjy\fbt\docs\srs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB471EC-BFAD-4703-B2B9-E9C36362A56A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177BA833-D5E4-464A-A4ED-8BC24839C6CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2F0AD6B2-A8A2-4F73-BAF4-7193D3382EE1}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="TestCase_SQL" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">요구사항명세서!$B$8:$H$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">요구사항명세서!$B$8:$H$48</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="202">
   <si>
     <t>요구사항 정의서</t>
   </si>
@@ -2347,435 +2347,6 @@
         <charset val="129"/>
       </rPr>
       <t>수정</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>해당</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>지인에게</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>초대</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>보내기(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nanum Gothic"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">invite)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>투표하면</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 1 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>안</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>하면</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>아예</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>넣지</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>않기(투표 취소)
-추후</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>채팅으로</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>변환</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>생각</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">중
-경기 관련 글은 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nanum Gothic"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">match_schedule </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>참조</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nanum Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>알람</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>화면</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>단에서</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>투표</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">?
-- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nanum Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>insert</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nanum Gothic"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>를 진행하나 에러 뜨면 기투표 여부 확인 후 기투표 시, 이미 투표했다고 알림 아니면 에러 페이지</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Nanum Gothic"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">
-V003</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>으로</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>연결
-마이페이지에서 투표 취소</t>
     </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -4462,6 +4033,820 @@
   </si>
   <si>
     <t>해당 팀의 진행 중인 투표 결과(멤버) 보기</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>V013</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>지인 찾기</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>지인 찾기(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">V013) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>후</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+해당</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>지인에게</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>초대</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>보내기(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">invite)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>투표하면</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>안</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>하면</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>아예</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>넣지</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>않기(투표 취소)
+추후</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>채팅으로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>변환</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>생각</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">중
+경기 관련 글은 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">match_schedule </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>참조</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>알람</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>화면</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>단에서</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>투표</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">?
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>insert</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>진행하나</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>에러</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>뜨면</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>기투표</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>여부</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>확인</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>후</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>기투표</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>시</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>이미</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>투표했다고</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>알림</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>아니면</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>에러</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>페이지</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+V003</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>으로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>연결
+마이페이지에서 투표 취소</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>초대할</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>지인</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>찾기</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+- 해당 팀 제외한 user 중</t>
+    </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -4469,7 +4854,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4605,13 +4990,6 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Nanum Gothic"/>
-      <family val="2"/>
-      <charset val="129"/>
     </font>
   </fonts>
   <fills count="14">
@@ -5272,13 +5650,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60EA499F-775F-49C1-B26C-B60E223B5AF8}">
-  <dimension ref="B1:I50"/>
+  <dimension ref="B1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomRight" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -5468,7 +5846,7 @@
         <v>32</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>30</v>
@@ -5531,7 +5909,7 @@
         <v>38</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>85</v>
@@ -5555,7 +5933,7 @@
         <v>170</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>171</v>
@@ -5577,10 +5955,10 @@
         <v>39</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>30</v>
@@ -5596,7 +5974,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="136.19999999999999" thickBot="1">
+    <row r="19" spans="2:9" ht="156.6" thickBot="1">
       <c r="B19" s="17" t="s">
         <v>40</v>
       </c>
@@ -5604,7 +5982,7 @@
         <v>41</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>172</v>
+        <v>200</v>
       </c>
       <c r="E19" s="12" t="s">
         <v>30</v>
@@ -5628,7 +6006,7 @@
         <v>43</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>44</v>
@@ -5652,7 +6030,7 @@
         <v>166</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>44</v>
@@ -5693,19 +6071,19 @@
     </row>
     <row r="23" spans="2:9" ht="29.4" thickBot="1">
       <c r="B23" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="C23" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>176</v>
-      </c>
       <c r="D23" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E23" s="12" t="s">
         <v>44</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
@@ -5713,19 +6091,19 @@
     </row>
     <row r="24" spans="2:9" ht="18" thickBot="1">
       <c r="B24" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C24" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>178</v>
-      </c>
       <c r="D24" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>44</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
@@ -5733,19 +6111,19 @@
     </row>
     <row r="25" spans="2:9" ht="29.4" thickBot="1">
       <c r="B25" s="34" t="s">
+        <v>178</v>
+      </c>
+      <c r="C25" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>180</v>
-      </c>
       <c r="D25" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>44</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G25" s="12"/>
       <c r="H25" s="12"/>
@@ -5753,13 +6131,13 @@
     </row>
     <row r="26" spans="2:9" ht="18" thickBot="1">
       <c r="B26" s="34" t="s">
+        <v>185</v>
+      </c>
+      <c r="C26" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="D26" s="18" t="s">
         <v>187</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>188</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>30</v>
@@ -5771,13 +6149,13 @@
     </row>
     <row r="27" spans="2:9" ht="18" thickBot="1">
       <c r="B27" s="34" t="s">
+        <v>195</v>
+      </c>
+      <c r="C27" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="D27" s="18" t="s">
         <v>197</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>198</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>30</v>
@@ -5787,36 +6165,33 @@
       <c r="H27" s="12"/>
       <c r="I27" s="33"/>
     </row>
-    <row r="28" spans="2:9" ht="18" thickBot="1">
-      <c r="B28" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>52</v>
+    <row r="28" spans="2:9" ht="29.4" thickBot="1">
+      <c r="B28" s="34" t="s">
+        <v>198</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>201</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H28" s="12" t="s">
-        <v>45</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F28" s="15"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="33"/>
     </row>
     <row r="29" spans="2:9" ht="18" thickBot="1">
       <c r="B29" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>51</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>44</v>
@@ -5826,60 +6201,60 @@
         <v>16</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
     </row>
-    <row r="30" spans="2:9" ht="27" thickBot="1">
+    <row r="30" spans="2:9" ht="18" thickBot="1">
       <c r="B30" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>55</v>
+        <v>26</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>53</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>44</v>
       </c>
       <c r="F30" s="12"/>
       <c r="G30" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="H30" s="12" t="s">
-        <v>45</v>
-      </c>
     </row>
-    <row r="31" spans="2:9" ht="18" thickBot="1">
+    <row r="31" spans="2:9" ht="27" thickBot="1">
       <c r="B31" s="20" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>44</v>
       </c>
       <c r="F31" s="12"/>
       <c r="G31" s="12" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="2:9" ht="18" thickBot="1">
       <c r="B32" s="20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>44</v>
@@ -5889,104 +6264,104 @@
         <v>16</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="91.8" thickBot="1">
+    <row r="33" spans="2:8" ht="18" thickBot="1">
       <c r="B33" s="20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D33" s="18" t="s">
-        <v>81</v>
+        <v>73</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="E33" s="12" t="s">
         <v>44</v>
       </c>
       <c r="F33" s="12"/>
       <c r="G33" s="12" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="H33" s="12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="18" thickBot="1">
+    <row r="34" spans="2:8" ht="91.8" thickBot="1">
       <c r="B34" s="20" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E34" s="12" t="s">
         <v>44</v>
       </c>
       <c r="F34" s="12"/>
       <c r="G34" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H34" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H34" s="12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="31.8" thickBot="1">
+    <row r="35" spans="2:8" ht="18" thickBot="1">
       <c r="B35" s="20" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="E35" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E35" s="12" t="s">
         <v>44</v>
       </c>
       <c r="F35" s="12"/>
       <c r="G35" s="12" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="H35" s="15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="18" thickBot="1">
-      <c r="B36" s="22" t="s">
-        <v>70</v>
+    <row r="36" spans="2:8" ht="31.8" thickBot="1">
+      <c r="B36" s="20" t="s">
+        <v>79</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>24</v>
+        <v>80</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>44</v>
       </c>
       <c r="F36" s="12"/>
       <c r="G36" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H36" s="12" t="s">
-        <v>16</v>
+        <v>25</v>
+      </c>
+      <c r="H36" s="15" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="2:8" ht="18" thickBot="1">
       <c r="B37" s="22" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="E37" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E37" s="12" t="s">
         <v>24</v>
       </c>
       <c r="F37" s="12"/>
@@ -5994,25 +6369,25 @@
         <v>16</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="18" thickBot="1">
       <c r="B38" s="22" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="F38" s="12"/>
       <c r="G38" s="12" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="H38" s="12" t="s">
         <v>25</v>
@@ -6020,20 +6395,20 @@
     </row>
     <row r="39" spans="2:8" ht="18" thickBot="1">
       <c r="B39" s="22" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="F39" s="12"/>
       <c r="G39" s="12" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H39" s="12" t="s">
         <v>25</v>
@@ -6041,36 +6416,36 @@
     </row>
     <row r="40" spans="2:8" ht="18" thickBot="1">
       <c r="B40" s="22" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="F40" s="12"/>
       <c r="G40" s="12" t="s">
         <v>16</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="41" spans="2:8" ht="18" thickBot="1">
-      <c r="B41" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>100</v>
+      <c r="B41" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>95</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="E41" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="E41" s="15" t="s">
         <v>44</v>
       </c>
       <c r="F41" s="12"/>
@@ -6078,18 +6453,18 @@
         <v>16</v>
       </c>
       <c r="H41" s="12" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="2:8" ht="18" thickBot="1">
       <c r="B42" s="29" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="D42" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>98</v>
       </c>
       <c r="E42" s="12" t="s">
         <v>44</v>
@@ -6104,13 +6479,13 @@
     </row>
     <row r="43" spans="2:8" ht="18" thickBot="1">
       <c r="B43" s="29" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E43" s="12" t="s">
         <v>44</v>
@@ -6125,13 +6500,13 @@
     </row>
     <row r="44" spans="2:8" ht="18" thickBot="1">
       <c r="B44" s="29" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E44" s="12" t="s">
         <v>44</v>
@@ -6141,18 +6516,18 @@
         <v>16</v>
       </c>
       <c r="H44" s="12" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="2:8" ht="18" thickBot="1">
       <c r="B45" s="29" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E45" s="12" t="s">
         <v>44</v>
@@ -6162,17 +6537,19 @@
         <v>16</v>
       </c>
       <c r="H45" s="12" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="2:8" ht="18" thickBot="1">
       <c r="B46" s="29" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="D46" s="18"/>
+        <v>110</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>111</v>
+      </c>
       <c r="E46" s="12" t="s">
         <v>44</v>
       </c>
@@ -6180,18 +6557,18 @@
       <c r="G46" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="H46" s="12"/>
+      <c r="H46" s="12" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="47" spans="2:8" ht="31.8" thickBot="1">
-      <c r="B47" s="31" t="s">
-        <v>161</v>
+    <row r="47" spans="2:8" ht="18" thickBot="1">
+      <c r="B47" s="29" t="s">
+        <v>112</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="D47" s="18" t="s">
-        <v>165</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="D47" s="18"/>
       <c r="E47" s="12" t="s">
         <v>44</v>
       </c>
@@ -6199,27 +6576,46 @@
       <c r="G47" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="H47" s="12" t="s">
+      <c r="H47" s="12"/>
+    </row>
+    <row r="48" spans="2:8" ht="31.8" thickBot="1">
+      <c r="B48" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H48" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="2:8">
-      <c r="D48" s="35" t="s">
+    <row r="49" spans="4:4">
+      <c r="D49" s="35" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" ht="52.2">
+      <c r="D50" s="36" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="49" spans="4:4" ht="52.2">
-      <c r="D49" s="36" t="s">
+    <row r="51" spans="4:4">
+      <c r="D51" s="37" t="s">
         <v>194</v>
-      </c>
-    </row>
-    <row r="50" spans="4:4">
-      <c r="D50" s="37" t="s">
-        <v>195</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B8:H47" xr:uid="{08681459-A406-4CEE-9A8A-D3DF83B63176}">
+  <autoFilter ref="B8:H48" xr:uid="{08681459-A406-4CEE-9A8A-D3DF83B63176}">
     <filterColumn colId="3" showButton="0"/>
   </autoFilter>
   <mergeCells count="8">
@@ -6377,21 +6773,21 @@
       </c>
       <c r="AB1">
         <f ca="1">RANDBETWEEN(170,185)</f>
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="AC1" t="s">
         <v>119</v>
       </c>
       <c r="AD1">
         <f ca="1">RANDBETWEEN(70,80)</f>
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="AE1" t="s">
         <v>119</v>
       </c>
       <c r="AF1">
         <f ca="1">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG1" t="s">
         <v>119</v>
@@ -6411,7 +6807,7 @@
       </c>
       <c r="AL1" t="str">
         <f ca="1">_xlfn.CONCAT(A1:AK1)</f>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman1@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,181,80,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman1@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,177,73,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="2" spans="1:38">
@@ -6496,7 +6892,7 @@
       </c>
       <c r="AB2">
         <f t="shared" ref="AB2:AB17" ca="1" si="0">RANDBETWEEN(170,185)</f>
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="AC2" t="s">
         <v>119</v>
@@ -6510,14 +6906,14 @@
       </c>
       <c r="AF2">
         <f t="shared" ref="AF2:AF17" ca="1" si="2">RANDBETWEEN(0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG2" t="s">
         <v>119</v>
       </c>
       <c r="AH2">
         <f t="shared" ref="AH2:AH17" ca="1" si="3">RANDBETWEEN(0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI2" t="s">
         <v>119</v>
@@ -6530,7 +6926,7 @@
       </c>
       <c r="AL2" t="str">
         <f t="shared" ref="AL2:AL17" ca="1" si="4">_xlfn.CONCAT(A2:AK2)</f>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman2@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,182,79,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman2@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,180,79,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="3" spans="1:38">
@@ -6615,28 +7011,28 @@
       </c>
       <c r="AB3">
         <f t="shared" ca="1" si="0"/>
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="AC3" t="s">
         <v>119</v>
       </c>
       <c r="AD3">
         <f t="shared" ca="1" si="1"/>
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="AE3" t="s">
         <v>119</v>
       </c>
       <c r="AF3">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG3" t="s">
         <v>119</v>
       </c>
       <c r="AH3">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI3" t="s">
         <v>119</v>
@@ -6649,7 +7045,7 @@
       </c>
       <c r="AL3" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman3@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,183,72,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman3@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,171,80,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="4" spans="1:38">
@@ -6734,21 +7130,21 @@
       </c>
       <c r="AB4">
         <f t="shared" ca="1" si="0"/>
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="AC4" t="s">
         <v>119</v>
       </c>
       <c r="AD4">
         <f t="shared" ca="1" si="1"/>
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="AE4" t="s">
         <v>119</v>
       </c>
       <c r="AF4">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG4" t="s">
         <v>119</v>
@@ -6768,7 +7164,7 @@
       </c>
       <c r="AL4" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman4@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,179,70,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman4@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,172,73,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="5" spans="1:38">
@@ -6853,14 +7249,14 @@
       </c>
       <c r="AB5">
         <f t="shared" ca="1" si="0"/>
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="AC5" t="s">
         <v>119</v>
       </c>
       <c r="AD5">
         <f t="shared" ca="1" si="1"/>
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="AE5" t="s">
         <v>119</v>
@@ -6874,7 +7270,7 @@
       </c>
       <c r="AH5">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI5" t="s">
         <v>119</v>
@@ -6887,7 +7283,7 @@
       </c>
       <c r="AL5" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman5@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,180,72,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman5@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,173,80,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="6" spans="1:38">
@@ -6972,14 +7368,14 @@
       </c>
       <c r="AB6">
         <f t="shared" ca="1" si="0"/>
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="AC6" t="s">
         <v>119</v>
       </c>
       <c r="AD6">
         <f t="shared" ca="1" si="1"/>
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="AE6" t="s">
         <v>119</v>
@@ -6993,7 +7389,7 @@
       </c>
       <c r="AH6">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI6" t="s">
         <v>119</v>
@@ -7006,7 +7402,7 @@
       </c>
       <c r="AL6" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman6@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,174,80,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman6@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,185,76,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="7" spans="1:38">
@@ -7091,14 +7487,14 @@
       </c>
       <c r="AB7">
         <f t="shared" ca="1" si="0"/>
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="AC7" t="s">
         <v>119</v>
       </c>
       <c r="AD7">
         <f t="shared" ca="1" si="1"/>
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AE7" t="s">
         <v>119</v>
@@ -7125,7 +7521,7 @@
       </c>
       <c r="AL7" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman7@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,185,73,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman7@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,178,74,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="8" spans="1:38">
@@ -7210,28 +7606,28 @@
       </c>
       <c r="AB8">
         <f t="shared" ca="1" si="0"/>
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="AC8" t="s">
         <v>119</v>
       </c>
       <c r="AD8">
         <f t="shared" ca="1" si="1"/>
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="AE8" t="s">
         <v>119</v>
       </c>
       <c r="AF8">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG8" t="s">
         <v>119</v>
       </c>
       <c r="AH8">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI8" t="s">
         <v>119</v>
@@ -7244,7 +7640,7 @@
       </c>
       <c r="AL8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman8@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,177,71,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman8@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,181,77,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="9" spans="1:38">
@@ -7329,21 +7725,21 @@
       </c>
       <c r="AB9">
         <f t="shared" ca="1" si="0"/>
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="AC9" t="s">
         <v>119</v>
       </c>
       <c r="AD9">
         <f t="shared" ca="1" si="1"/>
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AE9" t="s">
         <v>119</v>
       </c>
       <c r="AF9">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG9" t="s">
         <v>119</v>
@@ -7363,7 +7759,7 @@
       </c>
       <c r="AL9" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman9@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,180,78,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman9@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,171,74,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="10" spans="1:38">
@@ -7448,21 +7844,21 @@
       </c>
       <c r="AB10">
         <f t="shared" ca="1" si="0"/>
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="AC10" t="s">
         <v>119</v>
       </c>
       <c r="AD10">
         <f t="shared" ca="1" si="1"/>
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="AE10" t="s">
         <v>119</v>
       </c>
       <c r="AF10">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG10" t="s">
         <v>119</v>
@@ -7482,7 +7878,7 @@
       </c>
       <c r="AL10" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman10@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,183,72,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman10@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,175,77,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="11" spans="1:38">
@@ -7567,21 +7963,21 @@
       </c>
       <c r="AB11">
         <f t="shared" ca="1" si="0"/>
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="AC11" t="s">
         <v>119</v>
       </c>
       <c r="AD11">
         <f t="shared" ca="1" si="1"/>
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="AE11" t="s">
         <v>119</v>
       </c>
       <c r="AF11">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG11" t="s">
         <v>119</v>
@@ -7601,7 +7997,7 @@
       </c>
       <c r="AL11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman11@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,175,73,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman11@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,177,76,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="12" spans="1:38">
@@ -7686,28 +8082,28 @@
       </c>
       <c r="AB12">
         <f t="shared" ca="1" si="0"/>
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="AC12" t="s">
         <v>119</v>
       </c>
       <c r="AD12">
         <f t="shared" ca="1" si="1"/>
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="AE12" t="s">
         <v>119</v>
       </c>
       <c r="AF12">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG12" t="s">
         <v>119</v>
       </c>
       <c r="AH12">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI12" t="s">
         <v>119</v>
@@ -7720,7 +8116,7 @@
       </c>
       <c r="AL12" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman12@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,183,72,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman12@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,173,74,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="13" spans="1:38">
@@ -7812,7 +8208,7 @@
       </c>
       <c r="AD13">
         <f t="shared" ca="1" si="1"/>
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="AE13" t="s">
         <v>119</v>
@@ -7839,7 +8235,7 @@
       </c>
       <c r="AL13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman13@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,170,80,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman13@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,170,74,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="14" spans="1:38">
@@ -7924,28 +8320,28 @@
       </c>
       <c r="AB14">
         <f t="shared" ca="1" si="0"/>
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="AC14" t="s">
         <v>119</v>
       </c>
       <c r="AD14">
         <f t="shared" ca="1" si="1"/>
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AE14" t="s">
         <v>119</v>
       </c>
       <c r="AF14">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG14" t="s">
         <v>119</v>
       </c>
       <c r="AH14">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI14" t="s">
         <v>119</v>
@@ -7958,7 +8354,7 @@
       </c>
       <c r="AL14" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman14@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,178,75,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman14@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,171,73,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="15" spans="1:38">
@@ -8043,21 +8439,21 @@
       </c>
       <c r="AB15">
         <f t="shared" ca="1" si="0"/>
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="AC15" t="s">
         <v>119</v>
       </c>
       <c r="AD15">
         <f t="shared" ca="1" si="1"/>
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="AE15" t="s">
         <v>119</v>
       </c>
       <c r="AF15">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG15" t="s">
         <v>119</v>
@@ -8077,7 +8473,7 @@
       </c>
       <c r="AL15" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman15@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,171,76,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman15@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,181,79,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="16" spans="1:38">
@@ -8162,28 +8558,28 @@
       </c>
       <c r="AB16">
         <f t="shared" ca="1" si="0"/>
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="AC16" t="s">
         <v>119</v>
       </c>
       <c r="AD16">
         <f t="shared" ca="1" si="1"/>
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="AE16" t="s">
         <v>119</v>
       </c>
       <c r="AF16">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG16" t="s">
         <v>119</v>
       </c>
       <c r="AH16">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI16" t="s">
         <v>119</v>
@@ -8196,7 +8592,7 @@
       </c>
       <c r="AL16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman16@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,171,79,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman16@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,173,74,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="17" spans="1:38">
@@ -8281,14 +8677,14 @@
       </c>
       <c r="AB17">
         <f t="shared" ca="1" si="0"/>
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="AC17" t="s">
         <v>119</v>
       </c>
       <c r="AD17">
         <f t="shared" ca="1" si="1"/>
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="AE17" t="s">
         <v>119</v>
@@ -8315,7 +8711,7 @@
       </c>
       <c r="AL17" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman17@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,183,78,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman17@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,175,72,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="20" spans="1:38">
@@ -8370,7 +8766,7 @@
       </c>
       <c r="Q20">
         <f ca="1">RANDBETWEEN(0,5)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R20" t="s">
         <v>119</v>
@@ -8404,7 +8800,7 @@
       </c>
       <c r="AB20" t="str">
         <f ca="1">_xlfn.CONCAT(A20:AA20)</f>
-        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('왕십리FC','왕십리FC201018.jpg','성동구','성동구 구장','red',4,'2016-01-01',sysdate(),'1234','기업');</v>
+        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('왕십리FC','왕십리FC201018.jpg','성동구','성동구 구장','red',1,'2016-01-01',sysdate(),'1234','기업');</v>
       </c>
     </row>
     <row r="21" spans="1:38">
@@ -8459,7 +8855,7 @@
       </c>
       <c r="Q21">
         <f t="shared" ref="Q21:Q22" ca="1" si="6">RANDBETWEEN(0,5)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R21" t="s">
         <v>119</v>
@@ -8493,7 +8889,7 @@
       </c>
       <c r="AB21" t="str">
         <f t="shared" ref="AB21:AB22" ca="1" si="7">_xlfn.CONCAT(A21:AA21)</f>
-        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('답십리FC','답십리FC201018.jpg','성동구','응봉동 구장','blue',0,'2017-01-01',sysdate(),'5678','하나');</v>
+        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('답십리FC','답십리FC201018.jpg','성동구','응봉동 구장','blue',4,'2017-01-01',sysdate(),'5678','하나');</v>
       </c>
     </row>
     <row r="22" spans="1:38">

</xml_diff>

<commit_message>
[2020-11-11 02:58] VoteMatchManager 경기 시간까지
</commit_message>
<xml_diff>
--- a/docs/srs/fbt_docs.xlsx
+++ b/docs/srs/fbt_docs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\kjy\fbt\docs\srs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177BA833-D5E4-464A-A4ED-8BC24839C6CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF38EA90-4C21-4F10-BCCD-E0624CF801B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2F0AD6B2-A8A2-4F73-BAF4-7193D3382EE1}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="TestCase_SQL" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">요구사항명세서!$B$8:$H$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">요구사항명세서!$B$8:$H$49</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="205">
   <si>
     <t>요구사항 정의서</t>
   </si>
@@ -4847,6 +4847,18 @@
       <t xml:space="preserve">
 - 해당 팀 제외한 user 중</t>
     </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>T006</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>팀 검색</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>투표 혹은 일정 등록 시 상대 팀명으로 검색</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -5650,13 +5662,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60EA499F-775F-49C1-B26C-B60E223B5AF8}">
-  <dimension ref="B1:I51"/>
+  <dimension ref="B1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D29" sqref="D29"/>
+      <selection pane="bottomRight" activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -6457,16 +6469,16 @@
       </c>
     </row>
     <row r="42" spans="2:8" ht="18" thickBot="1">
-      <c r="B42" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="C42" s="16" t="s">
-        <v>100</v>
+      <c r="B42" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>203</v>
       </c>
       <c r="D42" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="E42" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="E42" s="15" t="s">
         <v>44</v>
       </c>
       <c r="F42" s="12"/>
@@ -6474,18 +6486,18 @@
         <v>16</v>
       </c>
       <c r="H42" s="12" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="2:8" ht="18" thickBot="1">
       <c r="B43" s="29" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="D43" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>98</v>
       </c>
       <c r="E43" s="12" t="s">
         <v>44</v>
@@ -6500,13 +6512,13 @@
     </row>
     <row r="44" spans="2:8" ht="18" thickBot="1">
       <c r="B44" s="29" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E44" s="12" t="s">
         <v>44</v>
@@ -6521,13 +6533,13 @@
     </row>
     <row r="45" spans="2:8" ht="18" thickBot="1">
       <c r="B45" s="29" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E45" s="12" t="s">
         <v>44</v>
@@ -6537,18 +6549,18 @@
         <v>16</v>
       </c>
       <c r="H45" s="12" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="2:8" ht="18" thickBot="1">
       <c r="B46" s="29" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E46" s="12" t="s">
         <v>44</v>
@@ -6558,17 +6570,19 @@
         <v>16</v>
       </c>
       <c r="H46" s="12" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="2:8" ht="18" thickBot="1">
       <c r="B47" s="29" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="D47" s="18"/>
+        <v>110</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>111</v>
+      </c>
       <c r="E47" s="12" t="s">
         <v>44</v>
       </c>
@@ -6576,18 +6590,18 @@
       <c r="G47" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="H47" s="12"/>
+      <c r="H47" s="12" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="48" spans="2:8" ht="31.8" thickBot="1">
-      <c r="B48" s="31" t="s">
-        <v>161</v>
+    <row r="48" spans="2:8" ht="18" thickBot="1">
+      <c r="B48" s="29" t="s">
+        <v>112</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="D48" s="18" t="s">
-        <v>165</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="D48" s="18"/>
       <c r="E48" s="12" t="s">
         <v>44</v>
       </c>
@@ -6595,27 +6609,46 @@
       <c r="G48" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="H48" s="12" t="s">
+      <c r="H48" s="12"/>
+    </row>
+    <row r="49" spans="2:8" ht="31.8" thickBot="1">
+      <c r="B49" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="C49" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H49" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="4:4">
-      <c r="D49" s="35" t="s">
+    <row r="50" spans="2:8">
+      <c r="D50" s="35" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="50" spans="4:4" ht="52.2">
-      <c r="D50" s="36" t="s">
+    <row r="51" spans="2:8" ht="52.2">
+      <c r="D51" s="36" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="51" spans="4:4">
-      <c r="D51" s="37" t="s">
+    <row r="52" spans="2:8">
+      <c r="D52" s="37" t="s">
         <v>194</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B8:H48" xr:uid="{08681459-A406-4CEE-9A8A-D3DF83B63176}">
+  <autoFilter ref="B8:H49" xr:uid="{08681459-A406-4CEE-9A8A-D3DF83B63176}">
     <filterColumn colId="3" showButton="0"/>
   </autoFilter>
   <mergeCells count="8">
@@ -6773,28 +6806,28 @@
       </c>
       <c r="AB1">
         <f ca="1">RANDBETWEEN(170,185)</f>
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AC1" t="s">
         <v>119</v>
       </c>
       <c r="AD1">
         <f ca="1">RANDBETWEEN(70,80)</f>
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="AE1" t="s">
         <v>119</v>
       </c>
       <c r="AF1">
         <f ca="1">RANDBETWEEN(0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG1" t="s">
         <v>119</v>
       </c>
       <c r="AH1">
         <f ca="1">RANDBETWEEN(0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI1" t="s">
         <v>119</v>
@@ -6807,7 +6840,7 @@
       </c>
       <c r="AL1" t="str">
         <f ca="1">_xlfn.CONCAT(A1:AK1)</f>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman1@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,177,73,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman1@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,176,75,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="2" spans="1:38">
@@ -6892,28 +6925,28 @@
       </c>
       <c r="AB2">
         <f t="shared" ref="AB2:AB17" ca="1" si="0">RANDBETWEEN(170,185)</f>
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="AC2" t="s">
         <v>119</v>
       </c>
       <c r="AD2">
         <f t="shared" ref="AD2:AD17" ca="1" si="1">RANDBETWEEN(70,80)</f>
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="AE2" t="s">
         <v>119</v>
       </c>
       <c r="AF2">
         <f t="shared" ref="AF2:AF17" ca="1" si="2">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG2" t="s">
         <v>119</v>
       </c>
       <c r="AH2">
         <f t="shared" ref="AH2:AH17" ca="1" si="3">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI2" t="s">
         <v>119</v>
@@ -6926,7 +6959,7 @@
       </c>
       <c r="AL2" t="str">
         <f t="shared" ref="AL2:AL17" ca="1" si="4">_xlfn.CONCAT(A2:AK2)</f>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman2@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,180,79,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman2@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,181,70,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="3" spans="1:38">
@@ -7011,14 +7044,14 @@
       </c>
       <c r="AB3">
         <f t="shared" ca="1" si="0"/>
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="AC3" t="s">
         <v>119</v>
       </c>
       <c r="AD3">
         <f t="shared" ca="1" si="1"/>
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="AE3" t="s">
         <v>119</v>
@@ -7032,7 +7065,7 @@
       </c>
       <c r="AH3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI3" t="s">
         <v>119</v>
@@ -7045,7 +7078,7 @@
       </c>
       <c r="AL3" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman3@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,171,80,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman3@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,179,76,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="4" spans="1:38">
@@ -7130,28 +7163,28 @@
       </c>
       <c r="AB4">
         <f t="shared" ca="1" si="0"/>
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="AC4" t="s">
         <v>119</v>
       </c>
       <c r="AD4">
         <f t="shared" ca="1" si="1"/>
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AE4" t="s">
         <v>119</v>
       </c>
       <c r="AF4">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG4" t="s">
         <v>119</v>
       </c>
       <c r="AH4">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI4" t="s">
         <v>119</v>
@@ -7164,7 +7197,7 @@
       </c>
       <c r="AL4" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman4@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,172,73,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman4@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,175,72,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="5" spans="1:38">
@@ -7249,14 +7282,14 @@
       </c>
       <c r="AB5">
         <f t="shared" ca="1" si="0"/>
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="AC5" t="s">
         <v>119</v>
       </c>
       <c r="AD5">
         <f t="shared" ca="1" si="1"/>
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="AE5" t="s">
         <v>119</v>
@@ -7270,7 +7303,7 @@
       </c>
       <c r="AH5">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI5" t="s">
         <v>119</v>
@@ -7283,7 +7316,7 @@
       </c>
       <c r="AL5" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman5@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,173,80,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman5@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,170,77,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="6" spans="1:38">
@@ -7375,14 +7408,14 @@
       </c>
       <c r="AD6">
         <f t="shared" ca="1" si="1"/>
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="AE6" t="s">
         <v>119</v>
       </c>
       <c r="AF6">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG6" t="s">
         <v>119</v>
@@ -7402,7 +7435,7 @@
       </c>
       <c r="AL6" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman6@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,185,76,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman6@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,185,70,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="7" spans="1:38">
@@ -7487,7 +7520,7 @@
       </c>
       <c r="AB7">
         <f t="shared" ca="1" si="0"/>
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="AC7" t="s">
         <v>119</v>
@@ -7501,7 +7534,7 @@
       </c>
       <c r="AF7">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG7" t="s">
         <v>119</v>
@@ -7521,7 +7554,7 @@
       </c>
       <c r="AL7" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman7@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,178,74,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman7@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,170,74,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="8" spans="1:38">
@@ -7606,7 +7639,7 @@
       </c>
       <c r="AB8">
         <f t="shared" ca="1" si="0"/>
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="AC8" t="s">
         <v>119</v>
@@ -7620,7 +7653,7 @@
       </c>
       <c r="AF8">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG8" t="s">
         <v>119</v>
@@ -7640,7 +7673,7 @@
       </c>
       <c r="AL8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman8@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,181,77,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman8@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,178,77,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="9" spans="1:38">
@@ -7725,14 +7758,14 @@
       </c>
       <c r="AB9">
         <f t="shared" ca="1" si="0"/>
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="AC9" t="s">
         <v>119</v>
       </c>
       <c r="AD9">
         <f t="shared" ca="1" si="1"/>
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AE9" t="s">
         <v>119</v>
@@ -7746,7 +7779,7 @@
       </c>
       <c r="AH9">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI9" t="s">
         <v>119</v>
@@ -7759,7 +7792,7 @@
       </c>
       <c r="AL9" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman9@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,171,74,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman9@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,184,75,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="10" spans="1:38">
@@ -7844,21 +7877,21 @@
       </c>
       <c r="AB10">
         <f t="shared" ca="1" si="0"/>
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="AC10" t="s">
         <v>119</v>
       </c>
       <c r="AD10">
         <f t="shared" ca="1" si="1"/>
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AE10" t="s">
         <v>119</v>
       </c>
       <c r="AF10">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG10" t="s">
         <v>119</v>
@@ -7878,7 +7911,7 @@
       </c>
       <c r="AL10" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman10@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,175,77,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman10@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,173,76,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="11" spans="1:38">
@@ -7963,14 +7996,14 @@
       </c>
       <c r="AB11">
         <f t="shared" ca="1" si="0"/>
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="AC11" t="s">
         <v>119</v>
       </c>
       <c r="AD11">
         <f t="shared" ca="1" si="1"/>
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="AE11" t="s">
         <v>119</v>
@@ -7997,7 +8030,7 @@
       </c>
       <c r="AL11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman11@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,177,76,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman11@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,170,70,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="12" spans="1:38">
@@ -8082,28 +8115,28 @@
       </c>
       <c r="AB12">
         <f t="shared" ca="1" si="0"/>
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AC12" t="s">
         <v>119</v>
       </c>
       <c r="AD12">
         <f t="shared" ca="1" si="1"/>
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="AE12" t="s">
         <v>119</v>
       </c>
       <c r="AF12">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG12" t="s">
         <v>119</v>
       </c>
       <c r="AH12">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI12" t="s">
         <v>119</v>
@@ -8116,7 +8149,7 @@
       </c>
       <c r="AL12" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman12@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,173,74,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman12@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,172,80,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="13" spans="1:38">
@@ -8201,28 +8234,28 @@
       </c>
       <c r="AB13">
         <f t="shared" ca="1" si="0"/>
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="AC13" t="s">
         <v>119</v>
       </c>
       <c r="AD13">
         <f t="shared" ca="1" si="1"/>
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="AE13" t="s">
         <v>119</v>
       </c>
       <c r="AF13">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG13" t="s">
         <v>119</v>
       </c>
       <c r="AH13">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI13" t="s">
         <v>119</v>
@@ -8235,7 +8268,7 @@
       </c>
       <c r="AL13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman13@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,170,74,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman13@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,177,78,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="14" spans="1:38">
@@ -8320,7 +8353,7 @@
       </c>
       <c r="AB14">
         <f t="shared" ca="1" si="0"/>
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="AC14" t="s">
         <v>119</v>
@@ -8334,14 +8367,14 @@
       </c>
       <c r="AF14">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG14" t="s">
         <v>119</v>
       </c>
       <c r="AH14">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI14" t="s">
         <v>119</v>
@@ -8354,7 +8387,7 @@
       </c>
       <c r="AL14" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman14@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,171,73,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman14@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,182,73,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="15" spans="1:38">
@@ -8439,14 +8472,14 @@
       </c>
       <c r="AB15">
         <f t="shared" ca="1" si="0"/>
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="AC15" t="s">
         <v>119</v>
       </c>
       <c r="AD15">
         <f t="shared" ca="1" si="1"/>
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AE15" t="s">
         <v>119</v>
@@ -8473,7 +8506,7 @@
       </c>
       <c r="AL15" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman15@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,181,79,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman15@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,185,78,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="16" spans="1:38">
@@ -8558,7 +8591,7 @@
       </c>
       <c r="AB16">
         <f t="shared" ca="1" si="0"/>
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="AC16" t="s">
         <v>119</v>
@@ -8579,7 +8612,7 @@
       </c>
       <c r="AH16">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI16" t="s">
         <v>119</v>
@@ -8592,7 +8625,7 @@
       </c>
       <c r="AL16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman16@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,173,74,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman16@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,177,74,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="17" spans="1:38">
@@ -8684,7 +8717,7 @@
       </c>
       <c r="AD17">
         <f t="shared" ca="1" si="1"/>
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="AE17" t="s">
         <v>119</v>
@@ -8711,7 +8744,7 @@
       </c>
       <c r="AL17" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman17@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,175,72,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman17@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,175,76,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="20" spans="1:38">
@@ -8855,7 +8888,7 @@
       </c>
       <c r="Q21">
         <f t="shared" ref="Q21:Q22" ca="1" si="6">RANDBETWEEN(0,5)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R21" t="s">
         <v>119</v>
@@ -8889,7 +8922,7 @@
       </c>
       <c r="AB21" t="str">
         <f t="shared" ref="AB21:AB22" ca="1" si="7">_xlfn.CONCAT(A21:AA21)</f>
-        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('답십리FC','답십리FC201018.jpg','성동구','응봉동 구장','blue',4,'2017-01-01',sysdate(),'5678','하나');</v>
+        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('답십리FC','답십리FC201018.jpg','성동구','응봉동 구장','blue',1,'2017-01-01',sysdate(),'5678','하나');</v>
       </c>
     </row>
     <row r="22" spans="1:38">
@@ -8944,7 +8977,7 @@
       </c>
       <c r="Q22">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="R22" t="s">
         <v>119</v>
@@ -8978,7 +9011,7 @@
       </c>
       <c r="AB22" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('대구FC','대구FC201018.jpg','달서구','달서구 구장','green',2,'2018-01-01',sysdate(),'2345','기업');</v>
+        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('대구FC','대구FC201018.jpg','달서구','달서구 구장','green',5,'2018-01-01',sysdate(),'2345','기업');</v>
       </c>
     </row>
     <row r="24" spans="1:38">

</xml_diff>

<commit_message>
[2020-11-13 06:25] VoteMatchManager 거의 구현 (exp. 버튼, 자동화)
</commit_message>
<xml_diff>
--- a/docs/srs/fbt_docs.xlsx
+++ b/docs/srs/fbt_docs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\kjy\fbt\docs\srs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF38EA90-4C21-4F10-BCCD-E0624CF801B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8628B36-E31F-4228-8EEB-2427FAFB2A49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2F0AD6B2-A8A2-4F73-BAF4-7193D3382EE1}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="207">
   <si>
     <t>요구사항 정의서</t>
   </si>
@@ -3950,19 +3950,6 @@
       </rPr>
       <t xml:space="preserve"> V003
 투표결과ID 양식 : '투표ID-팀멤버ID or 이메일(지인)'</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>카톡공유</t>
     </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -4859,6 +4846,93 @@
   </si>
   <si>
     <t>투표 혹은 일정 등록 시 상대 팀명으로 검색</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>S002</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>방금 등록된 팀</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>경기</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ID </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>출력</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">방금 등록된 팀 경기 ID 일정 </t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -5214,7 +5288,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -5319,9 +5393,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -5665,10 +5736,10 @@
   <dimension ref="B1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E43" sqref="E43"/>
+      <selection pane="bottomRight" activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -5686,10 +5757,10 @@
   <sheetData>
     <row r="1" spans="2:9" ht="18" thickBot="1"/>
     <row r="2" spans="2:9" ht="18" thickBot="1">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="41"/>
+      <c r="C2" s="40"/>
       <c r="E2" s="3" t="s">
         <v>63</v>
       </c>
@@ -5748,42 +5819,42 @@
     </row>
     <row r="7" spans="2:9" ht="18" thickBot="1"/>
     <row r="8" spans="2:9" ht="18" thickBot="1">
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="42" t="s">
+      <c r="E8" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="43"/>
-      <c r="G8" s="38" t="s">
+      <c r="F8" s="42"/>
+      <c r="G8" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="38" t="s">
+      <c r="H8" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="38" t="s">
+      <c r="I8" s="37" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="18" thickBot="1">
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
       <c r="E9" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
     </row>
     <row r="10" spans="2:9" ht="27" thickBot="1">
       <c r="B10" s="11" t="s">
@@ -5994,7 +6065,7 @@
         <v>41</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E19" s="12" t="s">
         <v>30</v>
@@ -6161,13 +6232,13 @@
     </row>
     <row r="27" spans="2:9" ht="18" thickBot="1">
       <c r="B27" s="34" t="s">
+        <v>194</v>
+      </c>
+      <c r="C27" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="D27" s="18" t="s">
         <v>196</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>197</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>30</v>
@@ -6179,13 +6250,13 @@
     </row>
     <row r="28" spans="2:9" ht="29.4" thickBot="1">
       <c r="B28" s="34" t="s">
+        <v>197</v>
+      </c>
+      <c r="C28" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="C28" s="16" t="s">
-        <v>199</v>
-      </c>
       <c r="D28" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>30</v>
@@ -6470,13 +6541,13 @@
     </row>
     <row r="42" spans="2:8" ht="18" thickBot="1">
       <c r="B42" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="C42" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="D42" s="13" t="s">
         <v>203</v>
-      </c>
-      <c r="D42" s="13" t="s">
-        <v>204</v>
       </c>
       <c r="E42" s="15" t="s">
         <v>44</v>
@@ -6632,19 +6703,35 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="2:8">
-      <c r="D50" s="35" t="s">
-        <v>192</v>
+    <row r="50" spans="2:8" ht="31.8" thickBot="1">
+      <c r="B50" s="31" t="s">
+        <v>204</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="E50" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H50" s="15" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="2:8" ht="52.2">
-      <c r="D51" s="36" t="s">
-        <v>193</v>
+      <c r="D51" s="35" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="52" spans="2:8">
-      <c r="D52" s="37" t="s">
-        <v>194</v>
+      <c r="D52" s="36" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -6806,21 +6893,21 @@
       </c>
       <c r="AB1">
         <f ca="1">RANDBETWEEN(170,185)</f>
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="AC1" t="s">
         <v>119</v>
       </c>
       <c r="AD1">
         <f ca="1">RANDBETWEEN(70,80)</f>
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="AE1" t="s">
         <v>119</v>
       </c>
       <c r="AF1">
         <f ca="1">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG1" t="s">
         <v>119</v>
@@ -6840,7 +6927,7 @@
       </c>
       <c r="AL1" t="str">
         <f ca="1">_xlfn.CONCAT(A1:AK1)</f>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman1@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,176,75,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman1@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,185,77,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="2" spans="1:38">
@@ -6925,21 +7012,21 @@
       </c>
       <c r="AB2">
         <f t="shared" ref="AB2:AB17" ca="1" si="0">RANDBETWEEN(170,185)</f>
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="AC2" t="s">
         <v>119</v>
       </c>
       <c r="AD2">
         <f t="shared" ref="AD2:AD17" ca="1" si="1">RANDBETWEEN(70,80)</f>
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="AE2" t="s">
         <v>119</v>
       </c>
       <c r="AF2">
         <f t="shared" ref="AF2:AF17" ca="1" si="2">RANDBETWEEN(0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG2" t="s">
         <v>119</v>
@@ -6959,7 +7046,7 @@
       </c>
       <c r="AL2" t="str">
         <f t="shared" ref="AL2:AL17" ca="1" si="4">_xlfn.CONCAT(A2:AK2)</f>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman2@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,181,70,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman2@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,170,75,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="3" spans="1:38">
@@ -7051,7 +7138,7 @@
       </c>
       <c r="AD3">
         <f t="shared" ca="1" si="1"/>
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="AE3" t="s">
         <v>119</v>
@@ -7078,7 +7165,7 @@
       </c>
       <c r="AL3" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman3@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,179,76,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman3@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,179,80,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="4" spans="1:38">
@@ -7170,7 +7257,7 @@
       </c>
       <c r="AD4">
         <f t="shared" ca="1" si="1"/>
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="AE4" t="s">
         <v>119</v>
@@ -7184,7 +7271,7 @@
       </c>
       <c r="AH4">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI4" t="s">
         <v>119</v>
@@ -7197,7 +7284,7 @@
       </c>
       <c r="AL4" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman4@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,175,72,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman4@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,175,79,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="5" spans="1:38">
@@ -7282,14 +7369,14 @@
       </c>
       <c r="AB5">
         <f t="shared" ca="1" si="0"/>
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="AC5" t="s">
         <v>119</v>
       </c>
       <c r="AD5">
         <f t="shared" ca="1" si="1"/>
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AE5" t="s">
         <v>119</v>
@@ -7316,7 +7403,7 @@
       </c>
       <c r="AL5" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman5@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,170,77,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman5@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,184,78,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="6" spans="1:38">
@@ -7401,7 +7488,7 @@
       </c>
       <c r="AB6">
         <f t="shared" ca="1" si="0"/>
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="AC6" t="s">
         <v>119</v>
@@ -7415,7 +7502,7 @@
       </c>
       <c r="AF6">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG6" t="s">
         <v>119</v>
@@ -7435,7 +7522,7 @@
       </c>
       <c r="AL6" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman6@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,185,70,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman6@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,183,70,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="7" spans="1:38">
@@ -7520,7 +7607,7 @@
       </c>
       <c r="AB7">
         <f t="shared" ca="1" si="0"/>
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="AC7" t="s">
         <v>119</v>
@@ -7541,7 +7628,7 @@
       </c>
       <c r="AH7">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI7" t="s">
         <v>119</v>
@@ -7554,7 +7641,7 @@
       </c>
       <c r="AL7" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman7@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,170,74,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman7@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,175,74,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="8" spans="1:38">
@@ -7639,21 +7726,21 @@
       </c>
       <c r="AB8">
         <f t="shared" ca="1" si="0"/>
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="AC8" t="s">
         <v>119</v>
       </c>
       <c r="AD8">
         <f t="shared" ca="1" si="1"/>
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AE8" t="s">
         <v>119</v>
       </c>
       <c r="AF8">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG8" t="s">
         <v>119</v>
@@ -7673,7 +7760,7 @@
       </c>
       <c r="AL8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman8@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,178,77,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman8@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,173,76,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="9" spans="1:38">
@@ -7758,21 +7845,21 @@
       </c>
       <c r="AB9">
         <f t="shared" ca="1" si="0"/>
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="AC9" t="s">
         <v>119</v>
       </c>
       <c r="AD9">
         <f t="shared" ca="1" si="1"/>
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="AE9" t="s">
         <v>119</v>
       </c>
       <c r="AF9">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG9" t="s">
         <v>119</v>
@@ -7792,7 +7879,7 @@
       </c>
       <c r="AL9" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman9@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,184,75,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman9@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,181,77,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="10" spans="1:38">
@@ -7877,28 +7964,28 @@
       </c>
       <c r="AB10">
         <f t="shared" ca="1" si="0"/>
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="AC10" t="s">
         <v>119</v>
       </c>
       <c r="AD10">
         <f t="shared" ca="1" si="1"/>
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="AE10" t="s">
         <v>119</v>
       </c>
       <c r="AF10">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG10" t="s">
         <v>119</v>
       </c>
       <c r="AH10">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI10" t="s">
         <v>119</v>
@@ -7911,7 +7998,7 @@
       </c>
       <c r="AL10" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman10@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,173,76,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman10@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,176,71,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="11" spans="1:38">
@@ -7996,28 +8083,28 @@
       </c>
       <c r="AB11">
         <f t="shared" ca="1" si="0"/>
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="AC11" t="s">
         <v>119</v>
       </c>
       <c r="AD11">
         <f t="shared" ca="1" si="1"/>
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AE11" t="s">
         <v>119</v>
       </c>
       <c r="AF11">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG11" t="s">
         <v>119</v>
       </c>
       <c r="AH11">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI11" t="s">
         <v>119</v>
@@ -8030,7 +8117,7 @@
       </c>
       <c r="AL11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman11@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,170,70,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman11@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,180,71,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="12" spans="1:38">
@@ -8115,14 +8202,14 @@
       </c>
       <c r="AB12">
         <f t="shared" ca="1" si="0"/>
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="AC12" t="s">
         <v>119</v>
       </c>
       <c r="AD12">
         <f t="shared" ca="1" si="1"/>
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="AE12" t="s">
         <v>119</v>
@@ -8136,7 +8223,7 @@
       </c>
       <c r="AH12">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI12" t="s">
         <v>119</v>
@@ -8149,7 +8236,7 @@
       </c>
       <c r="AL12" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman12@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,172,80,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman12@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,184,72,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="13" spans="1:38">
@@ -8234,14 +8321,14 @@
       </c>
       <c r="AB13">
         <f t="shared" ca="1" si="0"/>
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AC13" t="s">
         <v>119</v>
       </c>
       <c r="AD13">
         <f t="shared" ca="1" si="1"/>
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="AE13" t="s">
         <v>119</v>
@@ -8268,7 +8355,7 @@
       </c>
       <c r="AL13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman13@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,177,78,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman13@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,176,71,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="14" spans="1:38">
@@ -8353,21 +8440,21 @@
       </c>
       <c r="AB14">
         <f t="shared" ca="1" si="0"/>
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="AC14" t="s">
         <v>119</v>
       </c>
       <c r="AD14">
         <f t="shared" ca="1" si="1"/>
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="AE14" t="s">
         <v>119</v>
       </c>
       <c r="AF14">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG14" t="s">
         <v>119</v>
@@ -8387,7 +8474,7 @@
       </c>
       <c r="AL14" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman14@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,182,73,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman14@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,174,70,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="15" spans="1:38">
@@ -8472,7 +8559,7 @@
       </c>
       <c r="AB15">
         <f t="shared" ca="1" si="0"/>
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="AC15" t="s">
         <v>119</v>
@@ -8506,7 +8593,7 @@
       </c>
       <c r="AL15" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman15@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,185,78,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman15@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,173,78,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="16" spans="1:38">
@@ -8591,21 +8678,21 @@
       </c>
       <c r="AB16">
         <f t="shared" ca="1" si="0"/>
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="AC16" t="s">
         <v>119</v>
       </c>
       <c r="AD16">
         <f t="shared" ca="1" si="1"/>
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="AE16" t="s">
         <v>119</v>
       </c>
       <c r="AF16">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG16" t="s">
         <v>119</v>
@@ -8625,7 +8712,7 @@
       </c>
       <c r="AL16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman16@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,177,74,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman16@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,185,80,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="17" spans="1:38">
@@ -8710,28 +8797,28 @@
       </c>
       <c r="AB17">
         <f t="shared" ca="1" si="0"/>
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="AC17" t="s">
         <v>119</v>
       </c>
       <c r="AD17">
         <f t="shared" ca="1" si="1"/>
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AE17" t="s">
         <v>119</v>
       </c>
       <c r="AF17">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG17" t="s">
         <v>119</v>
       </c>
       <c r="AH17">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI17" t="s">
         <v>119</v>
@@ -8744,7 +8831,7 @@
       </c>
       <c r="AL17" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman17@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,175,76,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman17@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,170,75,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="20" spans="1:38">
@@ -8799,7 +8886,7 @@
       </c>
       <c r="Q20">
         <f ca="1">RANDBETWEEN(0,5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R20" t="s">
         <v>119</v>
@@ -8833,7 +8920,7 @@
       </c>
       <c r="AB20" t="str">
         <f ca="1">_xlfn.CONCAT(A20:AA20)</f>
-        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('왕십리FC','왕십리FC201018.jpg','성동구','성동구 구장','red',1,'2016-01-01',sysdate(),'1234','기업');</v>
+        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('왕십리FC','왕십리FC201018.jpg','성동구','성동구 구장','red',2,'2016-01-01',sysdate(),'1234','기업');</v>
       </c>
     </row>
     <row r="21" spans="1:38">
@@ -8888,7 +8975,7 @@
       </c>
       <c r="Q21">
         <f t="shared" ref="Q21:Q22" ca="1" si="6">RANDBETWEEN(0,5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R21" t="s">
         <v>119</v>
@@ -8922,7 +9009,7 @@
       </c>
       <c r="AB21" t="str">
         <f t="shared" ref="AB21:AB22" ca="1" si="7">_xlfn.CONCAT(A21:AA21)</f>
-        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('답십리FC','답십리FC201018.jpg','성동구','응봉동 구장','blue',1,'2017-01-01',sysdate(),'5678','하나');</v>
+        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('답십리FC','답십리FC201018.jpg','성동구','응봉동 구장','blue',2,'2017-01-01',sysdate(),'5678','하나');</v>
       </c>
     </row>
     <row r="22" spans="1:38">

</xml_diff>

<commit_message>
[2020-11-17 21:40] 일정 제작 중
</commit_message>
<xml_diff>
--- a/docs/srs/fbt_docs.xlsx
+++ b/docs/srs/fbt_docs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\kjy\fbt\docs\srs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8628B36-E31F-4228-8EEB-2427FAFB2A49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4A1331-E6FA-4362-A0C3-BECD2C69553F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2F0AD6B2-A8A2-4F73-BAF4-7193D3382EE1}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="217">
   <si>
     <t>요구사항 정의서</t>
   </si>
@@ -4933,6 +4933,46 @@
   </si>
   <si>
     <t xml:space="preserve">방금 등록된 팀 경기 ID 일정 </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>S003</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>팀 경기 일정 수정</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록된 경기 일정 수정</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>S004</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>팀 경기 일정 삭제</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록된 경기 일정 삭제</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">하 </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>S005</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>팀 경기 일정 출력</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록된 팀 경기 일정 출력</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -5158,7 +5198,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -5279,6 +5319,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -5288,7 +5365,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -5417,6 +5494,42 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5733,13 +5846,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60EA499F-775F-49C1-B26C-B60E223B5AF8}">
-  <dimension ref="B1:I52"/>
+  <dimension ref="B1:I55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B46" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D51" sqref="D51"/>
+      <selection pane="bottomRight" activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -6704,33 +6817,96 @@
       </c>
     </row>
     <row r="50" spans="2:8" ht="31.8" thickBot="1">
-      <c r="B50" s="31" t="s">
+      <c r="B50" s="43" t="s">
         <v>204</v>
       </c>
-      <c r="C50" s="15" t="s">
+      <c r="C50" s="44" t="s">
         <v>206</v>
       </c>
-      <c r="D50" s="18" t="s">
+      <c r="D50" s="45" t="s">
         <v>205</v>
       </c>
-      <c r="E50" s="15" t="s">
+      <c r="E50" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="F50" s="12"/>
-      <c r="G50" s="12" t="s">
+      <c r="F50" s="46"/>
+      <c r="G50" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="H50" s="15" t="s">
+      <c r="H50" s="44" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="2:8" ht="52.2">
-      <c r="D51" s="35" t="s">
+    <row r="51" spans="2:8" ht="18" thickBot="1">
+      <c r="B51" s="31" t="s">
+        <v>207</v>
+      </c>
+      <c r="C51" s="47" t="s">
+        <v>208</v>
+      </c>
+      <c r="D51" s="48" t="s">
+        <v>209</v>
+      </c>
+      <c r="E51" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="F51" s="49"/>
+      <c r="G51" s="49" t="s">
+        <v>213</v>
+      </c>
+      <c r="H51" s="47" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" ht="18" thickBot="1">
+      <c r="B52" s="50" t="s">
+        <v>210</v>
+      </c>
+      <c r="C52" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="D52" s="52" t="s">
+        <v>212</v>
+      </c>
+      <c r="E52" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="F52" s="53"/>
+      <c r="G52" s="53" t="s">
+        <v>213</v>
+      </c>
+      <c r="H52" s="51" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" ht="18" thickBot="1">
+      <c r="B53" s="50" t="s">
+        <v>214</v>
+      </c>
+      <c r="C53" s="51" t="s">
+        <v>215</v>
+      </c>
+      <c r="D53" s="54" t="s">
+        <v>216</v>
+      </c>
+      <c r="E53" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="F53" s="53"/>
+      <c r="G53" s="53" t="s">
+        <v>213</v>
+      </c>
+      <c r="H53" s="51" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" ht="52.2">
+      <c r="D54" s="35" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="52" spans="2:8">
-      <c r="D52" s="36" t="s">
+    <row r="55" spans="2:8">
+      <c r="D55" s="36" t="s">
         <v>193</v>
       </c>
     </row>
@@ -6893,14 +7069,14 @@
       </c>
       <c r="AB1">
         <f ca="1">RANDBETWEEN(170,185)</f>
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="AC1" t="s">
         <v>119</v>
       </c>
       <c r="AD1">
         <f ca="1">RANDBETWEEN(70,80)</f>
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="AE1" t="s">
         <v>119</v>
@@ -6927,7 +7103,7 @@
       </c>
       <c r="AL1" t="str">
         <f ca="1">_xlfn.CONCAT(A1:AK1)</f>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman1@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,185,77,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman1@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,175,74,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="2" spans="1:38">
@@ -7012,21 +7188,21 @@
       </c>
       <c r="AB2">
         <f t="shared" ref="AB2:AB17" ca="1" si="0">RANDBETWEEN(170,185)</f>
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="AC2" t="s">
         <v>119</v>
       </c>
       <c r="AD2">
         <f t="shared" ref="AD2:AD17" ca="1" si="1">RANDBETWEEN(70,80)</f>
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="AE2" t="s">
         <v>119</v>
       </c>
       <c r="AF2">
         <f t="shared" ref="AF2:AF17" ca="1" si="2">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG2" t="s">
         <v>119</v>
@@ -7046,7 +7222,7 @@
       </c>
       <c r="AL2" t="str">
         <f t="shared" ref="AL2:AL17" ca="1" si="4">_xlfn.CONCAT(A2:AK2)</f>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman2@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,170,75,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman2@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,176,79,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="3" spans="1:38">
@@ -7131,21 +7307,21 @@
       </c>
       <c r="AB3">
         <f t="shared" ca="1" si="0"/>
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="AC3" t="s">
         <v>119</v>
       </c>
       <c r="AD3">
         <f t="shared" ca="1" si="1"/>
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="AE3" t="s">
         <v>119</v>
       </c>
       <c r="AF3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG3" t="s">
         <v>119</v>
@@ -7165,7 +7341,7 @@
       </c>
       <c r="AL3" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman3@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,179,80,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman3@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,171,78,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="4" spans="1:38">
@@ -7250,14 +7426,14 @@
       </c>
       <c r="AB4">
         <f t="shared" ca="1" si="0"/>
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AC4" t="s">
         <v>119</v>
       </c>
       <c r="AD4">
         <f t="shared" ca="1" si="1"/>
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="AE4" t="s">
         <v>119</v>
@@ -7271,7 +7447,7 @@
       </c>
       <c r="AH4">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI4" t="s">
         <v>119</v>
@@ -7284,7 +7460,7 @@
       </c>
       <c r="AL4" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman4@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,175,79,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman4@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,174,76,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="5" spans="1:38">
@@ -7369,28 +7545,28 @@
       </c>
       <c r="AB5">
         <f t="shared" ca="1" si="0"/>
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="AC5" t="s">
         <v>119</v>
       </c>
       <c r="AD5">
         <f t="shared" ca="1" si="1"/>
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AE5" t="s">
         <v>119</v>
       </c>
       <c r="AF5">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG5" t="s">
         <v>119</v>
       </c>
       <c r="AH5">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI5" t="s">
         <v>119</v>
@@ -7403,7 +7579,7 @@
       </c>
       <c r="AL5" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman5@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,184,78,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman5@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,177,77,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="6" spans="1:38">
@@ -7488,28 +7664,28 @@
       </c>
       <c r="AB6">
         <f t="shared" ca="1" si="0"/>
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="AC6" t="s">
         <v>119</v>
       </c>
       <c r="AD6">
         <f t="shared" ca="1" si="1"/>
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="AE6" t="s">
         <v>119</v>
       </c>
       <c r="AF6">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG6" t="s">
         <v>119</v>
       </c>
       <c r="AH6">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI6" t="s">
         <v>119</v>
@@ -7522,7 +7698,7 @@
       </c>
       <c r="AL6" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman6@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,183,70,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman6@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,174,75,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="7" spans="1:38">
@@ -7607,14 +7783,14 @@
       </c>
       <c r="AB7">
         <f t="shared" ca="1" si="0"/>
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="AC7" t="s">
         <v>119</v>
       </c>
       <c r="AD7">
         <f t="shared" ca="1" si="1"/>
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AE7" t="s">
         <v>119</v>
@@ -7628,7 +7804,7 @@
       </c>
       <c r="AH7">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI7" t="s">
         <v>119</v>
@@ -7641,7 +7817,7 @@
       </c>
       <c r="AL7" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman7@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,175,74,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman7@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,173,72,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="8" spans="1:38">
@@ -7726,28 +7902,28 @@
       </c>
       <c r="AB8">
         <f t="shared" ca="1" si="0"/>
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="AC8" t="s">
         <v>119</v>
       </c>
       <c r="AD8">
         <f t="shared" ca="1" si="1"/>
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AE8" t="s">
         <v>119</v>
       </c>
       <c r="AF8">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG8" t="s">
         <v>119</v>
       </c>
       <c r="AH8">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI8" t="s">
         <v>119</v>
@@ -7760,7 +7936,7 @@
       </c>
       <c r="AL8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman8@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,173,76,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman8@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,174,74,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="9" spans="1:38">
@@ -7845,14 +8021,14 @@
       </c>
       <c r="AB9">
         <f t="shared" ca="1" si="0"/>
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="AC9" t="s">
         <v>119</v>
       </c>
       <c r="AD9">
         <f t="shared" ca="1" si="1"/>
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AE9" t="s">
         <v>119</v>
@@ -7879,7 +8055,7 @@
       </c>
       <c r="AL9" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman9@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,181,77,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman9@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,183,76,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="10" spans="1:38">
@@ -7964,7 +8140,7 @@
       </c>
       <c r="AB10">
         <f t="shared" ca="1" si="0"/>
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="AC10" t="s">
         <v>119</v>
@@ -7978,7 +8154,7 @@
       </c>
       <c r="AF10">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG10" t="s">
         <v>119</v>
@@ -7998,7 +8174,7 @@
       </c>
       <c r="AL10" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman10@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,176,71,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman10@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,178,71,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="11" spans="1:38">
@@ -8083,14 +8259,14 @@
       </c>
       <c r="AB11">
         <f t="shared" ca="1" si="0"/>
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="AC11" t="s">
         <v>119</v>
       </c>
       <c r="AD11">
         <f t="shared" ca="1" si="1"/>
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="AE11" t="s">
         <v>119</v>
@@ -8117,7 +8293,7 @@
       </c>
       <c r="AL11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman11@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,180,71,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman11@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,182,77,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="12" spans="1:38">
@@ -8202,14 +8378,14 @@
       </c>
       <c r="AB12">
         <f t="shared" ca="1" si="0"/>
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="AC12" t="s">
         <v>119</v>
       </c>
       <c r="AD12">
         <f t="shared" ca="1" si="1"/>
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="AE12" t="s">
         <v>119</v>
@@ -8223,7 +8399,7 @@
       </c>
       <c r="AH12">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI12" t="s">
         <v>119</v>
@@ -8236,7 +8412,7 @@
       </c>
       <c r="AL12" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman12@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,184,72,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman12@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,178,76,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="13" spans="1:38">
@@ -8321,21 +8497,21 @@
       </c>
       <c r="AB13">
         <f t="shared" ca="1" si="0"/>
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="AC13" t="s">
         <v>119</v>
       </c>
       <c r="AD13">
         <f t="shared" ca="1" si="1"/>
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="AE13" t="s">
         <v>119</v>
       </c>
       <c r="AF13">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG13" t="s">
         <v>119</v>
@@ -8355,7 +8531,7 @@
       </c>
       <c r="AL13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman13@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,176,71,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman13@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,173,80,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="14" spans="1:38">
@@ -8440,28 +8616,28 @@
       </c>
       <c r="AB14">
         <f t="shared" ca="1" si="0"/>
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="AC14" t="s">
         <v>119</v>
       </c>
       <c r="AD14">
         <f t="shared" ca="1" si="1"/>
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="AE14" t="s">
         <v>119</v>
       </c>
       <c r="AF14">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG14" t="s">
         <v>119</v>
       </c>
       <c r="AH14">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI14" t="s">
         <v>119</v>
@@ -8474,7 +8650,7 @@
       </c>
       <c r="AL14" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman14@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,174,70,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman14@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,179,77,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="15" spans="1:38">
@@ -8559,21 +8735,21 @@
       </c>
       <c r="AB15">
         <f t="shared" ca="1" si="0"/>
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="AC15" t="s">
         <v>119</v>
       </c>
       <c r="AD15">
         <f t="shared" ca="1" si="1"/>
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AE15" t="s">
         <v>119</v>
       </c>
       <c r="AF15">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG15" t="s">
         <v>119</v>
@@ -8593,7 +8769,7 @@
       </c>
       <c r="AL15" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman15@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,173,78,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman15@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,184,79,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="16" spans="1:38">
@@ -8685,7 +8861,7 @@
       </c>
       <c r="AD16">
         <f t="shared" ca="1" si="1"/>
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="AE16" t="s">
         <v>119</v>
@@ -8712,7 +8888,7 @@
       </c>
       <c r="AL16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman16@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,185,80,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman16@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,185,71,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="17" spans="1:38">
@@ -8797,21 +8973,21 @@
       </c>
       <c r="AB17">
         <f t="shared" ca="1" si="0"/>
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="AC17" t="s">
         <v>119</v>
       </c>
       <c r="AD17">
         <f t="shared" ca="1" si="1"/>
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="AE17" t="s">
         <v>119</v>
       </c>
       <c r="AF17">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG17" t="s">
         <v>119</v>
@@ -8831,7 +9007,7 @@
       </c>
       <c r="AL17" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman17@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,170,75,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman17@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,180,78,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="20" spans="1:38">
@@ -8975,7 +9151,7 @@
       </c>
       <c r="Q21">
         <f t="shared" ref="Q21:Q22" ca="1" si="6">RANDBETWEEN(0,5)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R21" t="s">
         <v>119</v>
@@ -9009,7 +9185,7 @@
       </c>
       <c r="AB21" t="str">
         <f t="shared" ref="AB21:AB22" ca="1" si="7">_xlfn.CONCAT(A21:AA21)</f>
-        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('답십리FC','답십리FC201018.jpg','성동구','응봉동 구장','blue',2,'2017-01-01',sysdate(),'5678','하나');</v>
+        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('답십리FC','답십리FC201018.jpg','성동구','응봉동 구장','blue',3,'2017-01-01',sysdate(),'5678','하나');</v>
       </c>
     </row>
     <row r="22" spans="1:38">
@@ -9064,7 +9240,7 @@
       </c>
       <c r="Q22">
         <f t="shared" ca="1" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="R22" t="s">
         <v>119</v>
@@ -9098,7 +9274,7 @@
       </c>
       <c r="AB22" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('대구FC','대구FC201018.jpg','달서구','달서구 구장','green',5,'2018-01-01',sysdate(),'2345','기업');</v>
+        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('대구FC','대구FC201018.jpg','달서구','달서구 구장','green',2,'2018-01-01',sysdate(),'2345','기업');</v>
       </c>
     </row>
     <row r="24" spans="1:38">

</xml_diff>

<commit_message>
[2020-12-13 08:09] FE01~FE10, FU01
</commit_message>
<xml_diff>
--- a/docs/srs/fbt_docs.xlsx
+++ b/docs/srs/fbt_docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\kjy\fbt\docs\srs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD2AFA7-D16F-4296-8A33-EE36FD33ED7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E246737D-C3DD-4A2A-84EE-A7DD3F109BB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{2F0AD6B2-A8A2-4F73-BAF4-7193D3382EE1}"/>
+    <workbookView xWindow="6492" yWindow="660" windowWidth="11280" windowHeight="9060" activeTab="1" xr2:uid="{2F0AD6B2-A8A2-4F73-BAF4-7193D3382EE1}"/>
   </bookViews>
   <sheets>
     <sheet name="요구사항명세서" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="변수 코드 북" sheetId="5" r:id="rId4"/>
     <sheet name="TestCase_시나리오" sheetId="2" r:id="rId5"/>
     <sheet name="TestCase_SQL" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'서비스 플로우'!$B$6:$F$22</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1496" uniqueCount="540">
   <si>
     <t>요구사항 정의서</t>
   </si>
@@ -24755,12 +24756,2525 @@
     </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
+  <si>
+    <t>FE02</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>용병찾기 글 검색</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>용병찾기</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>글</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>검색</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>검색</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>조건에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>해당하는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>용병찾기</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>출력</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>FE03</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>용병신청</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>신청팀이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>등록팀에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>용병</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">신청
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>- employ_result</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>등록</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> / status = 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>등록팀에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>알리기</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 개인</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>용병찾기를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">누른다
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2. employ_result</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>등록</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> / status =0 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>처리</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>등록팀에 알리기</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>FE04</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 용병 찾는 중 용병신청글 출력</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">I </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>유저 정보 보기</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 유저 정보, 용병횟수 출력</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>유저</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>정보</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>용병</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">횟수
+3. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+      </rPr>
+      <t>emp_score</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>FE05</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>용병찾기글 삭제</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>해당</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>용병찾기글</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>삭제한다</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. employId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">보냄
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2. employId </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>대응되는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> employ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>삭제
+3. 새로고침</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>용병찾기글 끌어올리기</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>해당</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>용병찾기글</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>등록일자를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>최신화한다</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>FE06</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. employId </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>보냄</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+2. employId </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>대응되는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> employ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">끌올
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">3. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>새로고침</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>FE07</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>용병찾기글 수락</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>신청글에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>대한</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>용병찾기</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수락</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>등록팀에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>알리기</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. empResultStatus = 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>인</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> empResult </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>객체를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>보낸다
+2. 현실에서는 연락처로 입금까지 확인</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+3. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>해당</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>매치</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>신청글의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> empResult_status = 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수정
+4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> 용병</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>에 알리기</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>용병찾기글 거절</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>신청글에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>대한</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>용병찾기</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>거절</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>등록팀에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>알리기</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. empResultStatus = -1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>인</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> empResult </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>객체를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>보낸다
+2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>해당</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>매치</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>신청글의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> empResult_status = -1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수정
+3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>용병에 알리기</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>FE08</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>FE09</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>FE10</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>팀별 용병찾기 실패 글 출력</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>팀별 용병찾기 성공 글 출력</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>팀별 용병 찾는 중 용병신청글</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>해당</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>경기</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일정
+- 해당 글 참여인원 관련 정보</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>용병 관련 정보</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. teamId, status = 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>보내</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>찾는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>중임을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">나타낸다
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>용병</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 찾는 중 조건</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>미마감
+3. 경기일정, 양도 글 정보 출력
+4. 3에 현재인원수와 상태에 대한 정보를 삽입</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+5. 3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>에 용병 관련 정보(용병 점수) 삽입</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>팀별</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>용병 찾기 성공</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>매치글</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">출력
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>해당 경기 일정
+- 해당 글 참여인원 관련 정보
+- 용병 관련 정보</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>팀별</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>용병</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>찾기</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>실패</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>매치글</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">출력
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>해당 경기 일정
+- 해당 글 참여인원 관련 정보
+- 용병 관련 정보</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. teamId, status = 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>보내</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>매치</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>중임을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>나타낸다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>용병찾기</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>실패</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>조건</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>마감</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>목표인원</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>이상</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+3. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>경기일정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>용병찾기</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>글</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>정보</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>출력
+4. 3에 현재인원수와 상태에 대한 정보를 삽입
+5. 3에 용병 관련 정보(용병 점수) 삽입</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. teamId, status = 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>보내</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>매치</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>중임을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>나타낸다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>용병찾기</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>실패</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>조건</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>마감</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>목표인원</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>미만</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+3. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>경기일정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>용병찾기</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>글</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>정보</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>출력
+4. 3에 현재인원수와 상태에 대한 정보를 삽입
+5. 3에 용병 관련 정보(용병 점수) 삽입</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>FU01</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="46">
+  <fonts count="47">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -25070,6 +27584,12 @@
       <family val="2"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="15">
     <fill>
@@ -25335,7 +27855,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -25531,6 +28051,42 @@
     <xf numFmtId="0" fontId="5" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -25571,12 +28127,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -25900,7 +28450,7 @@
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -25918,11 +28468,11 @@
   <sheetData>
     <row r="1" spans="2:11" ht="18" thickBot="1"/>
     <row r="2" spans="2:11" ht="18" thickBot="1">
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="69"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="81"/>
       <c r="G2" s="2" t="s">
         <v>61</v>
       </c>
@@ -25937,10 +28487,10 @@
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="74"/>
+      <c r="D3" s="86"/>
       <c r="G3" s="4" t="s">
         <v>36</v>
       </c>
@@ -25953,10 +28503,10 @@
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="75" t="s">
+      <c r="C4" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="76"/>
+      <c r="D4" s="88"/>
       <c r="G4" s="26" t="s">
         <v>59</v>
       </c>
@@ -25983,50 +28533,50 @@
     </row>
     <row r="7" spans="2:11" ht="18" thickBot="1"/>
     <row r="8" spans="2:11" ht="18" thickBot="1">
-      <c r="B8" s="70" t="s">
+      <c r="B8" s="82" t="s">
         <v>281</v>
       </c>
-      <c r="C8" s="65" t="s">
+      <c r="C8" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="65" t="s">
+      <c r="D8" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="65" t="s">
+      <c r="E8" s="77" t="s">
         <v>279</v>
       </c>
-      <c r="F8" s="65" t="s">
+      <c r="F8" s="77" t="s">
         <v>280</v>
       </c>
-      <c r="G8" s="71" t="s">
+      <c r="G8" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="72"/>
-      <c r="I8" s="65" t="s">
+      <c r="H8" s="84"/>
+      <c r="I8" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="65" t="s">
+      <c r="J8" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="65" t="s">
+      <c r="K8" s="77" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="18" thickBot="1">
-      <c r="B9" s="66"/>
-      <c r="C9" s="66"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="66"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
       <c r="G9" s="8" t="s">
         <v>8</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="66"/>
-      <c r="J9" s="66"/>
-      <c r="K9" s="66"/>
+      <c r="I9" s="78"/>
+      <c r="J9" s="78"/>
+      <c r="K9" s="78"/>
     </row>
     <row r="10" spans="2:11" ht="27" thickBot="1">
       <c r="B10" s="9" t="s">
@@ -27383,10 +29933,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB557C5E-BA25-400E-9AAB-8EC528CCF68C}">
-  <dimension ref="B1:F58"/>
+  <dimension ref="B1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -27400,29 +29950,29 @@
   <sheetData>
     <row r="1" spans="2:6" ht="18" thickBot="1"/>
     <row r="2" spans="2:6" ht="18.600000000000001" thickBot="1">
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="79" t="s">
         <v>296</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="69"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="81"/>
     </row>
     <row r="3" spans="2:6" ht="18" thickBot="1">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="74"/>
+      <c r="D3" s="86"/>
     </row>
     <row r="4" spans="2:6" ht="18" thickBot="1">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="75" t="s">
+      <c r="C4" s="87" t="s">
         <v>288</v>
       </c>
-      <c r="D4" s="76"/>
+      <c r="D4" s="88"/>
     </row>
     <row r="5" spans="2:6" ht="18" thickBot="1"/>
     <row r="6" spans="2:6" ht="18" customHeight="1" thickBot="1">
@@ -28035,7 +30585,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="42" spans="2:6" ht="61.2" thickBot="1">
+    <row r="42" spans="2:6" ht="60.6" thickBot="1">
       <c r="B42" s="64" t="s">
         <v>286</v>
       </c>
@@ -28289,13 +30839,13 @@
       </c>
     </row>
     <row r="57" spans="2:6" ht="63" thickBot="1">
-      <c r="B57" s="80" t="s">
+      <c r="B57" s="65" t="s">
         <v>493</v>
       </c>
-      <c r="C57" s="79" t="s">
+      <c r="C57" s="68" t="s">
         <v>494</v>
       </c>
-      <c r="D57" s="60" t="s">
+      <c r="D57" s="66" t="s">
         <v>495</v>
       </c>
       <c r="E57" s="59" t="s">
@@ -28305,21 +30855,191 @@
         <v>497</v>
       </c>
     </row>
-    <row r="58" spans="2:6" ht="78.599999999999994" thickBot="1">
-      <c r="B58" s="62" t="s">
+    <row r="58" spans="2:6" ht="109.8" thickBot="1">
+      <c r="B58" s="65" t="s">
+        <v>493</v>
+      </c>
+      <c r="C58" s="65" t="s">
+        <v>500</v>
+      </c>
+      <c r="D58" s="67" t="s">
+        <v>501</v>
+      </c>
+      <c r="E58" s="59" t="s">
+        <v>502</v>
+      </c>
+      <c r="F58" s="57" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" ht="47.4" thickBot="1">
+      <c r="B59" s="65" t="s">
+        <v>493</v>
+      </c>
+      <c r="C59" s="65" t="s">
+        <v>503</v>
+      </c>
+      <c r="D59" s="67" t="s">
+        <v>504</v>
+      </c>
+      <c r="E59" s="59" t="s">
+        <v>505</v>
+      </c>
+      <c r="F59" s="57" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" ht="94.2" thickBot="1">
+      <c r="B60" s="65" t="s">
+        <v>493</v>
+      </c>
+      <c r="C60" s="65" t="s">
+        <v>507</v>
+      </c>
+      <c r="D60" s="67" t="s">
+        <v>508</v>
+      </c>
+      <c r="E60" s="59" t="s">
+        <v>533</v>
+      </c>
+      <c r="F60" s="57" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" ht="47.4" thickBot="1">
+      <c r="B61" s="65" t="s">
+        <v>493</v>
+      </c>
+      <c r="C61" s="65" t="s">
+        <v>513</v>
+      </c>
+      <c r="D61" s="60" t="s">
+        <v>514</v>
+      </c>
+      <c r="E61" s="59" t="s">
+        <v>515</v>
+      </c>
+      <c r="F61" s="57" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" ht="43.8" thickBot="1">
+      <c r="B62" s="65" t="s">
+        <v>493</v>
+      </c>
+      <c r="C62" s="65" t="s">
+        <v>519</v>
+      </c>
+      <c r="D62" s="60" t="s">
+        <v>517</v>
+      </c>
+      <c r="E62" s="59" t="s">
+        <v>518</v>
+      </c>
+      <c r="F62" s="57" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" ht="63" thickBot="1">
+      <c r="B63" s="65" t="s">
+        <v>493</v>
+      </c>
+      <c r="C63" s="65" t="s">
+        <v>521</v>
+      </c>
+      <c r="D63" s="60" t="s">
+        <v>522</v>
+      </c>
+      <c r="E63" s="59" t="s">
+        <v>523</v>
+      </c>
+      <c r="F63" s="57" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" ht="47.4" thickBot="1">
+      <c r="B64" s="65" t="s">
+        <v>493</v>
+      </c>
+      <c r="C64" s="65" t="s">
+        <v>528</v>
+      </c>
+      <c r="D64" s="60" t="s">
+        <v>525</v>
+      </c>
+      <c r="E64" s="59" t="s">
+        <v>526</v>
+      </c>
+      <c r="F64" s="57" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" ht="87.6" thickBot="1">
+      <c r="B65" s="65" t="s">
+        <v>493</v>
+      </c>
+      <c r="C65" s="65" t="s">
+        <v>529</v>
+      </c>
+      <c r="D65" s="60" t="s">
+        <v>531</v>
+      </c>
+      <c r="E65" s="59" t="s">
+        <v>536</v>
+      </c>
+      <c r="F65" s="57" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" ht="87.6" thickBot="1">
+      <c r="B66" s="65" t="s">
+        <v>493</v>
+      </c>
+      <c r="C66" s="65" t="s">
+        <v>530</v>
+      </c>
+      <c r="D66" s="60" t="s">
+        <v>532</v>
+      </c>
+      <c r="E66" s="59" t="s">
+        <v>535</v>
+      </c>
+      <c r="F66" s="57" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" ht="78.599999999999994" thickBot="1">
+      <c r="B67" s="62" t="s">
         <v>368</v>
       </c>
-      <c r="C58" s="62" t="s">
+      <c r="C67" s="62" t="s">
         <v>369</v>
       </c>
-      <c r="D58" s="60" t="s">
+      <c r="D67" s="71" t="s">
         <v>370</v>
       </c>
-      <c r="E58" s="59" t="s">
+      <c r="E67" s="73" t="s">
         <v>486</v>
       </c>
-      <c r="F58" s="57" t="s">
+      <c r="F67" s="75" t="s">
         <v>461</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" ht="47.4" thickBot="1">
+      <c r="B68" s="69" t="s">
+        <v>509</v>
+      </c>
+      <c r="C68" s="70" t="s">
+        <v>539</v>
+      </c>
+      <c r="D68" s="72" t="s">
+        <v>510</v>
+      </c>
+      <c r="E68" s="74" t="s">
+        <v>512</v>
+      </c>
+      <c r="F68" s="76" t="s">
+        <v>511</v>
       </c>
     </row>
   </sheetData>
@@ -28339,7 +31059,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B24355E-CC1D-4763-8BDC-A7AD2ECA21E3}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -28588,7 +31308,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="89" t="s">
         <v>257</v>
       </c>
       <c r="B1">
@@ -28599,7 +31319,7 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="77"/>
+      <c r="A2" s="89"/>
       <c r="B2">
         <v>1</v>
       </c>
@@ -28608,7 +31328,7 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="77"/>
+      <c r="A3" s="89"/>
       <c r="B3">
         <v>2</v>
       </c>
@@ -28617,7 +31337,7 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="90" t="s">
         <v>261</v>
       </c>
       <c r="B4">
@@ -28628,7 +31348,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="78"/>
+      <c r="A5" s="90"/>
       <c r="B5">
         <v>1</v>
       </c>
@@ -28637,7 +31357,7 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="78"/>
+      <c r="A6" s="90"/>
       <c r="B6">
         <v>-1</v>
       </c>
@@ -28646,7 +31366,7 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="77" t="s">
+      <c r="A7" s="89" t="s">
         <v>266</v>
       </c>
       <c r="B7">
@@ -28657,7 +31377,7 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="77"/>
+      <c r="A8" s="89"/>
       <c r="B8">
         <v>1</v>
       </c>
@@ -28666,7 +31386,7 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="77"/>
+      <c r="A9" s="89"/>
       <c r="B9">
         <v>2</v>
       </c>
@@ -28690,7 +31410,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -28824,7 +31544,7 @@
       </c>
       <c r="AB1">
         <f ca="1">RANDBETWEEN(170,185)</f>
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AC1" t="s">
         <v>110</v>
@@ -28838,7 +31558,7 @@
       </c>
       <c r="AF1">
         <f ca="1">RANDBETWEEN(0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG1" t="s">
         <v>110</v>
@@ -28858,7 +31578,7 @@
       </c>
       <c r="AL1" t="str">
         <f ca="1">_xlfn.CONCAT(A1:AK1)</f>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman1@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,176,70,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman1@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,174,70,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="2" spans="1:38">
@@ -28943,28 +31663,28 @@
       </c>
       <c r="AB2">
         <f t="shared" ref="AB2:AB17" ca="1" si="0">RANDBETWEEN(170,185)</f>
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="AC2" t="s">
         <v>110</v>
       </c>
       <c r="AD2">
         <f t="shared" ref="AD2:AD17" ca="1" si="1">RANDBETWEEN(70,80)</f>
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="AE2" t="s">
         <v>110</v>
       </c>
       <c r="AF2">
         <f t="shared" ref="AF2:AF17" ca="1" si="2">RANDBETWEEN(0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG2" t="s">
         <v>110</v>
       </c>
       <c r="AH2">
         <f t="shared" ref="AH2:AH17" ca="1" si="3">RANDBETWEEN(0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI2" t="s">
         <v>110</v>
@@ -28977,7 +31697,7 @@
       </c>
       <c r="AL2" t="str">
         <f t="shared" ref="AL2:AL17" ca="1" si="4">_xlfn.CONCAT(A2:AK2)</f>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman2@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,176,79,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman2@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,172,76,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="3" spans="1:38">
@@ -29069,14 +31789,14 @@
       </c>
       <c r="AD3">
         <f t="shared" ca="1" si="1"/>
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="AE3" t="s">
         <v>110</v>
       </c>
       <c r="AF3">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG3" t="s">
         <v>110</v>
@@ -29096,7 +31816,7 @@
       </c>
       <c r="AL3" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman3@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,184,72,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman3@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,184,77,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="4" spans="1:38">
@@ -29181,7 +31901,7 @@
       </c>
       <c r="AB4">
         <f t="shared" ca="1" si="0"/>
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="AC4" t="s">
         <v>110</v>
@@ -29195,14 +31915,14 @@
       </c>
       <c r="AF4">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG4" t="s">
         <v>110</v>
       </c>
       <c r="AH4">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI4" t="s">
         <v>110</v>
@@ -29215,7 +31935,7 @@
       </c>
       <c r="AL4" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman4@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,173,77,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman4@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,174,77,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="5" spans="1:38">
@@ -29300,14 +32020,14 @@
       </c>
       <c r="AB5">
         <f t="shared" ca="1" si="0"/>
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="AC5" t="s">
         <v>110</v>
       </c>
       <c r="AD5">
         <f t="shared" ca="1" si="1"/>
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AE5" t="s">
         <v>110</v>
@@ -29321,7 +32041,7 @@
       </c>
       <c r="AH5">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI5" t="s">
         <v>110</v>
@@ -29334,7 +32054,7 @@
       </c>
       <c r="AL5" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman5@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,179,72,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman5@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,176,71,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="6" spans="1:38">
@@ -29419,28 +32139,28 @@
       </c>
       <c r="AB6">
         <f t="shared" ca="1" si="0"/>
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="AC6" t="s">
         <v>110</v>
       </c>
       <c r="AD6">
         <f t="shared" ca="1" si="1"/>
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AE6" t="s">
         <v>110</v>
       </c>
       <c r="AF6">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG6" t="s">
         <v>110</v>
       </c>
       <c r="AH6">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI6" t="s">
         <v>110</v>
@@ -29453,7 +32173,7 @@
       </c>
       <c r="AL6" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman6@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,177,70,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman6@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,174,71,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="7" spans="1:38">
@@ -29538,21 +32258,21 @@
       </c>
       <c r="AB7">
         <f t="shared" ca="1" si="0"/>
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AC7" t="s">
         <v>110</v>
       </c>
       <c r="AD7">
         <f t="shared" ca="1" si="1"/>
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AE7" t="s">
         <v>110</v>
       </c>
       <c r="AF7">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG7" t="s">
         <v>110</v>
@@ -29572,7 +32292,7 @@
       </c>
       <c r="AL7" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman7@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,176,72,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman7@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,179,73,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="8" spans="1:38">
@@ -29657,14 +32377,14 @@
       </c>
       <c r="AB8">
         <f t="shared" ca="1" si="0"/>
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="AC8" t="s">
         <v>110</v>
       </c>
       <c r="AD8">
         <f t="shared" ca="1" si="1"/>
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AE8" t="s">
         <v>110</v>
@@ -29678,7 +32398,7 @@
       </c>
       <c r="AH8">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI8" t="s">
         <v>110</v>
@@ -29691,7 +32411,7 @@
       </c>
       <c r="AL8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman8@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,173,77,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman8@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,178,75,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="9" spans="1:38">
@@ -29776,28 +32496,28 @@
       </c>
       <c r="AB9">
         <f t="shared" ca="1" si="0"/>
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="AC9" t="s">
         <v>110</v>
       </c>
       <c r="AD9">
         <f t="shared" ca="1" si="1"/>
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="AE9" t="s">
         <v>110</v>
       </c>
       <c r="AF9">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG9" t="s">
         <v>110</v>
       </c>
       <c r="AH9">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI9" t="s">
         <v>110</v>
@@ -29810,7 +32530,7 @@
       </c>
       <c r="AL9" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman9@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,170,71,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman9@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,180,77,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="10" spans="1:38">
@@ -29895,7 +32615,7 @@
       </c>
       <c r="AB10">
         <f t="shared" ca="1" si="0"/>
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AC10" t="s">
         <v>110</v>
@@ -29909,7 +32629,7 @@
       </c>
       <c r="AF10">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG10" t="s">
         <v>110</v>
@@ -29929,7 +32649,7 @@
       </c>
       <c r="AL10" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman10@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,176,78,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman10@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,170,78,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="11" spans="1:38">
@@ -30014,28 +32734,28 @@
       </c>
       <c r="AB11">
         <f t="shared" ca="1" si="0"/>
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="AC11" t="s">
         <v>110</v>
       </c>
       <c r="AD11">
         <f t="shared" ca="1" si="1"/>
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="AE11" t="s">
         <v>110</v>
       </c>
       <c r="AF11">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG11" t="s">
         <v>110</v>
       </c>
       <c r="AH11">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI11" t="s">
         <v>110</v>
@@ -30048,7 +32768,7 @@
       </c>
       <c r="AL11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman11@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,178,71,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman11@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,172,74,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="12" spans="1:38">
@@ -30133,14 +32853,14 @@
       </c>
       <c r="AB12">
         <f t="shared" ca="1" si="0"/>
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="AC12" t="s">
         <v>110</v>
       </c>
       <c r="AD12">
         <f t="shared" ca="1" si="1"/>
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="AE12" t="s">
         <v>110</v>
@@ -30154,7 +32874,7 @@
       </c>
       <c r="AH12">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI12" t="s">
         <v>110</v>
@@ -30167,7 +32887,7 @@
       </c>
       <c r="AL12" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman12@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,179,70,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman12@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,184,72,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="13" spans="1:38">
@@ -30252,21 +32972,21 @@
       </c>
       <c r="AB13">
         <f t="shared" ca="1" si="0"/>
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="AC13" t="s">
         <v>110</v>
       </c>
       <c r="AD13">
         <f t="shared" ca="1" si="1"/>
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="AE13" t="s">
         <v>110</v>
       </c>
       <c r="AF13">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG13" t="s">
         <v>110</v>
@@ -30286,7 +33006,7 @@
       </c>
       <c r="AL13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman13@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,177,73,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman13@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,173,79,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="14" spans="1:38">
@@ -30371,21 +33091,21 @@
       </c>
       <c r="AB14">
         <f t="shared" ca="1" si="0"/>
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="AC14" t="s">
         <v>110</v>
       </c>
       <c r="AD14">
         <f t="shared" ca="1" si="1"/>
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AE14" t="s">
         <v>110</v>
       </c>
       <c r="AF14">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG14" t="s">
         <v>110</v>
@@ -30405,7 +33125,7 @@
       </c>
       <c r="AL14" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman14@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,179,75,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman14@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,173,73,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="15" spans="1:38">
@@ -30490,28 +33210,28 @@
       </c>
       <c r="AB15">
         <f t="shared" ca="1" si="0"/>
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="AC15" t="s">
         <v>110</v>
       </c>
       <c r="AD15">
         <f t="shared" ca="1" si="1"/>
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AE15" t="s">
         <v>110</v>
       </c>
       <c r="AF15">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG15" t="s">
         <v>110</v>
       </c>
       <c r="AH15">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI15" t="s">
         <v>110</v>
@@ -30524,7 +33244,7 @@
       </c>
       <c r="AL15" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman15@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,177,79,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman15@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,171,78,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="16" spans="1:38">
@@ -30609,14 +33329,14 @@
       </c>
       <c r="AB16">
         <f t="shared" ca="1" si="0"/>
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AC16" t="s">
         <v>110</v>
       </c>
       <c r="AD16">
         <f t="shared" ca="1" si="1"/>
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="AE16" t="s">
         <v>110</v>
@@ -30630,7 +33350,7 @@
       </c>
       <c r="AH16">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI16" t="s">
         <v>110</v>
@@ -30643,7 +33363,7 @@
       </c>
       <c r="AL16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman16@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,180,77,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman16@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,177,72,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="17" spans="1:38">
@@ -30742,14 +33462,14 @@
       </c>
       <c r="AF17">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG17" t="s">
         <v>110</v>
       </c>
       <c r="AH17">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI17" t="s">
         <v>110</v>
@@ -30762,7 +33482,7 @@
       </c>
       <c r="AL17" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman17@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,176,79,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman17@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,176,79,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="20" spans="1:38">
@@ -30817,7 +33537,7 @@
       </c>
       <c r="Q20">
         <f ca="1">RANDBETWEEN(0,5)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R20" t="s">
         <v>110</v>
@@ -30851,7 +33571,7 @@
       </c>
       <c r="AB20" t="str">
         <f ca="1">_xlfn.CONCAT(A20:AA20)</f>
-        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('왕십리FC','왕십리FC201018.jpg','성동구','성동구 구장','red',2,'2016-01-01',sysdate(),'1234','기업');</v>
+        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('왕십리FC','왕십리FC201018.jpg','성동구','성동구 구장','red',4,'2016-01-01',sysdate(),'1234','기업');</v>
       </c>
     </row>
     <row r="21" spans="1:38">
@@ -30906,7 +33626,7 @@
       </c>
       <c r="Q21">
         <f t="shared" ref="Q21:Q22" ca="1" si="6">RANDBETWEEN(0,5)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R21" t="s">
         <v>110</v>
@@ -30940,7 +33660,7 @@
       </c>
       <c r="AB21" t="str">
         <f t="shared" ref="AB21:AB22" ca="1" si="7">_xlfn.CONCAT(A21:AA21)</f>
-        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('답십리FC','답십리FC201018.jpg','성동구','응봉동 구장','blue',0,'2017-01-01',sysdate(),'5678','하나');</v>
+        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('답십리FC','답십리FC201018.jpg','성동구','응봉동 구장','blue',3,'2017-01-01',sysdate(),'5678','하나');</v>
       </c>
     </row>
     <row r="22" spans="1:38">
@@ -30995,7 +33715,7 @@
       </c>
       <c r="Q22">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R22" t="s">
         <v>110</v>
@@ -31029,7 +33749,7 @@
       </c>
       <c r="AB22" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('대구FC','대구FC201018.jpg','달서구','달서구 구장','green',0,'2018-01-01',sysdate(),'2345','기업');</v>
+        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('대구FC','대구FC201018.jpg','달서구','달서구 구장','green',4,'2018-01-01',sysdate(),'2345','기업');</v>
       </c>
     </row>
     <row r="24" spans="1:38">
@@ -31881,4 +34601,183 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4CA4EE-DE18-469F-A352-6DA033B77CCB}">
+  <dimension ref="A1:L6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1">
+        <f>AVERAGE(B1:XFD1)</f>
+        <v>8.1818181818181817</v>
+      </c>
+      <c r="B1">
+        <v>7</v>
+      </c>
+      <c r="C1">
+        <v>7</v>
+      </c>
+      <c r="D1">
+        <v>9</v>
+      </c>
+      <c r="E1">
+        <v>7</v>
+      </c>
+      <c r="F1">
+        <v>8</v>
+      </c>
+      <c r="G1">
+        <v>9</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>10</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2">
+        <f t="shared" ref="A2:A6" si="0">AVERAGE(B2:XFD2)</f>
+        <v>8.3636363636363633</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <v>8</v>
+      </c>
+      <c r="H2">
+        <v>9</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>8</v>
+      </c>
+      <c r="K2">
+        <v>7</v>
+      </c>
+      <c r="L2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3">
+        <f t="shared" si="0"/>
+        <v>8.545454545454545</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>9</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>8</v>
+      </c>
+      <c r="H3">
+        <v>9</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3">
+        <v>9</v>
+      </c>
+      <c r="K3">
+        <v>7</v>
+      </c>
+      <c r="L3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4">
+        <f t="shared" si="0"/>
+        <v>7.666666666666667</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="B6">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[2020-12-13 20:35] FE11 ~ FE14
</commit_message>
<xml_diff>
--- a/docs/srs/fbt_docs.xlsx
+++ b/docs/srs/fbt_docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\kjy\fbt\docs\srs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E246737D-C3DD-4A2A-84EE-A7DD3F109BB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E04A18-E628-4A29-A634-F8863311F0E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6492" yWindow="660" windowWidth="11280" windowHeight="9060" activeTab="1" xr2:uid="{2F0AD6B2-A8A2-4F73-BAF4-7193D3382EE1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{2F0AD6B2-A8A2-4F73-BAF4-7193D3382EE1}"/>
   </bookViews>
   <sheets>
     <sheet name="요구사항명세서" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1496" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1516" uniqueCount="554">
   <si>
     <t>요구사항 정의서</t>
   </si>
@@ -23318,419 +23318,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>경기</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>투표</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>수정</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>버튼의</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">조건
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>매치 중 단계일 때만</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">2. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>클릭</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>시</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>수정페이지로</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">넘어간다
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- props: assign </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>객체</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">전부
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">3. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>사용자가</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>수정</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>후</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>수정</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>완료</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>버튼을</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>누르면</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> search </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>객체를</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve"> 서버로 넘겨 수정한다
-4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Nanum Gothic"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>매치</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>등록</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>현황 페이지로 이동한다.</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>FA15</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -26318,156 +25905,6 @@
   </si>
   <si>
     <r>
-      <t>1. teamId, status = 0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>로</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>보내</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>찾는</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>중임을</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">나타낸다
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">2. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>용병</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve"> 찾는 중 조건</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Nanum Gothic"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">
-- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>미마감
-3. 경기일정, 양도 글 정보 출력
-4. 3에 현재인원수와 상태에 대한 정보를 삽입</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Nanum Gothic"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">
-5. 3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>에 용병 관련 정보(용병 점수) 삽입</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">1. </t>
     </r>
     <r>
@@ -26696,8 +26133,166 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>1. teamId, status = 2</t>
+    <t>FU01</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. teamId, status = 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>보내</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>찾는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>중임을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">나타낸다
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>용병</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 찾는 중 조건</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>미마감 + 수락인원 &lt; 목표인원(미완료)
+3. 경기일정, 양도 글 정보 출력
+4. 3에 현재인원수와 상태에 대한 정보를 삽입</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+5. 3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>에 용병 관련 정보(용병 점수) 삽입</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>FE11</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. email, status = 2</t>
     </r>
     <r>
       <rPr>
@@ -26850,15 +26445,16 @@
         <family val="3"/>
         <charset val="129"/>
       </rPr>
-      <t>마감</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> + </t>
+      <t>수락인원</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> &gt;= </t>
     </r>
     <r>
       <rPr>
@@ -26868,24 +26464,6 @@
         <charset val="129"/>
       </rPr>
       <t>목표인원</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Nanum Gothic"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>이상</t>
     </r>
     <r>
       <rPr>
@@ -26982,7 +26560,7 @@
   </si>
   <si>
     <r>
-      <t>1. teamId, status = 1</t>
+      <t>1. email, status = 1</t>
     </r>
     <r>
       <rPr>
@@ -27152,7 +26730,7 @@
         <family val="3"/>
         <charset val="129"/>
       </rPr>
-      <t>목표인원</t>
+      <t>수락인원</t>
     </r>
     <r>
       <rPr>
@@ -27161,25 +26739,25 @@
         <family val="2"/>
         <charset val="129"/>
       </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>미만</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-3. </t>
+      <t xml:space="preserve"> &lt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">목표인원
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">3. </t>
     </r>
     <r>
       <rPr>
@@ -27266,7 +26844,1383 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>FU01</t>
+    <t>FE12</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>용병 신청 단계별 출력</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>팀별</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>용병신청</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 단계별</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>출력</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>해당</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>경기</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일정</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>용병신청 취소</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 용병</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>신청한</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>것</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>취소</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. email, employId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">보냄
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>해당하는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 용병</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 신청</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">삭제
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">3. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>새로고침</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. email, empResultStatus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>보냄</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>신청</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">조건
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">- empResultStatus = 0 + 미마감: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>신청</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+- -1: 실패
+- 1: 성공</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>3.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>경기일정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>매치글</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>정보 출력
+4. 신청 팀 정보 출력하여 3에 삽입</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>FE13</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. FE12</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>FE14</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>용병찾기 수정</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 용병찾기글 수정</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>경기</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>투표</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>버튼의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">조건
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>양도 중 단계일 때만</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>클릭</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>시</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수정페이지로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">넘어간다
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">- props: assign </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>객체</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">전부
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">3. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>사용자가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>후</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>완료</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>버튼을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>누르면</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> search </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>객체를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> 서버로 넘겨 수정한다
+4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>양도</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>등록</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>현황 페이지로 이동한다.</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>경기</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>투표</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>버튼의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>조건</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+- 용병찾기 중 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>단계일</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>때만</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>클릭</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>시</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수정페이지로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>넘어간다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+- props: employ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>객체</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>전부</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+3. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>사용자가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>후</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>완료</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>버튼을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>누르면</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> employ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>객체를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>서버로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>넘겨</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수정한다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+4. 용병찾기 중 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>페이지로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>이동한다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Nanum Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>.</t>
+    </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -29933,10 +30887,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB557C5E-BA25-400E-9AAB-8EC528CCF68C}">
-  <dimension ref="B1:F68"/>
+  <dimension ref="B1:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -30295,7 +31249,7 @@
         <v>362</v>
       </c>
       <c r="F24" s="57" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="109.8" thickBot="1">
@@ -30599,7 +31553,7 @@
         <v>438</v>
       </c>
       <c r="F42" s="57" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="43" spans="2:6" ht="125.4" thickBot="1">
@@ -30828,45 +31782,45 @@
         <v>286</v>
       </c>
       <c r="C56" s="64" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D56" s="60" t="s">
         <v>490</v>
       </c>
       <c r="E56" s="59"/>
       <c r="F56" s="57" t="s">
-        <v>491</v>
+        <v>552</v>
       </c>
     </row>
     <row r="57" spans="2:6" ht="63" thickBot="1">
       <c r="B57" s="65" t="s">
+        <v>492</v>
+      </c>
+      <c r="C57" s="68" t="s">
         <v>493</v>
       </c>
-      <c r="C57" s="68" t="s">
+      <c r="D57" s="66" t="s">
         <v>494</v>
       </c>
-      <c r="D57" s="66" t="s">
+      <c r="E57" s="59" t="s">
         <v>495</v>
       </c>
-      <c r="E57" s="59" t="s">
+      <c r="F57" s="57" t="s">
         <v>496</v>
-      </c>
-      <c r="F57" s="57" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="58" spans="2:6" ht="109.8" thickBot="1">
       <c r="B58" s="65" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C58" s="65" t="s">
+        <v>499</v>
+      </c>
+      <c r="D58" s="67" t="s">
         <v>500</v>
       </c>
-      <c r="D58" s="67" t="s">
+      <c r="E58" s="59" t="s">
         <v>501</v>
-      </c>
-      <c r="E58" s="59" t="s">
-        <v>502</v>
       </c>
       <c r="F58" s="57" t="s">
         <v>365</v>
@@ -30874,172 +31828,240 @@
     </row>
     <row r="59" spans="2:6" ht="47.4" thickBot="1">
       <c r="B59" s="65" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C59" s="65" t="s">
+        <v>502</v>
+      </c>
+      <c r="D59" s="67" t="s">
         <v>503</v>
       </c>
-      <c r="D59" s="67" t="s">
+      <c r="E59" s="59" t="s">
         <v>504</v>
       </c>
-      <c r="E59" s="59" t="s">
+      <c r="F59" s="57" t="s">
         <v>505</v>
-      </c>
-      <c r="F59" s="57" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="60" spans="2:6" ht="94.2" thickBot="1">
       <c r="B60" s="65" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C60" s="65" t="s">
+        <v>506</v>
+      </c>
+      <c r="D60" s="67" t="s">
         <v>507</v>
       </c>
-      <c r="D60" s="67" t="s">
-        <v>508</v>
-      </c>
       <c r="E60" s="59" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="F60" s="57" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
     </row>
     <row r="61" spans="2:6" ht="47.4" thickBot="1">
       <c r="B61" s="65" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C61" s="65" t="s">
+        <v>512</v>
+      </c>
+      <c r="D61" s="60" t="s">
         <v>513</v>
       </c>
-      <c r="D61" s="60" t="s">
+      <c r="E61" s="59" t="s">
         <v>514</v>
       </c>
-      <c r="E61" s="59" t="s">
+      <c r="F61" s="57" t="s">
         <v>515</v>
-      </c>
-      <c r="F61" s="57" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="62" spans="2:6" ht="43.8" thickBot="1">
       <c r="B62" s="65" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C62" s="65" t="s">
+        <v>518</v>
+      </c>
+      <c r="D62" s="60" t="s">
+        <v>516</v>
+      </c>
+      <c r="E62" s="59" t="s">
+        <v>517</v>
+      </c>
+      <c r="F62" s="57" t="s">
         <v>519</v>
-      </c>
-      <c r="D62" s="60" t="s">
-        <v>517</v>
-      </c>
-      <c r="E62" s="59" t="s">
-        <v>518</v>
-      </c>
-      <c r="F62" s="57" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="63" spans="2:6" ht="63" thickBot="1">
       <c r="B63" s="65" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C63" s="65" t="s">
+        <v>520</v>
+      </c>
+      <c r="D63" s="60" t="s">
         <v>521</v>
       </c>
-      <c r="D63" s="60" t="s">
+      <c r="E63" s="59" t="s">
         <v>522</v>
       </c>
-      <c r="E63" s="59" t="s">
+      <c r="F63" s="57" t="s">
         <v>523</v>
-      </c>
-      <c r="F63" s="57" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="64" spans="2:6" ht="47.4" thickBot="1">
       <c r="B64" s="65" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C64" s="65" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D64" s="60" t="s">
+        <v>524</v>
+      </c>
+      <c r="E64" s="59" t="s">
         <v>525</v>
       </c>
-      <c r="E64" s="59" t="s">
+      <c r="F64" s="57" t="s">
         <v>526</v>
-      </c>
-      <c r="F64" s="57" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="65" spans="2:6" ht="87.6" thickBot="1">
       <c r="B65" s="65" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C65" s="65" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D65" s="60" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E65" s="59" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="F65" s="57" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="66" spans="2:6" ht="87.6" thickBot="1">
       <c r="B66" s="65" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C66" s="65" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D66" s="60" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E66" s="59" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="F66" s="57" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" ht="109.8" thickBot="1">
+      <c r="B67" s="65" t="s">
+        <v>492</v>
+      </c>
+      <c r="C67" s="65" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="67" spans="2:6" ht="78.599999999999994" thickBot="1">
-      <c r="B67" s="62" t="s">
-        <v>368</v>
-      </c>
-      <c r="C67" s="62" t="s">
-        <v>369</v>
-      </c>
-      <c r="D67" s="71" t="s">
-        <v>370</v>
-      </c>
-      <c r="E67" s="73" t="s">
-        <v>486</v>
-      </c>
-      <c r="F67" s="75" t="s">
-        <v>461</v>
+      <c r="D67" s="60" t="s">
+        <v>541</v>
+      </c>
+      <c r="E67" s="59" t="s">
+        <v>542</v>
+      </c>
+      <c r="F67" s="57" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="68" spans="2:6" ht="47.4" thickBot="1">
-      <c r="B68" s="69" t="s">
+      <c r="B68" s="65" t="s">
+        <v>492</v>
+      </c>
+      <c r="C68" s="65" t="s">
+        <v>540</v>
+      </c>
+      <c r="D68" s="60" t="s">
+        <v>543</v>
+      </c>
+      <c r="E68" s="59" t="s">
+        <v>544</v>
+      </c>
+      <c r="F68" s="57" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" ht="18" thickBot="1">
+      <c r="B69" s="65" t="s">
+        <v>492</v>
+      </c>
+      <c r="C69" s="65" t="s">
+        <v>547</v>
+      </c>
+      <c r="D69" s="60" t="s">
+        <v>471</v>
+      </c>
+      <c r="E69" s="59" t="s">
+        <v>544</v>
+      </c>
+      <c r="F69" s="57" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" ht="109.8" thickBot="1">
+      <c r="B70" s="65" t="s">
+        <v>492</v>
+      </c>
+      <c r="C70" s="65" t="s">
+        <v>549</v>
+      </c>
+      <c r="D70" s="60" t="s">
+        <v>550</v>
+      </c>
+      <c r="E70" s="59" t="s">
+        <v>551</v>
+      </c>
+      <c r="F70" s="57" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" ht="78.599999999999994" thickBot="1">
+      <c r="B71" s="62" t="s">
+        <v>368</v>
+      </c>
+      <c r="C71" s="62" t="s">
+        <v>369</v>
+      </c>
+      <c r="D71" s="71" t="s">
+        <v>370</v>
+      </c>
+      <c r="E71" s="73" t="s">
+        <v>486</v>
+      </c>
+      <c r="F71" s="75" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" ht="47.4" thickBot="1">
+      <c r="B72" s="69" t="s">
+        <v>508</v>
+      </c>
+      <c r="C72" s="70" t="s">
+        <v>535</v>
+      </c>
+      <c r="D72" s="72" t="s">
         <v>509</v>
       </c>
-      <c r="C68" s="70" t="s">
-        <v>539</v>
-      </c>
-      <c r="D68" s="72" t="s">
+      <c r="E72" s="74" t="s">
+        <v>511</v>
+      </c>
+      <c r="F72" s="76" t="s">
         <v>510</v>
-      </c>
-      <c r="E68" s="74" t="s">
-        <v>512</v>
-      </c>
-      <c r="F68" s="76" t="s">
-        <v>511</v>
       </c>
     </row>
   </sheetData>
@@ -31544,21 +32566,21 @@
       </c>
       <c r="AB1">
         <f ca="1">RANDBETWEEN(170,185)</f>
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="AC1" t="s">
         <v>110</v>
       </c>
       <c r="AD1">
         <f ca="1">RANDBETWEEN(70,80)</f>
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="AE1" t="s">
         <v>110</v>
       </c>
       <c r="AF1">
         <f ca="1">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG1" t="s">
         <v>110</v>
@@ -31578,7 +32600,7 @@
       </c>
       <c r="AL1" t="str">
         <f ca="1">_xlfn.CONCAT(A1:AK1)</f>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman1@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,174,70,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman1@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,171,79,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="2" spans="1:38">
@@ -31663,7 +32685,7 @@
       </c>
       <c r="AB2">
         <f t="shared" ref="AB2:AB17" ca="1" si="0">RANDBETWEEN(170,185)</f>
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="AC2" t="s">
         <v>110</v>
@@ -31684,7 +32706,7 @@
       </c>
       <c r="AH2">
         <f t="shared" ref="AH2:AH17" ca="1" si="3">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI2" t="s">
         <v>110</v>
@@ -31697,7 +32719,7 @@
       </c>
       <c r="AL2" t="str">
         <f t="shared" ref="AL2:AL17" ca="1" si="4">_xlfn.CONCAT(A2:AK2)</f>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman2@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,172,76,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman2@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,179,76,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="3" spans="1:38">
@@ -31782,21 +32804,21 @@
       </c>
       <c r="AB3">
         <f t="shared" ca="1" si="0"/>
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="AC3" t="s">
         <v>110</v>
       </c>
       <c r="AD3">
         <f t="shared" ca="1" si="1"/>
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AE3" t="s">
         <v>110</v>
       </c>
       <c r="AF3">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG3" t="s">
         <v>110</v>
@@ -31816,7 +32838,7 @@
       </c>
       <c r="AL3" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman3@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,184,77,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman3@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,171,75,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="4" spans="1:38">
@@ -31901,21 +32923,21 @@
       </c>
       <c r="AB4">
         <f t="shared" ca="1" si="0"/>
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="AC4" t="s">
         <v>110</v>
       </c>
       <c r="AD4">
         <f t="shared" ca="1" si="1"/>
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AE4" t="s">
         <v>110</v>
       </c>
       <c r="AF4">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG4" t="s">
         <v>110</v>
@@ -31935,7 +32957,7 @@
       </c>
       <c r="AL4" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman4@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,174,77,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman4@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,171,76,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="5" spans="1:38">
@@ -32020,28 +33042,28 @@
       </c>
       <c r="AB5">
         <f t="shared" ca="1" si="0"/>
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="AC5" t="s">
         <v>110</v>
       </c>
       <c r="AD5">
         <f t="shared" ca="1" si="1"/>
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="AE5" t="s">
         <v>110</v>
       </c>
       <c r="AF5">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG5" t="s">
         <v>110</v>
       </c>
       <c r="AH5">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI5" t="s">
         <v>110</v>
@@ -32054,7 +33076,7 @@
       </c>
       <c r="AL5" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman5@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,176,71,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman5@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,184,78,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="6" spans="1:38">
@@ -32139,21 +33161,21 @@
       </c>
       <c r="AB6">
         <f t="shared" ca="1" si="0"/>
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="AC6" t="s">
         <v>110</v>
       </c>
       <c r="AD6">
         <f t="shared" ca="1" si="1"/>
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="AE6" t="s">
         <v>110</v>
       </c>
       <c r="AF6">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG6" t="s">
         <v>110</v>
@@ -32173,7 +33195,7 @@
       </c>
       <c r="AL6" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman6@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,174,71,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman6@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,179,75,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="7" spans="1:38">
@@ -32258,21 +33280,21 @@
       </c>
       <c r="AB7">
         <f t="shared" ca="1" si="0"/>
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="AC7" t="s">
         <v>110</v>
       </c>
       <c r="AD7">
         <f t="shared" ca="1" si="1"/>
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="AE7" t="s">
         <v>110</v>
       </c>
       <c r="AF7">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG7" t="s">
         <v>110</v>
@@ -32292,7 +33314,7 @@
       </c>
       <c r="AL7" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman7@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,179,73,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman7@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,184,79,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="8" spans="1:38">
@@ -32377,14 +33399,14 @@
       </c>
       <c r="AB8">
         <f t="shared" ca="1" si="0"/>
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="AC8" t="s">
         <v>110</v>
       </c>
       <c r="AD8">
         <f t="shared" ca="1" si="1"/>
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="AE8" t="s">
         <v>110</v>
@@ -32411,7 +33433,7 @@
       </c>
       <c r="AL8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman8@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,178,75,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman8@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,180,78,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="9" spans="1:38">
@@ -32496,14 +33518,14 @@
       </c>
       <c r="AB9">
         <f t="shared" ca="1" si="0"/>
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="AC9" t="s">
         <v>110</v>
       </c>
       <c r="AD9">
         <f t="shared" ca="1" si="1"/>
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AE9" t="s">
         <v>110</v>
@@ -32517,7 +33539,7 @@
       </c>
       <c r="AH9">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI9" t="s">
         <v>110</v>
@@ -32530,7 +33552,7 @@
       </c>
       <c r="AL9" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman9@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,180,77,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman9@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,175,75,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="10" spans="1:38">
@@ -32615,7 +33637,7 @@
       </c>
       <c r="AB10">
         <f t="shared" ca="1" si="0"/>
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="AC10" t="s">
         <v>110</v>
@@ -32629,14 +33651,14 @@
       </c>
       <c r="AF10">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG10" t="s">
         <v>110</v>
       </c>
       <c r="AH10">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI10" t="s">
         <v>110</v>
@@ -32649,7 +33671,7 @@
       </c>
       <c r="AL10" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman10@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,170,78,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman10@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,179,78,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="11" spans="1:38">
@@ -32748,14 +33770,14 @@
       </c>
       <c r="AF11">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG11" t="s">
         <v>110</v>
       </c>
       <c r="AH11">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI11" t="s">
         <v>110</v>
@@ -32768,7 +33790,7 @@
       </c>
       <c r="AL11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman11@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,172,74,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman11@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,172,74,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="12" spans="1:38">
@@ -32853,14 +33875,14 @@
       </c>
       <c r="AB12">
         <f t="shared" ca="1" si="0"/>
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="AC12" t="s">
         <v>110</v>
       </c>
       <c r="AD12">
         <f t="shared" ca="1" si="1"/>
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AE12" t="s">
         <v>110</v>
@@ -32887,7 +33909,7 @@
       </c>
       <c r="AL12" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman12@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,184,72,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman12@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,174,70,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="13" spans="1:38">
@@ -32972,7 +33994,7 @@
       </c>
       <c r="AB13">
         <f t="shared" ca="1" si="0"/>
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="AC13" t="s">
         <v>110</v>
@@ -33006,7 +34028,7 @@
       </c>
       <c r="AL13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman13@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,173,79,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman13@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,177,79,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="14" spans="1:38">
@@ -33091,7 +34113,7 @@
       </c>
       <c r="AB14">
         <f t="shared" ca="1" si="0"/>
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="AC14" t="s">
         <v>110</v>
@@ -33125,7 +34147,7 @@
       </c>
       <c r="AL14" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman14@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,173,73,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman14@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,182,73,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="15" spans="1:38">
@@ -33210,28 +34232,28 @@
       </c>
       <c r="AB15">
         <f t="shared" ca="1" si="0"/>
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="AC15" t="s">
         <v>110</v>
       </c>
       <c r="AD15">
         <f t="shared" ca="1" si="1"/>
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="AE15" t="s">
         <v>110</v>
       </c>
       <c r="AF15">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG15" t="s">
         <v>110</v>
       </c>
       <c r="AH15">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI15" t="s">
         <v>110</v>
@@ -33244,7 +34266,7 @@
       </c>
       <c r="AL15" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman15@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,171,78,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman15@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,176,73,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="16" spans="1:38">
@@ -33329,14 +34351,14 @@
       </c>
       <c r="AB16">
         <f t="shared" ca="1" si="0"/>
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="AC16" t="s">
         <v>110</v>
       </c>
       <c r="AD16">
         <f t="shared" ca="1" si="1"/>
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="AE16" t="s">
         <v>110</v>
@@ -33350,7 +34372,7 @@
       </c>
       <c r="AH16">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI16" t="s">
         <v>110</v>
@@ -33363,7 +34385,7 @@
       </c>
       <c r="AL16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman16@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,177,72,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman16@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,181,74,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="17" spans="1:38">
@@ -33448,28 +34470,28 @@
       </c>
       <c r="AB17">
         <f t="shared" ca="1" si="0"/>
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="AC17" t="s">
         <v>110</v>
       </c>
       <c r="AD17">
         <f t="shared" ca="1" si="1"/>
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="AE17" t="s">
         <v>110</v>
       </c>
       <c r="AF17">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG17" t="s">
         <v>110</v>
       </c>
       <c r="AH17">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI17" t="s">
         <v>110</v>
@@ -33482,7 +34504,7 @@
       </c>
       <c r="AL17" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman17@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,176,79,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman17@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,178,75,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="20" spans="1:38">
@@ -33537,7 +34559,7 @@
       </c>
       <c r="Q20">
         <f ca="1">RANDBETWEEN(0,5)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R20" t="s">
         <v>110</v>
@@ -33571,7 +34593,7 @@
       </c>
       <c r="AB20" t="str">
         <f ca="1">_xlfn.CONCAT(A20:AA20)</f>
-        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('왕십리FC','왕십리FC201018.jpg','성동구','성동구 구장','red',4,'2016-01-01',sysdate(),'1234','기업');</v>
+        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('왕십리FC','왕십리FC201018.jpg','성동구','성동구 구장','red',5,'2016-01-01',sysdate(),'1234','기업');</v>
       </c>
     </row>
     <row r="21" spans="1:38">
@@ -33626,7 +34648,7 @@
       </c>
       <c r="Q21">
         <f t="shared" ref="Q21:Q22" ca="1" si="6">RANDBETWEEN(0,5)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R21" t="s">
         <v>110</v>
@@ -33660,7 +34682,7 @@
       </c>
       <c r="AB21" t="str">
         <f t="shared" ref="AB21:AB22" ca="1" si="7">_xlfn.CONCAT(A21:AA21)</f>
-        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('답십리FC','답십리FC201018.jpg','성동구','응봉동 구장','blue',3,'2017-01-01',sysdate(),'5678','하나');</v>
+        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('답십리FC','답십리FC201018.jpg','성동구','응봉동 구장','blue',2,'2017-01-01',sysdate(),'5678','하나');</v>
       </c>
     </row>
     <row r="22" spans="1:38">
@@ -33715,7 +34737,7 @@
       </c>
       <c r="Q22">
         <f t="shared" ca="1" si="6"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="R22" t="s">
         <v>110</v>
@@ -33749,7 +34771,7 @@
       </c>
       <c r="AB22" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('대구FC','대구FC201018.jpg','달서구','달서구 구장','green',4,'2018-01-01',sysdate(),'2345','기업');</v>
+        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('대구FC','대구FC201018.jpg','달서구','달서구 구장','green',0,'2018-01-01',sysdate(),'2345','기업');</v>
       </c>
     </row>
     <row r="24" spans="1:38">

</xml_diff>

<commit_message>
[2021-01-15 15:42] 1차 완료
</commit_message>
<xml_diff>
--- a/docs/srs/fbt_docs.xlsx
+++ b/docs/srs/fbt_docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\kjy\fbt\docs\srs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DC730F-421B-458B-A756-C24B95F4939B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0F3494-42A1-44A4-BD34-649E0ED871E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{2F0AD6B2-A8A2-4F73-BAF4-7193D3382EE1}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{2F0AD6B2-A8A2-4F73-BAF4-7193D3382EE1}"/>
   </bookViews>
   <sheets>
     <sheet name="요구사항명세서" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1668" uniqueCount="686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1692" uniqueCount="701">
   <si>
     <t>요구사항 정의서</t>
   </si>
@@ -30572,6 +30572,66 @@
   </si>
   <si>
     <t>(지인용) 아이디로 투표 정보 가져오기</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>?</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>FE15</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>용병 확정하기</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>검색 조건 객체 만들기</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>재사용성 극대화된 아키텍쳐로 리팩토링</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>FS18</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>일정 수정하기</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>home_team_content / away_team_content 추가하기</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>주차, 샤워 수정하면, 만일 awayTeam이 있으면 그쪽 일정 정보도 수정되는데 괜찮은가?</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>FS19</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>일정 삭제하기</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">매치, 양도, 용병 </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>매치 용병에서 투표 자동 생성하지 않고 그러니까 일정에서는 일정만 호출. 투표 정보는 추가요청에 있을 때만</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>매치 등록 시 경기 타입별 최소인원 넘길 때만 등록가능하게</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>상세정보 추가하기</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -31438,6 +31498,9 @@
     <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -31478,9 +31541,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -31822,11 +31882,11 @@
   <sheetData>
     <row r="1" spans="2:11" ht="18" thickBot="1"/>
     <row r="2" spans="2:11" ht="18" thickBot="1">
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="91"/>
-      <c r="D2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="93"/>
       <c r="G2" s="2" t="s">
         <v>61</v>
       </c>
@@ -31841,10 +31901,10 @@
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="96" t="s">
+      <c r="C3" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="97"/>
+      <c r="D3" s="98"/>
       <c r="G3" s="4" t="s">
         <v>36</v>
       </c>
@@ -31857,10 +31917,10 @@
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="98" t="s">
+      <c r="C4" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="99"/>
+      <c r="D4" s="100"/>
       <c r="G4" s="26" t="s">
         <v>59</v>
       </c>
@@ -31887,50 +31947,50 @@
     </row>
     <row r="7" spans="2:11" ht="18" thickBot="1"/>
     <row r="8" spans="2:11" ht="18" thickBot="1">
-      <c r="B8" s="93" t="s">
+      <c r="B8" s="94" t="s">
         <v>281</v>
       </c>
-      <c r="C8" s="88" t="s">
+      <c r="C8" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="88" t="s">
+      <c r="D8" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="88" t="s">
+      <c r="E8" s="89" t="s">
         <v>279</v>
       </c>
-      <c r="F8" s="88" t="s">
+      <c r="F8" s="89" t="s">
         <v>280</v>
       </c>
-      <c r="G8" s="94" t="s">
+      <c r="G8" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="95"/>
-      <c r="I8" s="88" t="s">
+      <c r="H8" s="96"/>
+      <c r="I8" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="88" t="s">
+      <c r="J8" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="88" t="s">
+      <c r="K8" s="89" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="18" thickBot="1">
-      <c r="B9" s="89"/>
-      <c r="C9" s="89"/>
-      <c r="D9" s="89"/>
-      <c r="E9" s="89"/>
-      <c r="F9" s="89"/>
+      <c r="B9" s="90"/>
+      <c r="C9" s="90"/>
+      <c r="D9" s="90"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="90"/>
       <c r="G9" s="8" t="s">
         <v>8</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="89"/>
-      <c r="J9" s="89"/>
-      <c r="K9" s="89"/>
+      <c r="I9" s="90"/>
+      <c r="J9" s="90"/>
+      <c r="K9" s="90"/>
     </row>
     <row r="10" spans="2:11" ht="27" thickBot="1">
       <c r="B10" s="9" t="s">
@@ -33289,7 +33349,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E79B312C-DFE2-49DD-9159-A1F267AFEEB8}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -33356,10 +33416,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB557C5E-BA25-400E-9AAB-8EC528CCF68C}">
-  <dimension ref="B1:F106"/>
+  <dimension ref="B1:F109"/>
   <sheetViews>
-    <sheetView topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="C36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -33373,29 +33433,29 @@
   <sheetData>
     <row r="1" spans="2:6" ht="18" thickBot="1"/>
     <row r="2" spans="2:6" ht="18.600000000000001" thickBot="1">
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="91" t="s">
         <v>293</v>
       </c>
-      <c r="C2" s="91"/>
-      <c r="D2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="93"/>
     </row>
     <row r="3" spans="2:6" ht="18" thickBot="1">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="96" t="s">
+      <c r="C3" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="97"/>
+      <c r="D3" s="98"/>
     </row>
     <row r="4" spans="2:6" ht="18" thickBot="1">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="98" t="s">
+      <c r="C4" s="99" t="s">
         <v>288</v>
       </c>
-      <c r="D4" s="99"/>
+      <c r="D4" s="100"/>
     </row>
     <row r="5" spans="2:6" ht="18" thickBot="1"/>
     <row r="6" spans="2:6" ht="18" customHeight="1" thickBot="1">
@@ -33687,7 +33747,7 @@
     </row>
     <row r="23" spans="2:6" ht="31.8" thickBot="1">
       <c r="B23" s="32"/>
-      <c r="C23" s="102" t="s">
+      <c r="C23" s="88" t="s">
         <v>684</v>
       </c>
       <c r="D23" s="13" t="s">
@@ -33957,72 +34017,60 @@
         <v>641</v>
       </c>
     </row>
-    <row r="41" spans="2:6" ht="78.599999999999994" thickBot="1">
-      <c r="B41" s="58" t="s">
-        <v>348</v>
-      </c>
-      <c r="C41" s="58" t="s">
-        <v>344</v>
-      </c>
-      <c r="D41" s="60" t="s">
-        <v>349</v>
-      </c>
-      <c r="E41" s="59" t="s">
-        <v>350</v>
-      </c>
-      <c r="F41" s="57" t="s">
-        <v>471</v>
-      </c>
+    <row r="41" spans="2:6" ht="18" thickBot="1">
+      <c r="B41" s="77"/>
+      <c r="C41" s="61" t="s">
+        <v>691</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>692</v>
+      </c>
+      <c r="E41" s="16"/>
+      <c r="F41" s="57"/>
     </row>
-    <row r="42" spans="2:6" ht="109.8" thickBot="1">
-      <c r="B42" s="58" t="s">
-        <v>348</v>
-      </c>
-      <c r="C42" s="58" t="s">
-        <v>345</v>
-      </c>
-      <c r="D42" s="60" t="s">
-        <v>352</v>
-      </c>
-      <c r="E42" s="59" t="s">
-        <v>355</v>
-      </c>
-      <c r="F42" s="57" t="s">
-        <v>353</v>
-      </c>
+    <row r="42" spans="2:6" ht="18" thickBot="1">
+      <c r="B42" s="77"/>
+      <c r="C42" s="61" t="s">
+        <v>695</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>696</v>
+      </c>
+      <c r="E42" s="16"/>
+      <c r="F42" s="57"/>
     </row>
-    <row r="43" spans="2:6" ht="47.4" thickBot="1">
+    <row r="43" spans="2:6" ht="78.599999999999994" thickBot="1">
       <c r="B43" s="58" t="s">
         <v>348</v>
       </c>
       <c r="C43" s="58" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="D43" s="60" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="E43" s="59" t="s">
-        <v>664</v>
+        <v>350</v>
       </c>
       <c r="F43" s="57" t="s">
-        <v>665</v>
+        <v>471</v>
       </c>
     </row>
-    <row r="44" spans="2:6" ht="63" thickBot="1">
+    <row r="44" spans="2:6" ht="109.8" thickBot="1">
       <c r="B44" s="58" t="s">
         <v>348</v>
       </c>
       <c r="C44" s="58" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
       <c r="D44" s="60" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="E44" s="59" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="F44" s="57" t="s">
-        <v>370</v>
+        <v>353</v>
       </c>
     </row>
     <row r="45" spans="2:6" ht="47.4" thickBot="1">
@@ -34030,303 +34078,303 @@
         <v>348</v>
       </c>
       <c r="C45" s="58" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
       <c r="D45" s="60" t="s">
-        <v>221</v>
+        <v>354</v>
       </c>
       <c r="E45" s="59" t="s">
-        <v>363</v>
+        <v>664</v>
       </c>
       <c r="F45" s="57" t="s">
-        <v>364</v>
+        <v>665</v>
       </c>
     </row>
-    <row r="46" spans="2:6" ht="42" thickBot="1">
+    <row r="46" spans="2:6" ht="63" thickBot="1">
       <c r="B46" s="58" t="s">
         <v>348</v>
       </c>
       <c r="C46" s="58" t="s">
+        <v>359</v>
+      </c>
+      <c r="D46" s="60" t="s">
+        <v>360</v>
+      </c>
+      <c r="E46" s="59" t="s">
+        <v>361</v>
+      </c>
+      <c r="F46" s="57" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" ht="47.4" thickBot="1">
+      <c r="B47" s="58" t="s">
+        <v>348</v>
+      </c>
+      <c r="C47" s="58" t="s">
+        <v>362</v>
+      </c>
+      <c r="D47" s="60" t="s">
+        <v>221</v>
+      </c>
+      <c r="E47" s="59" t="s">
+        <v>363</v>
+      </c>
+      <c r="F47" s="57" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" ht="42" thickBot="1">
+      <c r="B48" s="58" t="s">
+        <v>348</v>
+      </c>
+      <c r="C48" s="58" t="s">
         <v>365</v>
       </c>
-      <c r="D46" s="60" t="s">
+      <c r="D48" s="60" t="s">
         <v>224</v>
       </c>
-      <c r="E46" s="59" t="s">
+      <c r="E48" s="59" t="s">
         <v>366</v>
       </c>
-      <c r="F46" s="57" t="s">
+      <c r="F48" s="57" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="47" spans="2:6" ht="78.599999999999994" thickBot="1">
-      <c r="B47" s="63" t="s">
-        <v>348</v>
-      </c>
-      <c r="C47" s="58" t="s">
-        <v>368</v>
-      </c>
-      <c r="D47" s="60" t="s">
-        <v>369</v>
-      </c>
-      <c r="E47" s="59" t="s">
-        <v>377</v>
-      </c>
-      <c r="F47" s="57" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" ht="172.2" thickBot="1">
-      <c r="B48" s="63" t="s">
-        <v>348</v>
-      </c>
-      <c r="C48" s="58" t="s">
-        <v>371</v>
-      </c>
-      <c r="D48" s="60" t="s">
-        <v>372</v>
-      </c>
-      <c r="E48" s="59" t="s">
-        <v>666</v>
-      </c>
-      <c r="F48" s="57" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" ht="43.8" thickBot="1">
+    <row r="49" spans="2:6" ht="78.599999999999994" thickBot="1">
       <c r="B49" s="63" t="s">
         <v>348</v>
       </c>
       <c r="C49" s="58" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="D49" s="60" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="E49" s="59" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="F49" s="57" t="s">
-        <v>383</v>
+        <v>462</v>
       </c>
     </row>
-    <row r="50" spans="2:6" ht="78.599999999999994" thickBot="1">
+    <row r="50" spans="2:6" ht="172.2" thickBot="1">
       <c r="B50" s="63" t="s">
         <v>348</v>
       </c>
       <c r="C50" s="58" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="D50" s="60" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="E50" s="59" t="s">
-        <v>378</v>
+        <v>666</v>
       </c>
       <c r="F50" s="57" t="s">
-        <v>379</v>
+        <v>667</v>
       </c>
     </row>
-    <row r="51" spans="2:6" ht="59.4" thickBot="1">
+    <row r="51" spans="2:6" ht="43.8" thickBot="1">
       <c r="B51" s="63" t="s">
         <v>348</v>
       </c>
       <c r="C51" s="58" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="D51" s="60" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="E51" s="59" t="s">
-        <v>668</v>
+        <v>382</v>
       </c>
       <c r="F51" s="57" t="s">
-        <v>669</v>
+        <v>383</v>
       </c>
     </row>
-    <row r="52" spans="2:6" ht="57.6" thickBot="1">
+    <row r="52" spans="2:6" ht="78.599999999999994" thickBot="1">
       <c r="B52" s="63" t="s">
         <v>348</v>
       </c>
       <c r="C52" s="58" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="D52" s="60" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="E52" s="59" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="F52" s="57" t="s">
-        <v>444</v>
+        <v>379</v>
       </c>
     </row>
-    <row r="53" spans="2:6" ht="40.200000000000003" thickBot="1">
+    <row r="53" spans="2:6" ht="59.4" thickBot="1">
       <c r="B53" s="63" t="s">
         <v>348</v>
       </c>
       <c r="C53" s="58" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="D53" s="60" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="E53" s="59" t="s">
-        <v>389</v>
+        <v>668</v>
       </c>
       <c r="F53" s="57" t="s">
-        <v>390</v>
+        <v>669</v>
       </c>
     </row>
-    <row r="54" spans="2:6" ht="94.2" thickBot="1">
+    <row r="54" spans="2:6" ht="57.6" thickBot="1">
       <c r="B54" s="63" t="s">
         <v>348</v>
       </c>
       <c r="C54" s="58" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="D54" s="60" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="E54" s="59" t="s">
-        <v>439</v>
+        <v>386</v>
       </c>
       <c r="F54" s="57" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
-    <row r="55" spans="2:6" ht="109.8" thickBot="1">
+    <row r="55" spans="2:6" ht="40.200000000000003" thickBot="1">
       <c r="B55" s="63" t="s">
         <v>348</v>
       </c>
       <c r="C55" s="58" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="D55" s="60" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="E55" s="59" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="F55" s="57" t="s">
-        <v>671</v>
+        <v>390</v>
       </c>
     </row>
-    <row r="56" spans="2:6" ht="123" thickBot="1">
+    <row r="56" spans="2:6" ht="94.2" thickBot="1">
       <c r="B56" s="63" t="s">
         <v>348</v>
       </c>
       <c r="C56" s="58" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="D56" s="60" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="E56" s="59" t="s">
-        <v>402</v>
+        <v>439</v>
       </c>
       <c r="F56" s="57" t="s">
-        <v>403</v>
+        <v>445</v>
       </c>
     </row>
-    <row r="57" spans="2:6" ht="63" thickBot="1">
+    <row r="57" spans="2:6" ht="109.8" thickBot="1">
       <c r="B57" s="63" t="s">
         <v>348</v>
       </c>
       <c r="C57" s="58" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D57" s="60" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="E57" s="59" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="F57" s="57" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
-    <row r="58" spans="2:6" ht="109.8" thickBot="1">
+    <row r="58" spans="2:6" ht="123" thickBot="1">
       <c r="B58" s="63" t="s">
         <v>348</v>
       </c>
       <c r="C58" s="58" t="s">
+        <v>396</v>
+      </c>
+      <c r="D58" s="60" t="s">
+        <v>401</v>
+      </c>
+      <c r="E58" s="59" t="s">
+        <v>402</v>
+      </c>
+      <c r="F58" s="57" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" ht="63" thickBot="1">
+      <c r="B59" s="63" t="s">
+        <v>348</v>
+      </c>
+      <c r="C59" s="58" t="s">
+        <v>398</v>
+      </c>
+      <c r="D59" s="60" t="s">
+        <v>399</v>
+      </c>
+      <c r="E59" s="59" t="s">
+        <v>400</v>
+      </c>
+      <c r="F59" s="57" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" ht="109.8" thickBot="1">
+      <c r="B60" s="63" t="s">
+        <v>348</v>
+      </c>
+      <c r="C60" s="58" t="s">
         <v>404</v>
       </c>
-      <c r="D58" s="60" t="s">
+      <c r="D60" s="60" t="s">
         <v>405</v>
       </c>
-      <c r="E58" s="59"/>
-      <c r="F58" s="57" t="s">
+      <c r="E60" s="59"/>
+      <c r="F60" s="57" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="59" spans="2:6" ht="60.6" thickBot="1">
-      <c r="B59" s="64" t="s">
-        <v>286</v>
-      </c>
-      <c r="C59" s="64" t="s">
-        <v>407</v>
-      </c>
-      <c r="D59" s="60" t="s">
-        <v>417</v>
-      </c>
-      <c r="E59" s="59" t="s">
-        <v>418</v>
-      </c>
-      <c r="F59" s="57" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6" ht="125.4" thickBot="1">
-      <c r="B60" s="64" t="s">
-        <v>286</v>
-      </c>
-      <c r="C60" s="64" t="s">
-        <v>408</v>
-      </c>
-      <c r="D60" s="60" t="s">
-        <v>426</v>
-      </c>
-      <c r="E60" s="59" t="s">
-        <v>428</v>
-      </c>
-      <c r="F60" s="57" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="61" spans="2:6" ht="47.4" thickBot="1">
+    <row r="61" spans="2:6" ht="60.6" thickBot="1">
       <c r="B61" s="64" t="s">
         <v>286</v>
       </c>
       <c r="C61" s="64" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D61" s="60" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="E61" s="59" t="s">
-        <v>673</v>
+        <v>418</v>
       </c>
       <c r="F61" s="57" t="s">
-        <v>674</v>
+        <v>470</v>
       </c>
     </row>
-    <row r="62" spans="2:6" ht="63" thickBot="1">
+    <row r="62" spans="2:6" ht="125.4" thickBot="1">
       <c r="B62" s="64" t="s">
         <v>286</v>
       </c>
       <c r="C62" s="64" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D62" s="60" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="E62" s="59" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F62" s="57" t="s">
-        <v>436</v>
+        <v>423</v>
       </c>
     </row>
     <row r="63" spans="2:6" ht="47.4" thickBot="1">
@@ -34334,169 +34382,169 @@
         <v>286</v>
       </c>
       <c r="C63" s="64" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D63" s="60" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="E63" s="59" t="s">
-        <v>430</v>
+        <v>673</v>
       </c>
       <c r="F63" s="57" t="s">
-        <v>433</v>
+        <v>674</v>
       </c>
     </row>
-    <row r="64" spans="2:6" ht="43.8" thickBot="1">
+    <row r="64" spans="2:6" ht="63" thickBot="1">
       <c r="B64" s="64" t="s">
         <v>286</v>
       </c>
       <c r="C64" s="64" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D64" s="60" t="s">
-        <v>95</v>
+        <v>425</v>
       </c>
       <c r="E64" s="59" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="F64" s="57" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
     </row>
-    <row r="65" spans="2:6" ht="78.599999999999994" thickBot="1">
+    <row r="65" spans="2:6" ht="47.4" thickBot="1">
       <c r="B65" s="64" t="s">
         <v>286</v>
       </c>
       <c r="C65" s="64" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D65" s="60" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="E65" s="59" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F65" s="57" t="s">
-        <v>397</v>
+        <v>433</v>
       </c>
     </row>
-    <row r="66" spans="2:6" ht="125.4" thickBot="1">
+    <row r="66" spans="2:6" ht="43.8" thickBot="1">
       <c r="B66" s="64" t="s">
         <v>286</v>
       </c>
       <c r="C66" s="64" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D66" s="60" t="s">
-        <v>437</v>
+        <v>95</v>
       </c>
       <c r="E66" s="59" t="s">
-        <v>677</v>
+        <v>432</v>
       </c>
       <c r="F66" s="57" t="s">
-        <v>678</v>
+        <v>434</v>
       </c>
     </row>
-    <row r="67" spans="2:6" ht="43.8" thickBot="1">
+    <row r="67" spans="2:6" ht="78.599999999999994" thickBot="1">
       <c r="B67" s="64" t="s">
         <v>286</v>
       </c>
       <c r="C67" s="64" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D67" s="60" t="s">
-        <v>440</v>
+        <v>427</v>
       </c>
       <c r="E67" s="59" t="s">
-        <v>679</v>
+        <v>435</v>
       </c>
       <c r="F67" s="57" t="s">
-        <v>680</v>
+        <v>397</v>
       </c>
     </row>
-    <row r="68" spans="2:6" ht="61.2" thickBot="1">
+    <row r="68" spans="2:6" ht="125.4" thickBot="1">
       <c r="B68" s="64" t="s">
         <v>286</v>
       </c>
       <c r="C68" s="64" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D68" s="60" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="E68" s="59" t="s">
-        <v>443</v>
+        <v>677</v>
       </c>
       <c r="F68" s="57" t="s">
-        <v>447</v>
+        <v>678</v>
       </c>
     </row>
-    <row r="69" spans="2:6" ht="18" thickBot="1">
+    <row r="69" spans="2:6" ht="43.8" thickBot="1">
       <c r="B69" s="64" t="s">
         <v>286</v>
       </c>
       <c r="C69" s="64" t="s">
-        <v>448</v>
+        <v>415</v>
       </c>
       <c r="D69" s="60" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="E69" s="59" t="s">
-        <v>450</v>
+        <v>679</v>
       </c>
       <c r="F69" s="57" t="s">
-        <v>449</v>
+        <v>680</v>
       </c>
     </row>
-    <row r="70" spans="2:6" ht="78.599999999999994" thickBot="1">
+    <row r="70" spans="2:6" ht="61.2" thickBot="1">
       <c r="B70" s="64" t="s">
         <v>286</v>
       </c>
       <c r="C70" s="64" t="s">
-        <v>451</v>
+        <v>416</v>
       </c>
       <c r="D70" s="60" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="E70" s="59" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="F70" s="57" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
     </row>
-    <row r="71" spans="2:6" ht="109.8" thickBot="1">
+    <row r="71" spans="2:6" ht="18" thickBot="1">
       <c r="B71" s="64" t="s">
         <v>286</v>
       </c>
       <c r="C71" s="64" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="D71" s="60" t="s">
-        <v>457</v>
+        <v>446</v>
       </c>
       <c r="E71" s="59" t="s">
-        <v>402</v>
+        <v>450</v>
       </c>
       <c r="F71" s="57" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
     </row>
-    <row r="72" spans="2:6" ht="47.4" thickBot="1">
+    <row r="72" spans="2:6" ht="78.599999999999994" thickBot="1">
       <c r="B72" s="64" t="s">
         <v>286</v>
       </c>
       <c r="C72" s="64" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="D72" s="60" t="s">
-        <v>456</v>
+        <v>441</v>
       </c>
       <c r="E72" s="59" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="F72" s="57" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
     </row>
     <row r="73" spans="2:6" ht="109.8" thickBot="1">
@@ -34504,93 +34552,93 @@
         <v>286</v>
       </c>
       <c r="C73" s="64" t="s">
+        <v>454</v>
+      </c>
+      <c r="D73" s="60" t="s">
+        <v>457</v>
+      </c>
+      <c r="E73" s="59" t="s">
+        <v>402</v>
+      </c>
+      <c r="F73" s="57" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" ht="47.4" thickBot="1">
+      <c r="B74" s="64" t="s">
+        <v>286</v>
+      </c>
+      <c r="C74" s="64" t="s">
+        <v>455</v>
+      </c>
+      <c r="D74" s="60" t="s">
+        <v>456</v>
+      </c>
+      <c r="E74" s="59" t="s">
+        <v>460</v>
+      </c>
+      <c r="F74" s="57" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" ht="109.8" thickBot="1">
+      <c r="B75" s="64" t="s">
+        <v>286</v>
+      </c>
+      <c r="C75" s="64" t="s">
         <v>464</v>
       </c>
-      <c r="D73" s="60" t="s">
+      <c r="D75" s="60" t="s">
         <v>463</v>
       </c>
-      <c r="E73" s="59"/>
-      <c r="F73" s="57" t="s">
+      <c r="E75" s="59"/>
+      <c r="F75" s="57" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="74" spans="2:6" ht="18" thickBot="1">
-      <c r="B74" s="64"/>
-      <c r="C74" s="87" t="s">
+    <row r="76" spans="2:6" ht="18" thickBot="1">
+      <c r="B76" s="64"/>
+      <c r="C76" s="87" t="s">
         <v>675</v>
       </c>
-      <c r="D74" s="66" t="s">
+      <c r="D76" s="66" t="s">
         <v>676</v>
       </c>
-      <c r="E74" s="59"/>
-      <c r="F74" s="57"/>
+      <c r="E76" s="59"/>
+      <c r="F76" s="57"/>
     </row>
-    <row r="75" spans="2:6" ht="63" thickBot="1">
-      <c r="B75" s="65" t="s">
-        <v>465</v>
-      </c>
-      <c r="C75" s="68" t="s">
-        <v>466</v>
-      </c>
-      <c r="D75" s="66" t="s">
-        <v>467</v>
-      </c>
-      <c r="E75" s="59" t="s">
-        <v>468</v>
-      </c>
-      <c r="F75" s="57" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="76" spans="2:6" ht="109.8" thickBot="1">
-      <c r="B76" s="65" t="s">
-        <v>465</v>
-      </c>
-      <c r="C76" s="65" t="s">
-        <v>472</v>
-      </c>
-      <c r="D76" s="67" t="s">
-        <v>473</v>
-      </c>
-      <c r="E76" s="59" t="s">
-        <v>474</v>
-      </c>
-      <c r="F76" s="57" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="77" spans="2:6" ht="47.4" thickBot="1">
+    <row r="77" spans="2:6" ht="63" thickBot="1">
       <c r="B77" s="65" t="s">
         <v>465</v>
       </c>
-      <c r="C77" s="65" t="s">
-        <v>475</v>
-      </c>
-      <c r="D77" s="67" t="s">
-        <v>476</v>
+      <c r="C77" s="68" t="s">
+        <v>466</v>
+      </c>
+      <c r="D77" s="66" t="s">
+        <v>467</v>
       </c>
       <c r="E77" s="59" t="s">
-        <v>681</v>
+        <v>468</v>
       </c>
       <c r="F77" s="57" t="s">
-        <v>682</v>
+        <v>469</v>
       </c>
     </row>
-    <row r="78" spans="2:6" ht="94.2" thickBot="1">
+    <row r="78" spans="2:6" ht="109.8" thickBot="1">
       <c r="B78" s="65" t="s">
         <v>465</v>
       </c>
       <c r="C78" s="65" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="D78" s="67" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="E78" s="59" t="s">
-        <v>502</v>
+        <v>474</v>
       </c>
       <c r="F78" s="57" t="s">
-        <v>506</v>
+        <v>353</v>
       </c>
     </row>
     <row r="79" spans="2:6" ht="47.4" thickBot="1">
@@ -34598,382 +34646,427 @@
         <v>465</v>
       </c>
       <c r="C79" s="65" t="s">
-        <v>483</v>
-      </c>
-      <c r="D79" s="60" t="s">
-        <v>484</v>
+        <v>475</v>
+      </c>
+      <c r="D79" s="67" t="s">
+        <v>476</v>
       </c>
       <c r="E79" s="59" t="s">
-        <v>485</v>
+        <v>681</v>
       </c>
       <c r="F79" s="57" t="s">
-        <v>486</v>
+        <v>682</v>
       </c>
     </row>
-    <row r="80" spans="2:6" ht="43.8" thickBot="1">
+    <row r="80" spans="2:6" ht="94.2" thickBot="1">
       <c r="B80" s="65" t="s">
         <v>465</v>
       </c>
       <c r="C80" s="65" t="s">
-        <v>489</v>
-      </c>
-      <c r="D80" s="60" t="s">
-        <v>487</v>
+        <v>477</v>
+      </c>
+      <c r="D80" s="67" t="s">
+        <v>478</v>
       </c>
       <c r="E80" s="59" t="s">
-        <v>488</v>
+        <v>502</v>
       </c>
       <c r="F80" s="57" t="s">
-        <v>490</v>
+        <v>506</v>
       </c>
     </row>
-    <row r="81" spans="2:6" ht="94.2" thickBot="1">
+    <row r="81" spans="2:6" ht="47.4" thickBot="1">
       <c r="B81" s="65" t="s">
         <v>465</v>
       </c>
       <c r="C81" s="65" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="D81" s="60" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="E81" s="59" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="F81" s="57" t="s">
-        <v>540</v>
+        <v>486</v>
       </c>
     </row>
-    <row r="82" spans="2:6" ht="47.4" thickBot="1">
+    <row r="82" spans="2:6" ht="43.8" thickBot="1">
       <c r="B82" s="65" t="s">
         <v>465</v>
       </c>
       <c r="C82" s="65" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="D82" s="60" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="E82" s="59" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="F82" s="57" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
     </row>
-    <row r="83" spans="2:6" ht="87.6" thickBot="1">
+    <row r="83" spans="2:6" ht="94.2" thickBot="1">
       <c r="B83" s="65" t="s">
         <v>465</v>
       </c>
       <c r="C83" s="65" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
       <c r="D83" s="60" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="E83" s="59" t="s">
-        <v>504</v>
+        <v>493</v>
       </c>
       <c r="F83" s="57" t="s">
-        <v>509</v>
+        <v>540</v>
       </c>
     </row>
-    <row r="84" spans="2:6" ht="87.6" thickBot="1">
+    <row r="84" spans="2:6" ht="47.4" thickBot="1">
       <c r="B84" s="65" t="s">
         <v>465</v>
       </c>
       <c r="C84" s="65" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D84" s="60" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
       <c r="E84" s="59" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="F84" s="57" t="s">
-        <v>508</v>
+        <v>496</v>
       </c>
     </row>
-    <row r="85" spans="2:6" ht="109.8" thickBot="1">
+    <row r="85" spans="2:6" ht="87.6" thickBot="1">
       <c r="B85" s="65" t="s">
         <v>465</v>
       </c>
       <c r="C85" s="65" t="s">
-        <v>507</v>
+        <v>498</v>
       </c>
       <c r="D85" s="60" t="s">
-        <v>511</v>
+        <v>500</v>
       </c>
       <c r="E85" s="59" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="F85" s="57" t="s">
-        <v>516</v>
+        <v>509</v>
       </c>
     </row>
-    <row r="86" spans="2:6" ht="47.4" thickBot="1">
+    <row r="86" spans="2:6" ht="87.6" thickBot="1">
       <c r="B86" s="65" t="s">
         <v>465</v>
       </c>
       <c r="C86" s="65" t="s">
-        <v>510</v>
+        <v>499</v>
       </c>
       <c r="D86" s="60" t="s">
-        <v>513</v>
+        <v>501</v>
       </c>
       <c r="E86" s="59" t="s">
-        <v>514</v>
+        <v>503</v>
       </c>
       <c r="F86" s="57" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
     </row>
-    <row r="87" spans="2:6" ht="18" thickBot="1">
+    <row r="87" spans="2:6" ht="109.8" thickBot="1">
       <c r="B87" s="65" t="s">
         <v>465</v>
       </c>
       <c r="C87" s="65" t="s">
-        <v>517</v>
+        <v>507</v>
       </c>
       <c r="D87" s="60" t="s">
-        <v>446</v>
+        <v>511</v>
       </c>
       <c r="E87" s="59" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="F87" s="57" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
-    <row r="88" spans="2:6" ht="109.8" thickBot="1">
+    <row r="88" spans="2:6" ht="47.4" thickBot="1">
       <c r="B88" s="65" t="s">
         <v>465</v>
       </c>
       <c r="C88" s="65" t="s">
+        <v>510</v>
+      </c>
+      <c r="D88" s="60" t="s">
+        <v>513</v>
+      </c>
+      <c r="E88" s="59" t="s">
+        <v>514</v>
+      </c>
+      <c r="F88" s="57" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" ht="18" thickBot="1">
+      <c r="B89" s="65" t="s">
+        <v>465</v>
+      </c>
+      <c r="C89" s="65" t="s">
+        <v>517</v>
+      </c>
+      <c r="D89" s="60" t="s">
+        <v>446</v>
+      </c>
+      <c r="E89" s="59" t="s">
+        <v>514</v>
+      </c>
+      <c r="F89" s="57" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" ht="109.8" thickBot="1">
+      <c r="B90" s="65" t="s">
+        <v>465</v>
+      </c>
+      <c r="C90" s="65" t="s">
         <v>519</v>
       </c>
-      <c r="D88" s="60" t="s">
+      <c r="D90" s="60" t="s">
         <v>520</v>
       </c>
-      <c r="E88" s="59" t="s">
+      <c r="E90" s="59" t="s">
         <v>521</v>
       </c>
-      <c r="F88" s="57" t="s">
+      <c r="F90" s="57" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="89" spans="2:6" ht="78.599999999999994" thickBot="1">
-      <c r="B89" s="62" t="s">
+    <row r="91" spans="2:6" ht="18" thickBot="1">
+      <c r="B91" s="65"/>
+      <c r="C91" s="65" t="s">
+        <v>687</v>
+      </c>
+      <c r="D91" s="71" t="s">
+        <v>688</v>
+      </c>
+      <c r="E91" s="73"/>
+      <c r="F91" s="75"/>
+    </row>
+    <row r="92" spans="2:6" ht="78.599999999999994" thickBot="1">
+      <c r="B92" s="62" t="s">
         <v>356</v>
       </c>
-      <c r="C89" s="62" t="s">
+      <c r="C92" s="62" t="s">
         <v>357</v>
       </c>
-      <c r="D89" s="71" t="s">
+      <c r="D92" s="71" t="s">
         <v>358</v>
       </c>
-      <c r="E89" s="73" t="s">
+      <c r="E92" s="73" t="s">
         <v>461</v>
       </c>
-      <c r="F89" s="75" t="s">
+      <c r="F92" s="75" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="90" spans="2:6" ht="34.799999999999997">
-      <c r="B90" s="83"/>
-      <c r="C90" s="83" t="s">
+    <row r="93" spans="2:6" ht="34.799999999999997">
+      <c r="B93" s="83"/>
+      <c r="C93" s="83" t="s">
         <v>630</v>
       </c>
-      <c r="D90" s="82" t="s">
+      <c r="D93" s="82" t="s">
         <v>628</v>
       </c>
-      <c r="F90" s="33" t="s">
+      <c r="F93" s="33" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="91" spans="2:6" ht="69.599999999999994">
-      <c r="B91" s="83"/>
-      <c r="C91" s="83" t="s">
+    <row r="94" spans="2:6" ht="69.599999999999994">
+      <c r="B94" s="83"/>
+      <c r="C94" s="83" t="s">
         <v>631</v>
       </c>
-      <c r="D91" s="82" t="s">
+      <c r="D94" s="82" t="s">
         <v>632</v>
       </c>
-      <c r="F91" s="33" t="s">
+      <c r="F94" s="33" t="s">
         <v>633</v>
       </c>
     </row>
-    <row r="92" spans="2:6" ht="70.2" thickBot="1">
-      <c r="B92" s="83"/>
-      <c r="C92" s="83" t="s">
+    <row r="95" spans="2:6" ht="70.2" thickBot="1">
+      <c r="B95" s="83"/>
+      <c r="C95" s="83" t="s">
         <v>634</v>
       </c>
-      <c r="D92" s="82" t="s">
+      <c r="D95" s="82" t="s">
         <v>635</v>
       </c>
-      <c r="F92" s="33" t="s">
+      <c r="F95" s="33" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="93" spans="2:6" ht="47.4" thickBot="1">
-      <c r="B93" s="69" t="s">
+    <row r="96" spans="2:6" ht="47.4" thickBot="1">
+      <c r="B96" s="69" t="s">
         <v>479</v>
       </c>
-      <c r="C93" s="70" t="s">
+      <c r="C96" s="70" t="s">
         <v>505</v>
       </c>
-      <c r="D93" s="72" t="s">
+      <c r="D96" s="72" t="s">
         <v>480</v>
       </c>
-      <c r="E93" s="74" t="s">
+      <c r="E96" s="74" t="s">
         <v>482</v>
       </c>
-      <c r="F93" s="76" t="s">
+      <c r="F96" s="76" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="94" spans="2:6" ht="34.799999999999997">
-      <c r="B94" s="84"/>
-      <c r="C94" s="84" t="s">
-        <v>637</v>
-      </c>
-      <c r="D94" s="82" t="s">
-        <v>638</v>
-      </c>
-      <c r="E94" s="85"/>
-      <c r="F94" s="86" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="95" spans="2:6">
-      <c r="B95" s="84"/>
-      <c r="C95" s="84" t="s">
-        <v>643</v>
-      </c>
-      <c r="D95" s="82" t="s">
-        <v>644</v>
-      </c>
-      <c r="E95" s="85"/>
-      <c r="F95" s="86"/>
-    </row>
-    <row r="96" spans="2:6">
-      <c r="B96" s="84"/>
-      <c r="C96" s="84" t="s">
-        <v>645</v>
-      </c>
-      <c r="D96" s="82" t="s">
-        <v>646</v>
-      </c>
-      <c r="E96" s="85"/>
-      <c r="F96" s="86"/>
-    </row>
-    <row r="97" spans="2:6">
+    <row r="97" spans="2:6" ht="34.799999999999997">
       <c r="B97" s="84"/>
       <c r="C97" s="84" t="s">
-        <v>647</v>
+        <v>637</v>
       </c>
       <c r="D97" s="82" t="s">
-        <v>648</v>
+        <v>638</v>
       </c>
       <c r="E97" s="85"/>
-      <c r="F97" s="86"/>
+      <c r="F97" s="86" t="s">
+        <v>639</v>
+      </c>
     </row>
-    <row r="98" spans="2:6" ht="69.599999999999994">
+    <row r="98" spans="2:6">
       <c r="B98" s="84"/>
       <c r="C98" s="84" t="s">
-        <v>652</v>
+        <v>643</v>
       </c>
       <c r="D98" s="82" t="s">
-        <v>653</v>
+        <v>644</v>
       </c>
       <c r="E98" s="85"/>
-      <c r="F98" s="86" t="s">
-        <v>654</v>
-      </c>
+      <c r="F98" s="86"/>
     </row>
     <row r="99" spans="2:6">
-      <c r="C99" s="81" t="s">
+      <c r="B99" s="84"/>
+      <c r="C99" s="84" t="s">
+        <v>645</v>
+      </c>
+      <c r="D99" s="82" t="s">
+        <v>646</v>
+      </c>
+      <c r="E99" s="85"/>
+      <c r="F99" s="86"/>
+    </row>
+    <row r="100" spans="2:6">
+      <c r="B100" s="84"/>
+      <c r="C100" s="84" t="s">
+        <v>647</v>
+      </c>
+      <c r="D100" s="82" t="s">
+        <v>648</v>
+      </c>
+      <c r="E100" s="85"/>
+      <c r="F100" s="86"/>
+    </row>
+    <row r="101" spans="2:6" ht="69.599999999999994">
+      <c r="B101" s="84"/>
+      <c r="C101" s="84" t="s">
+        <v>652</v>
+      </c>
+      <c r="D101" s="82" t="s">
+        <v>653</v>
+      </c>
+      <c r="E101" s="85"/>
+      <c r="F101" s="86" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="102" spans="2:6">
+      <c r="C102" s="81" t="s">
         <v>612</v>
       </c>
-      <c r="D99" s="82" t="s">
+      <c r="D102" s="82" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="100" spans="2:6" ht="104.4">
-      <c r="C100" s="81" t="s">
+    <row r="103" spans="2:6" ht="104.4">
+      <c r="C103" s="81" t="s">
         <v>613</v>
       </c>
-      <c r="D100" s="82" t="s">
+      <c r="D103" s="82" t="s">
         <v>614</v>
       </c>
-      <c r="F100" s="33" t="s">
+      <c r="F103" s="33" t="s">
         <v>615</v>
-      </c>
-    </row>
-    <row r="101" spans="2:6" ht="34.799999999999997">
-      <c r="C101" s="81" t="s">
-        <v>616</v>
-      </c>
-      <c r="D101" s="82" t="s">
-        <v>617</v>
-      </c>
-      <c r="F101" s="33" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="102" spans="2:6" ht="34.799999999999997">
-      <c r="C102" s="81" t="s">
-        <v>619</v>
-      </c>
-      <c r="D102" s="82" t="s">
-        <v>620</v>
-      </c>
-      <c r="F102" s="33" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="103" spans="2:6" ht="34.799999999999997">
-      <c r="C103" s="81" t="s">
-        <v>622</v>
-      </c>
-      <c r="D103" s="82" t="s">
-        <v>623</v>
-      </c>
-      <c r="F103" s="33" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="104" spans="2:6" ht="34.799999999999997">
       <c r="C104" s="81" t="s">
+        <v>616</v>
+      </c>
+      <c r="D104" s="82" t="s">
+        <v>617</v>
+      </c>
+      <c r="F104" s="33" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="105" spans="2:6" ht="34.799999999999997">
+      <c r="C105" s="81" t="s">
+        <v>619</v>
+      </c>
+      <c r="D105" s="82" t="s">
+        <v>620</v>
+      </c>
+      <c r="F105" s="33" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="106" spans="2:6" ht="34.799999999999997">
+      <c r="C106" s="81" t="s">
+        <v>622</v>
+      </c>
+      <c r="D106" s="82" t="s">
+        <v>623</v>
+      </c>
+      <c r="F106" s="33" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="107" spans="2:6" ht="34.799999999999997">
+      <c r="C107" s="81" t="s">
         <v>624</v>
       </c>
-      <c r="D104" s="82" t="s">
+      <c r="D107" s="82" t="s">
         <v>625</v>
       </c>
-      <c r="F104" s="33" t="s">
+      <c r="F107" s="33" t="s">
         <v>626</v>
       </c>
     </row>
-    <row r="105" spans="2:6" ht="52.2">
-      <c r="C105" s="81" t="s">
+    <row r="108" spans="2:6" ht="52.2">
+      <c r="C108" s="81" t="s">
         <v>649</v>
       </c>
-      <c r="D105" s="82" t="s">
+      <c r="D108" s="82" t="s">
         <v>650</v>
       </c>
-      <c r="F105" s="33" t="s">
+      <c r="F108" s="33" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="106" spans="2:6" ht="52.2">
-      <c r="C106" s="81" t="s">
+    <row r="109" spans="2:6" ht="52.2">
+      <c r="C109" s="81" t="s">
         <v>655</v>
       </c>
-      <c r="D106" s="82" t="s">
+      <c r="D109" s="82" t="s">
         <v>656</v>
       </c>
-      <c r="F106" s="33" t="s">
+      <c r="F109" s="33" t="s">
         <v>657</v>
       </c>
     </row>
@@ -34992,10 +35085,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5771FFE9-0A00-44DE-A281-68110209A845}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -35003,28 +35096,34 @@
     <col min="2" max="2" width="66.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="C1" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>562</v>
       </c>
+      <c r="C2" t="s">
+        <v>587</v>
+      </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>563</v>
       </c>
+      <c r="C3" t="s">
+        <v>587</v>
+      </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -35035,7 +35134,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -35043,79 +35142,106 @@
         <v>565</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>566</v>
       </c>
+      <c r="C6" t="s">
+        <v>587</v>
+      </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>567</v>
       </c>
+      <c r="C7" t="s">
+        <v>587</v>
+      </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>568</v>
       </c>
+      <c r="C8" t="s">
+        <v>686</v>
+      </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>569</v>
       </c>
+      <c r="C9" t="s">
+        <v>587</v>
+      </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>570</v>
       </c>
+      <c r="C10" t="s">
+        <v>587</v>
+      </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>571</v>
       </c>
+      <c r="D11" t="s">
+        <v>694</v>
+      </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>573</v>
       </c>
+      <c r="C12" t="s">
+        <v>587</v>
+      </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>574</v>
       </c>
+      <c r="C13" t="s">
+        <v>587</v>
+      </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>575</v>
       </c>
+      <c r="C14" t="s">
+        <v>587</v>
+      </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>14</v>
       </c>
@@ -35123,7 +35249,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>12</v>
       </c>
@@ -35131,7 +35257,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>15</v>
       </c>
@@ -35139,7 +35265,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>16</v>
       </c>
@@ -35147,7 +35273,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>17</v>
       </c>
@@ -35155,7 +35281,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>18</v>
       </c>
@@ -35165,8 +35291,11 @@
       <c r="C20" t="s">
         <v>587</v>
       </c>
+      <c r="D20" t="s">
+        <v>700</v>
+      </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>19</v>
       </c>
@@ -35177,7 +35306,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>20</v>
       </c>
@@ -35185,17 +35314,66 @@
         <v>582</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>683</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>699</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -35460,7 +35638,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="101" t="s">
         <v>257</v>
       </c>
       <c r="B1">
@@ -35471,7 +35649,7 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="100"/>
+      <c r="A2" s="101"/>
       <c r="B2">
         <v>1</v>
       </c>
@@ -35480,7 +35658,7 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="100"/>
+      <c r="A3" s="101"/>
       <c r="B3">
         <v>2</v>
       </c>
@@ -35489,7 +35667,7 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="101" t="s">
+      <c r="A4" s="102" t="s">
         <v>261</v>
       </c>
       <c r="B4">
@@ -35500,7 +35678,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="101"/>
+      <c r="A5" s="102"/>
       <c r="B5">
         <v>1</v>
       </c>
@@ -35509,7 +35687,7 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="101"/>
+      <c r="A6" s="102"/>
       <c r="B6">
         <v>-1</v>
       </c>
@@ -35518,7 +35696,7 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="100" t="s">
+      <c r="A7" s="101" t="s">
         <v>266</v>
       </c>
       <c r="B7">
@@ -35529,7 +35707,7 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="100"/>
+      <c r="A8" s="101"/>
       <c r="B8">
         <v>1</v>
       </c>
@@ -35538,7 +35716,7 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="100"/>
+      <c r="A9" s="101"/>
       <c r="B9">
         <v>2</v>
       </c>
@@ -35696,14 +35874,14 @@
       </c>
       <c r="AB1">
         <f ca="1">RANDBETWEEN(170,185)</f>
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="AC1" t="s">
         <v>110</v>
       </c>
       <c r="AD1">
         <f ca="1">RANDBETWEEN(70,80)</f>
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="AE1" t="s">
         <v>110</v>
@@ -35717,7 +35895,7 @@
       </c>
       <c r="AH1">
         <f ca="1">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI1" t="s">
         <v>110</v>
@@ -35730,7 +35908,7 @@
       </c>
       <c r="AL1" t="str">
         <f ca="1">_xlfn.CONCAT(A1:AK1)</f>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman1@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,183,72,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman1@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,178,75,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="2" spans="1:38">
@@ -35815,28 +35993,28 @@
       </c>
       <c r="AB2">
         <f t="shared" ref="AB2:AB17" ca="1" si="0">RANDBETWEEN(170,185)</f>
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AC2" t="s">
         <v>110</v>
       </c>
       <c r="AD2">
         <f t="shared" ref="AD2:AD17" ca="1" si="1">RANDBETWEEN(70,80)</f>
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="AE2" t="s">
         <v>110</v>
       </c>
       <c r="AF2">
         <f t="shared" ref="AF2:AF17" ca="1" si="2">RANDBETWEEN(0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG2" t="s">
         <v>110</v>
       </c>
       <c r="AH2">
         <f t="shared" ref="AH2:AH17" ca="1" si="3">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI2" t="s">
         <v>110</v>
@@ -35849,7 +36027,7 @@
       </c>
       <c r="AL2" t="str">
         <f t="shared" ref="AL2:AL17" ca="1" si="4">_xlfn.CONCAT(A2:AK2)</f>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman2@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,177,70,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman2@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,175,79,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="3" spans="1:38">
@@ -35934,28 +36112,28 @@
       </c>
       <c r="AB3">
         <f t="shared" ca="1" si="0"/>
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="AC3" t="s">
         <v>110</v>
       </c>
       <c r="AD3">
         <f t="shared" ca="1" si="1"/>
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AE3" t="s">
         <v>110</v>
       </c>
       <c r="AF3">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG3" t="s">
         <v>110</v>
       </c>
       <c r="AH3">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI3" t="s">
         <v>110</v>
@@ -35968,7 +36146,7 @@
       </c>
       <c r="AL3" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman3@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,182,77,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman3@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,178,78,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="4" spans="1:38">
@@ -36053,7 +36231,7 @@
       </c>
       <c r="AB4">
         <f t="shared" ca="1" si="0"/>
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AC4" t="s">
         <v>110</v>
@@ -36067,7 +36245,7 @@
       </c>
       <c r="AF4">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG4" t="s">
         <v>110</v>
@@ -36087,7 +36265,7 @@
       </c>
       <c r="AL4" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman4@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,171,80,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman4@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,170,80,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="5" spans="1:38">
@@ -36172,14 +36350,14 @@
       </c>
       <c r="AB5">
         <f t="shared" ca="1" si="0"/>
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="AC5" t="s">
         <v>110</v>
       </c>
       <c r="AD5">
         <f t="shared" ca="1" si="1"/>
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="AE5" t="s">
         <v>110</v>
@@ -36193,7 +36371,7 @@
       </c>
       <c r="AH5">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI5" t="s">
         <v>110</v>
@@ -36206,7 +36384,7 @@
       </c>
       <c r="AL5" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman5@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,172,76,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman5@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,176,70,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="6" spans="1:38">
@@ -36291,14 +36469,14 @@
       </c>
       <c r="AB6">
         <f t="shared" ca="1" si="0"/>
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="AC6" t="s">
         <v>110</v>
       </c>
       <c r="AD6">
         <f t="shared" ca="1" si="1"/>
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AE6" t="s">
         <v>110</v>
@@ -36325,7 +36503,7 @@
       </c>
       <c r="AL6" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman6@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,174,73,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman6@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,182,74,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="7" spans="1:38">
@@ -36410,14 +36588,14 @@
       </c>
       <c r="AB7">
         <f t="shared" ca="1" si="0"/>
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="AC7" t="s">
         <v>110</v>
       </c>
       <c r="AD7">
         <f t="shared" ca="1" si="1"/>
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="AE7" t="s">
         <v>110</v>
@@ -36444,7 +36622,7 @@
       </c>
       <c r="AL7" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman7@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,181,70,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman7@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,174,75,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="8" spans="1:38">
@@ -36529,7 +36707,7 @@
       </c>
       <c r="AB8">
         <f t="shared" ca="1" si="0"/>
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="AC8" t="s">
         <v>110</v>
@@ -36543,7 +36721,7 @@
       </c>
       <c r="AF8">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG8" t="s">
         <v>110</v>
@@ -36563,7 +36741,7 @@
       </c>
       <c r="AL8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman8@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,185,76,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman8@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,174,76,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="9" spans="1:38">
@@ -36655,14 +36833,14 @@
       </c>
       <c r="AD9">
         <f t="shared" ca="1" si="1"/>
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AE9" t="s">
         <v>110</v>
       </c>
       <c r="AF9">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG9" t="s">
         <v>110</v>
@@ -36682,7 +36860,7 @@
       </c>
       <c r="AL9" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman9@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,179,74,1,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman9@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,179,72,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="10" spans="1:38">
@@ -36767,28 +36945,28 @@
       </c>
       <c r="AB10">
         <f t="shared" ca="1" si="0"/>
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="AC10" t="s">
         <v>110</v>
       </c>
       <c r="AD10">
         <f t="shared" ca="1" si="1"/>
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="AE10" t="s">
         <v>110</v>
       </c>
       <c r="AF10">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG10" t="s">
         <v>110</v>
       </c>
       <c r="AH10">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI10" t="s">
         <v>110</v>
@@ -36801,7 +36979,7 @@
       </c>
       <c r="AL10" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman10@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,174,75,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman10@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,181,79,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="11" spans="1:38">
@@ -36886,14 +37064,14 @@
       </c>
       <c r="AB11">
         <f t="shared" ca="1" si="0"/>
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="AC11" t="s">
         <v>110</v>
       </c>
       <c r="AD11">
         <f t="shared" ca="1" si="1"/>
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="AE11" t="s">
         <v>110</v>
@@ -36920,7 +37098,7 @@
       </c>
       <c r="AL11" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman11@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,184,79,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman11@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,179,76,0,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="12" spans="1:38">
@@ -37005,28 +37183,28 @@
       </c>
       <c r="AB12">
         <f t="shared" ca="1" si="0"/>
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="AC12" t="s">
         <v>110</v>
       </c>
       <c r="AD12">
         <f t="shared" ca="1" si="1"/>
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AE12" t="s">
         <v>110</v>
       </c>
       <c r="AF12">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG12" t="s">
         <v>110</v>
       </c>
       <c r="AH12">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI12" t="s">
         <v>110</v>
@@ -37039,7 +37217,7 @@
       </c>
       <c r="AL12" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman12@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,185,76,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman12@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','DF',null,177,77,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="13" spans="1:38">
@@ -37124,28 +37302,28 @@
       </c>
       <c r="AB13">
         <f t="shared" ca="1" si="0"/>
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="AC13" t="s">
         <v>110</v>
       </c>
       <c r="AD13">
         <f t="shared" ca="1" si="1"/>
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="AE13" t="s">
         <v>110</v>
       </c>
       <c r="AF13">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG13" t="s">
         <v>110</v>
       </c>
       <c r="AH13">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI13" t="s">
         <v>110</v>
@@ -37158,7 +37336,7 @@
       </c>
       <c r="AL13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman13@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,176,71,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman13@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','FW',null,181,73,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="14" spans="1:38">
@@ -37243,21 +37421,21 @@
       </c>
       <c r="AB14">
         <f t="shared" ca="1" si="0"/>
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="AC14" t="s">
         <v>110</v>
       </c>
       <c r="AD14">
         <f t="shared" ca="1" si="1"/>
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="AE14" t="s">
         <v>110</v>
       </c>
       <c r="AF14">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG14" t="s">
         <v>110</v>
@@ -37277,7 +37455,7 @@
       </c>
       <c r="AL14" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman14@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,178,75,0,0,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman14@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','MF',null,172,71,1,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="15" spans="1:38">
@@ -37362,14 +37540,14 @@
       </c>
       <c r="AB15">
         <f t="shared" ca="1" si="0"/>
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="AC15" t="s">
         <v>110</v>
       </c>
       <c r="AD15">
         <f t="shared" ca="1" si="1"/>
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AE15" t="s">
         <v>110</v>
@@ -37396,7 +37574,7 @@
       </c>
       <c r="AL15" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman15@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,173,74,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman15@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','DF',null,171,75,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="16" spans="1:38">
@@ -37481,28 +37659,28 @@
       </c>
       <c r="AB16">
         <f t="shared" ca="1" si="0"/>
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AC16" t="s">
         <v>110</v>
       </c>
       <c r="AD16">
         <f t="shared" ca="1" si="1"/>
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="AE16" t="s">
         <v>110</v>
       </c>
       <c r="AF16">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG16" t="s">
         <v>110</v>
       </c>
       <c r="AH16">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI16" t="s">
         <v>110</v>
@@ -37515,7 +37693,7 @@
       </c>
       <c r="AL16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman16@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,174,72,1,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman16@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'오른발','FW',null,177,77,0,0,'1995-06-01');</v>
       </c>
     </row>
     <row r="17" spans="1:38">
@@ -37600,21 +37778,21 @@
       </c>
       <c r="AB17">
         <f t="shared" ca="1" si="0"/>
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="AC17" t="s">
         <v>110</v>
       </c>
       <c r="AD17">
         <f t="shared" ca="1" si="1"/>
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AE17" t="s">
         <v>110</v>
       </c>
       <c r="AF17">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG17" t="s">
         <v>110</v>
@@ -37634,7 +37812,7 @@
       </c>
       <c r="AL17" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman17@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,177,72,0,1,'1995-06-01');</v>
+        <v>INSERT INTO user(email, pass, name, phone_num, user_reg_date, recent_login, main_foot, position, api_key, height, weight, was_pro, gender, born_date) VALUES('bioman17@gmail.com','1234','bioman1','010-1234-5678',sysdate(),sysdate(),'왼발','MF',null,182,70,1,1,'1995-06-01');</v>
       </c>
     </row>
     <row r="20" spans="1:38">
@@ -37689,7 +37867,7 @@
       </c>
       <c r="Q20">
         <f ca="1">RANDBETWEEN(0,5)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R20" t="s">
         <v>110</v>
@@ -37723,7 +37901,7 @@
       </c>
       <c r="AB20" t="str">
         <f ca="1">_xlfn.CONCAT(A20:AA20)</f>
-        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('왕십리FC','왕십리FC201018.jpg','성동구','성동구 구장','red',1,'2016-01-01',sysdate(),'1234','기업');</v>
+        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('왕십리FC','왕십리FC201018.jpg','성동구','성동구 구장','red',3,'2016-01-01',sysdate(),'1234','기업');</v>
       </c>
     </row>
     <row r="21" spans="1:38">
@@ -37778,7 +37956,7 @@
       </c>
       <c r="Q21">
         <f ca="1">RANDBETWEEN(0,5)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R21" t="s">
         <v>110</v>
@@ -37812,7 +37990,7 @@
       </c>
       <c r="AB21" t="str">
         <f ca="1">_xlfn.CONCAT(A21:AA21)</f>
-        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('답십리FC','답십리FC201018.jpg','성동구','응봉동 구장','blue',0,'2017-01-01',sysdate(),'5678','하나');</v>
+        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('답십리FC','답십리FC201018.jpg','성동구','응봉동 구장','blue',2,'2017-01-01',sysdate(),'5678','하나');</v>
       </c>
     </row>
     <row r="22" spans="1:38">
@@ -37867,7 +38045,7 @@
       </c>
       <c r="Q22">
         <f ca="1">RANDBETWEEN(0,5)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R22" t="s">
         <v>110</v>
@@ -37901,7 +38079,7 @@
       </c>
       <c r="AB22" t="str">
         <f ca="1">_xlfn.CONCAT(A22:AA22)</f>
-        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('대구FC','대구FC201018.jpg','달서구','달서구 구장','green',0,'2018-01-01',sysdate(),'2345','기업');</v>
+        <v>INSERT INTO team(team_name, emblem, area, stadium_info, uniform_color, uniform_type, founding_date, team_reg_date, account, bank) VALUES('대구FC','대구FC201018.jpg','달서구','달서구 구장','green',5,'2018-01-01',sysdate(),'2345','기업');</v>
       </c>
     </row>
     <row r="24" spans="1:38">

</xml_diff>